<commit_message>
feat：update dragon tower test
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Monster_怪物表.xlsx
+++ b/nevergiveup/Excel/Monster_怪物表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">铁钩怪人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">龙娘测试</t>
   </si>
 </sst>
 </file>
@@ -245,14 +248,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
@@ -324,7 +327,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -361,7 +364,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,20 +372,32 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -573,7 +588,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topRight" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -846,10 +861,10 @@
         <v>43</v>
       </c>
       <c r="E5" s="9" t="n">
-        <v>146036</v>
+        <v>268048</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>97857</v>
+        <v>268567</v>
       </c>
       <c r="G5" s="6" t="n">
         <v>550</v>
@@ -875,23 +890,23 @@
       <c r="N5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O5" s="9" t="n">
+      <c r="O5" s="12" t="n">
         <v>97861</v>
       </c>
       <c r="P5" s="6" t="n">
         <v>0.3</v>
       </c>
-      <c r="Q5" s="9" t="n">
+      <c r="Q5" s="12" t="n">
         <v>285139</v>
       </c>
       <c r="R5" s="6" t="n">
         <v>1.5</v>
       </c>
-      <c r="V5" s="12"/>
+      <c r="V5" s="13"/>
       <c r="W5" s="11"/>
-      <c r="X5" s="12"/>
+      <c r="X5" s="13"/>
       <c r="AA5" s="11"/>
-      <c r="AD5" s="13"/>
+      <c r="AD5" s="14"/>
       <c r="AMH5" s="2"/>
       <c r="AMI5" s="2"/>
       <c r="AMJ5" s="2"/>
@@ -900,19 +915,19 @@
       <c r="A6" s="7" t="n">
         <v>1002</v>
       </c>
-      <c r="B6" s="14" t="n">
+      <c r="B6" s="15" t="n">
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="9" t="n">
+      <c r="E6" s="12" t="n">
         <v>174947</v>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="12" t="n">
         <v>122498</v>
       </c>
       <c r="G6" s="6" t="n">
@@ -939,20 +954,20 @@
       <c r="N6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O6" s="9" t="n">
+      <c r="O6" s="12" t="n">
         <v>97861</v>
       </c>
       <c r="P6" s="6" t="n">
         <v>0.3</v>
       </c>
-      <c r="Q6" s="9" t="n">
+      <c r="Q6" s="12" t="n">
         <v>285139</v>
       </c>
       <c r="R6" s="6" t="n">
         <v>1.5</v>
       </c>
-      <c r="V6" s="12"/>
-      <c r="X6" s="12"/>
+      <c r="V6" s="13"/>
+      <c r="X6" s="13"/>
       <c r="AMH6" s="2"/>
       <c r="AMI6" s="2"/>
       <c r="AMJ6" s="2"/>
@@ -970,10 +985,10 @@
       <c r="D7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="9" t="n">
+      <c r="E7" s="12" t="n">
         <v>146185</v>
       </c>
-      <c r="F7" s="9" t="n">
+      <c r="F7" s="12" t="n">
         <v>122549</v>
       </c>
       <c r="G7" s="6" t="n">
@@ -1000,21 +1015,21 @@
       <c r="N7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O7" s="9"/>
+      <c r="O7" s="12"/>
       <c r="P7" s="6" t="n">
         <v>0.3</v>
       </c>
-      <c r="Q7" s="9" t="n">
+      <c r="Q7" s="12" t="n">
         <v>20291</v>
       </c>
       <c r="R7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="V7" s="12"/>
+      <c r="V7" s="13"/>
       <c r="W7" s="11"/>
-      <c r="X7" s="12"/>
+      <c r="X7" s="13"/>
       <c r="AA7" s="11"/>
-      <c r="AD7" s="13"/>
+      <c r="AD7" s="14"/>
       <c r="AMH7" s="2"/>
       <c r="AMI7" s="2"/>
       <c r="AMJ7" s="2"/>
@@ -1023,13 +1038,13 @@
       <c r="A8" s="7" t="n">
         <v>1004</v>
       </c>
-      <c r="B8" s="14" t="n">
+      <c r="B8" s="15" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="15" t="s">
         <v>50</v>
       </c>
       <c r="E8" s="6" t="n">
@@ -1062,7 +1077,7 @@
       <c r="N8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O8" s="9" t="n">
+      <c r="O8" s="12" t="n">
         <v>145952</v>
       </c>
       <c r="P8" s="6" t="n">
@@ -1074,8 +1089,8 @@
       <c r="R8" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="V8" s="12"/>
-      <c r="X8" s="12"/>
+      <c r="V8" s="13"/>
+      <c r="X8" s="13"/>
       <c r="AMH8" s="2"/>
       <c r="AMI8" s="2"/>
       <c r="AMJ8" s="2"/>
@@ -1084,19 +1099,19 @@
       <c r="A9" s="7" t="n">
         <v>1005</v>
       </c>
-      <c r="B9" s="14" t="n">
+      <c r="B9" s="15" t="n">
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="15" t="s">
         <v>52</v>
       </c>
       <c r="E9" s="6" t="n">
         <v>174911</v>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F9" s="12" t="n">
         <v>97860</v>
       </c>
       <c r="G9" s="6" t="n">
@@ -1123,20 +1138,20 @@
       <c r="N9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="9" t="n">
+      <c r="O9" s="12" t="n">
         <v>97861</v>
       </c>
       <c r="P9" s="6" t="n">
         <v>0.3</v>
       </c>
-      <c r="Q9" s="9" t="n">
+      <c r="Q9" s="12" t="n">
         <v>285139</v>
       </c>
       <c r="R9" s="6" t="n">
         <v>1.5</v>
       </c>
-      <c r="V9" s="12"/>
-      <c r="X9" s="12"/>
+      <c r="V9" s="13"/>
+      <c r="X9" s="13"/>
       <c r="AMH9" s="2"/>
       <c r="AMI9" s="2"/>
       <c r="AMJ9" s="2"/>
@@ -1145,19 +1160,19 @@
       <c r="A10" s="7" t="n">
         <v>1006</v>
       </c>
-      <c r="B10" s="14" t="n">
+      <c r="B10" s="15" t="n">
         <v>5</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="15" t="s">
         <v>54</v>
       </c>
       <c r="E10" s="6" t="n">
         <v>145900</v>
       </c>
-      <c r="F10" s="9" t="n">
+      <c r="F10" s="12" t="n">
         <v>122498</v>
       </c>
       <c r="G10" s="6" t="n">
@@ -1184,41 +1199,95 @@
       <c r="N10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O10" s="9" t="n">
+      <c r="O10" s="12" t="n">
         <v>97861</v>
       </c>
       <c r="P10" s="6" t="n">
         <v>0.3</v>
       </c>
-      <c r="Q10" s="9" t="n">
+      <c r="Q10" s="12" t="n">
         <v>285139</v>
       </c>
       <c r="R10" s="6" t="n">
         <v>1.5</v>
       </c>
-      <c r="V10" s="12"/>
-      <c r="X10" s="12"/>
+      <c r="V10" s="13"/>
+      <c r="X10" s="13"/>
       <c r="AMH10" s="2"/>
       <c r="AMI10" s="2"/>
       <c r="AMJ10" s="2"/>
     </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="n">
+        <v>1007</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>268048</v>
+      </c>
+      <c r="F11" s="6" t="n">
+        <v>268567</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="H11" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="I11" s="17" t="n">
+        <v>107535</v>
+      </c>
+      <c r="J11" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="L11" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="M11" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" s="6" t="n">
+        <v>97861</v>
+      </c>
+      <c r="P11" s="6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="Q11" s="6" t="n">
+        <v>281693</v>
+      </c>
+      <c r="R11" s="6" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
     <row r="15" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
-      <c r="V15" s="12"/>
-      <c r="X15" s="12"/>
+      <c r="V15" s="13"/>
+      <c r="X15" s="13"/>
       <c r="AMH15" s="2"/>
       <c r="AMI15" s="2"/>
       <c r="AMJ15" s="2"/>
     </row>
     <row r="16" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="K16" s="13"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="12"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="K16" s="14"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="13"/>
       <c r="AA16" s="11"/>
       <c r="AD16" s="11"/>
       <c r="AMH16" s="2"/>
@@ -1227,8 +1296,8 @@
     </row>
     <row r="17" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7"/>
-      <c r="V17" s="12"/>
-      <c r="X17" s="12"/>
+      <c r="V17" s="13"/>
+      <c r="X17" s="13"/>
       <c r="AMH17" s="2"/>
       <c r="AMI17" s="2"/>
       <c r="AMJ17" s="2"/>

</xml_diff>

<commit_message>
feat：update monster excel change
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Monster_怪物表.xlsx
+++ b/nevergiveup/Excel/Monster_怪物表.xlsx
@@ -554,7 +554,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -647,7 +647,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -659,16 +659,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -691,11 +683,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -884,10 +876,10 @@
   </sheetPr>
   <dimension ref="A1:AML376"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="D16" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
-      <selection pane="topRight" activeCell="I45" activeCellId="0" sqref="I45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="0" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="V20" activeCellId="0" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1696,7 +1688,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" s="26" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="25" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="n">
         <v>1008</v>
       </c>
@@ -1717,10 +1709,10 @@
         <v>268562</v>
       </c>
       <c r="H12" s="20" t="n">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="I12" s="20" t="n">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="J12" s="24" t="n">
         <v>107535</v>
@@ -1756,10 +1748,10 @@
         <v>3</v>
       </c>
       <c r="U12" s="20" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V12" s="20" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W12" s="20"/>
       <c r="Y12" s="20"/>
@@ -2768,16 +2760,16 @@
       <c r="C13" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="26" t="s">
         <v>69</v>
       </c>
       <c r="E13" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="28" t="n">
+      <c r="F13" s="14" t="n">
         <v>157055</v>
       </c>
-      <c r="G13" s="29" t="n">
+      <c r="G13" s="27" t="n">
         <v>122498</v>
       </c>
       <c r="H13" s="1" t="n">
@@ -2826,24 +2818,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" s="35" customFormat="true" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="n">
+    <row r="14" s="33" customFormat="true" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="28" t="n">
         <v>1010</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="32" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="30" t="n">
+      <c r="E14" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="34" t="n">
+      <c r="F14" s="32" t="n">
         <v>183662</v>
       </c>
-      <c r="G14" s="31" t="n">
+      <c r="G14" s="29" t="n">
         <v>285174</v>
       </c>
       <c r="H14" s="1" t="n">
@@ -2891,1005 +2883,1005 @@
       <c r="V14" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="W14" s="31"/>
-      <c r="Y14" s="31"/>
-      <c r="AA14" s="31"/>
-      <c r="AB14" s="31"/>
-      <c r="AC14" s="31"/>
-      <c r="AD14" s="31"/>
-      <c r="AE14" s="31"/>
-      <c r="AF14" s="31"/>
-      <c r="AG14" s="31"/>
-      <c r="AH14" s="31"/>
-      <c r="AI14" s="31"/>
-      <c r="AJ14" s="31"/>
-      <c r="AK14" s="31"/>
-      <c r="AL14" s="31"/>
-      <c r="AM14" s="31"/>
-      <c r="AN14" s="31"/>
-      <c r="AO14" s="31"/>
-      <c r="AP14" s="31"/>
-      <c r="AQ14" s="31"/>
-      <c r="AR14" s="31"/>
-      <c r="AS14" s="31"/>
-      <c r="AT14" s="31"/>
-      <c r="AU14" s="31"/>
-      <c r="AV14" s="31"/>
-      <c r="AW14" s="31"/>
-      <c r="AX14" s="31"/>
-      <c r="AY14" s="31"/>
-      <c r="AZ14" s="31"/>
-      <c r="BA14" s="31"/>
-      <c r="BB14" s="31"/>
-      <c r="BC14" s="31"/>
-      <c r="BD14" s="31"/>
-      <c r="BE14" s="31"/>
-      <c r="BF14" s="31"/>
-      <c r="BG14" s="31"/>
-      <c r="BH14" s="31"/>
-      <c r="BI14" s="31"/>
-      <c r="BJ14" s="31"/>
-      <c r="BK14" s="31"/>
-      <c r="BL14" s="31"/>
-      <c r="BM14" s="31"/>
-      <c r="BN14" s="31"/>
-      <c r="BO14" s="31"/>
-      <c r="BP14" s="31"/>
-      <c r="BQ14" s="31"/>
-      <c r="BR14" s="31"/>
-      <c r="BS14" s="31"/>
-      <c r="BT14" s="31"/>
-      <c r="BU14" s="31"/>
-      <c r="BV14" s="31"/>
-      <c r="BW14" s="31"/>
-      <c r="BX14" s="31"/>
-      <c r="BY14" s="31"/>
-      <c r="BZ14" s="31"/>
-      <c r="CA14" s="31"/>
-      <c r="CB14" s="31"/>
-      <c r="CC14" s="31"/>
-      <c r="CD14" s="31"/>
-      <c r="CE14" s="31"/>
-      <c r="CF14" s="31"/>
-      <c r="CG14" s="31"/>
-      <c r="CH14" s="31"/>
-      <c r="CI14" s="31"/>
-      <c r="CJ14" s="31"/>
-      <c r="CK14" s="31"/>
-      <c r="CL14" s="31"/>
-      <c r="CM14" s="31"/>
-      <c r="CN14" s="31"/>
-      <c r="CO14" s="31"/>
-      <c r="CP14" s="31"/>
-      <c r="CQ14" s="31"/>
-      <c r="CR14" s="31"/>
-      <c r="CS14" s="31"/>
-      <c r="CT14" s="31"/>
-      <c r="CU14" s="31"/>
-      <c r="CV14" s="31"/>
-      <c r="CW14" s="31"/>
-      <c r="CX14" s="31"/>
-      <c r="CY14" s="31"/>
-      <c r="CZ14" s="31"/>
-      <c r="DA14" s="31"/>
-      <c r="DB14" s="31"/>
-      <c r="DC14" s="31"/>
-      <c r="DD14" s="31"/>
-      <c r="DE14" s="31"/>
-      <c r="DF14" s="31"/>
-      <c r="DG14" s="31"/>
-      <c r="DH14" s="31"/>
-      <c r="DI14" s="31"/>
-      <c r="DJ14" s="31"/>
-      <c r="DK14" s="31"/>
-      <c r="DL14" s="31"/>
-      <c r="DM14" s="31"/>
-      <c r="DN14" s="31"/>
-      <c r="DO14" s="31"/>
-      <c r="DP14" s="31"/>
-      <c r="DQ14" s="31"/>
-      <c r="DR14" s="31"/>
-      <c r="DS14" s="31"/>
-      <c r="DT14" s="31"/>
-      <c r="DU14" s="31"/>
-      <c r="DV14" s="31"/>
-      <c r="DW14" s="31"/>
-      <c r="DX14" s="31"/>
-      <c r="DY14" s="31"/>
-      <c r="DZ14" s="31"/>
-      <c r="EA14" s="31"/>
-      <c r="EB14" s="31"/>
-      <c r="EC14" s="31"/>
-      <c r="ED14" s="31"/>
-      <c r="EE14" s="31"/>
-      <c r="EF14" s="31"/>
-      <c r="EG14" s="31"/>
-      <c r="EH14" s="31"/>
-      <c r="EI14" s="31"/>
-      <c r="EJ14" s="31"/>
-      <c r="EK14" s="31"/>
-      <c r="EL14" s="31"/>
-      <c r="EM14" s="31"/>
-      <c r="EN14" s="31"/>
-      <c r="EO14" s="31"/>
-      <c r="EP14" s="31"/>
-      <c r="EQ14" s="31"/>
-      <c r="ER14" s="31"/>
-      <c r="ES14" s="31"/>
-      <c r="ET14" s="31"/>
-      <c r="EU14" s="31"/>
-      <c r="EV14" s="31"/>
-      <c r="EW14" s="31"/>
-      <c r="EX14" s="31"/>
-      <c r="EY14" s="31"/>
-      <c r="EZ14" s="31"/>
-      <c r="FA14" s="31"/>
-      <c r="FB14" s="31"/>
-      <c r="FC14" s="31"/>
-      <c r="FD14" s="31"/>
-      <c r="FE14" s="31"/>
-      <c r="FF14" s="31"/>
-      <c r="FG14" s="31"/>
-      <c r="FH14" s="31"/>
-      <c r="FI14" s="31"/>
-      <c r="FJ14" s="31"/>
-      <c r="FK14" s="31"/>
-      <c r="FL14" s="31"/>
-      <c r="FM14" s="31"/>
-      <c r="FN14" s="31"/>
-      <c r="FO14" s="31"/>
-      <c r="FP14" s="31"/>
-      <c r="FQ14" s="31"/>
-      <c r="FR14" s="31"/>
-      <c r="FS14" s="31"/>
-      <c r="FT14" s="31"/>
-      <c r="FU14" s="31"/>
-      <c r="FV14" s="31"/>
-      <c r="FW14" s="31"/>
-      <c r="FX14" s="31"/>
-      <c r="FY14" s="31"/>
-      <c r="FZ14" s="31"/>
-      <c r="GA14" s="31"/>
-      <c r="GB14" s="31"/>
-      <c r="GC14" s="31"/>
-      <c r="GD14" s="31"/>
-      <c r="GE14" s="31"/>
-      <c r="GF14" s="31"/>
-      <c r="GG14" s="31"/>
-      <c r="GH14" s="31"/>
-      <c r="GI14" s="31"/>
-      <c r="GJ14" s="31"/>
-      <c r="GK14" s="31"/>
-      <c r="GL14" s="31"/>
-      <c r="GM14" s="31"/>
-      <c r="GN14" s="31"/>
-      <c r="GO14" s="31"/>
-      <c r="GP14" s="31"/>
-      <c r="GQ14" s="31"/>
-      <c r="GR14" s="31"/>
-      <c r="GS14" s="31"/>
-      <c r="GT14" s="31"/>
-      <c r="GU14" s="31"/>
-      <c r="GV14" s="31"/>
-      <c r="GW14" s="31"/>
-      <c r="GX14" s="31"/>
-      <c r="GY14" s="31"/>
-      <c r="GZ14" s="31"/>
-      <c r="HA14" s="31"/>
-      <c r="HB14" s="31"/>
-      <c r="HC14" s="31"/>
-      <c r="HD14" s="31"/>
-      <c r="HE14" s="31"/>
-      <c r="HF14" s="31"/>
-      <c r="HG14" s="31"/>
-      <c r="HH14" s="31"/>
-      <c r="HI14" s="31"/>
-      <c r="HJ14" s="31"/>
-      <c r="HK14" s="31"/>
-      <c r="HL14" s="31"/>
-      <c r="HM14" s="31"/>
-      <c r="HN14" s="31"/>
-      <c r="HO14" s="31"/>
-      <c r="HP14" s="31"/>
-      <c r="HQ14" s="31"/>
-      <c r="HR14" s="31"/>
-      <c r="HS14" s="31"/>
-      <c r="HT14" s="31"/>
-      <c r="HU14" s="31"/>
-      <c r="HV14" s="31"/>
-      <c r="HW14" s="31"/>
-      <c r="HX14" s="31"/>
-      <c r="HY14" s="31"/>
-      <c r="HZ14" s="31"/>
-      <c r="IA14" s="31"/>
-      <c r="IB14" s="31"/>
-      <c r="IC14" s="31"/>
-      <c r="ID14" s="31"/>
-      <c r="IE14" s="31"/>
-      <c r="IF14" s="31"/>
-      <c r="IG14" s="31"/>
-      <c r="IH14" s="31"/>
-      <c r="II14" s="31"/>
-      <c r="IJ14" s="31"/>
-      <c r="IK14" s="31"/>
-      <c r="IL14" s="31"/>
-      <c r="IM14" s="31"/>
-      <c r="IN14" s="31"/>
-      <c r="IO14" s="31"/>
-      <c r="IP14" s="31"/>
-      <c r="IQ14" s="31"/>
-      <c r="IR14" s="31"/>
-      <c r="IS14" s="31"/>
-      <c r="IT14" s="31"/>
-      <c r="IU14" s="31"/>
-      <c r="IV14" s="31"/>
-      <c r="IW14" s="31"/>
-      <c r="IX14" s="31"/>
-      <c r="IY14" s="31"/>
-      <c r="IZ14" s="31"/>
-      <c r="JA14" s="31"/>
-      <c r="JB14" s="31"/>
-      <c r="JC14" s="31"/>
-      <c r="JD14" s="31"/>
-      <c r="JE14" s="31"/>
-      <c r="JF14" s="31"/>
-      <c r="JG14" s="31"/>
-      <c r="JH14" s="31"/>
-      <c r="JI14" s="31"/>
-      <c r="JJ14" s="31"/>
-      <c r="JK14" s="31"/>
-      <c r="JL14" s="31"/>
-      <c r="JM14" s="31"/>
-      <c r="JN14" s="31"/>
-      <c r="JO14" s="31"/>
-      <c r="JP14" s="31"/>
-      <c r="JQ14" s="31"/>
-      <c r="JR14" s="31"/>
-      <c r="JS14" s="31"/>
-      <c r="JT14" s="31"/>
-      <c r="JU14" s="31"/>
-      <c r="JV14" s="31"/>
-      <c r="JW14" s="31"/>
-      <c r="JX14" s="31"/>
-      <c r="JY14" s="31"/>
-      <c r="JZ14" s="31"/>
-      <c r="KA14" s="31"/>
-      <c r="KB14" s="31"/>
-      <c r="KC14" s="31"/>
-      <c r="KD14" s="31"/>
-      <c r="KE14" s="31"/>
-      <c r="KF14" s="31"/>
-      <c r="KG14" s="31"/>
-      <c r="KH14" s="31"/>
-      <c r="KI14" s="31"/>
-      <c r="KJ14" s="31"/>
-      <c r="KK14" s="31"/>
-      <c r="KL14" s="31"/>
-      <c r="KM14" s="31"/>
-      <c r="KN14" s="31"/>
-      <c r="KO14" s="31"/>
-      <c r="KP14" s="31"/>
-      <c r="KQ14" s="31"/>
-      <c r="KR14" s="31"/>
-      <c r="KS14" s="31"/>
-      <c r="KT14" s="31"/>
-      <c r="KU14" s="31"/>
-      <c r="KV14" s="31"/>
-      <c r="KW14" s="31"/>
-      <c r="KX14" s="31"/>
-      <c r="KY14" s="31"/>
-      <c r="KZ14" s="31"/>
-      <c r="LA14" s="31"/>
-      <c r="LB14" s="31"/>
-      <c r="LC14" s="31"/>
-      <c r="LD14" s="31"/>
-      <c r="LE14" s="31"/>
-      <c r="LF14" s="31"/>
-      <c r="LG14" s="31"/>
-      <c r="LH14" s="31"/>
-      <c r="LI14" s="31"/>
-      <c r="LJ14" s="31"/>
-      <c r="LK14" s="31"/>
-      <c r="LL14" s="31"/>
-      <c r="LM14" s="31"/>
-      <c r="LN14" s="31"/>
-      <c r="LO14" s="31"/>
-      <c r="LP14" s="31"/>
-      <c r="LQ14" s="31"/>
-      <c r="LR14" s="31"/>
-      <c r="LS14" s="31"/>
-      <c r="LT14" s="31"/>
-      <c r="LU14" s="31"/>
-      <c r="LV14" s="31"/>
-      <c r="LW14" s="31"/>
-      <c r="LX14" s="31"/>
-      <c r="LY14" s="31"/>
-      <c r="LZ14" s="31"/>
-      <c r="MA14" s="31"/>
-      <c r="MB14" s="31"/>
-      <c r="MC14" s="31"/>
-      <c r="MD14" s="31"/>
-      <c r="ME14" s="31"/>
-      <c r="MF14" s="31"/>
-      <c r="MG14" s="31"/>
-      <c r="MH14" s="31"/>
-      <c r="MI14" s="31"/>
-      <c r="MJ14" s="31"/>
-      <c r="MK14" s="31"/>
-      <c r="ML14" s="31"/>
-      <c r="MM14" s="31"/>
-      <c r="MN14" s="31"/>
-      <c r="MO14" s="31"/>
-      <c r="MP14" s="31"/>
-      <c r="MQ14" s="31"/>
-      <c r="MR14" s="31"/>
-      <c r="MS14" s="31"/>
-      <c r="MT14" s="31"/>
-      <c r="MU14" s="31"/>
-      <c r="MV14" s="31"/>
-      <c r="MW14" s="31"/>
-      <c r="MX14" s="31"/>
-      <c r="MY14" s="31"/>
-      <c r="MZ14" s="31"/>
-      <c r="NA14" s="31"/>
-      <c r="NB14" s="31"/>
-      <c r="NC14" s="31"/>
-      <c r="ND14" s="31"/>
-      <c r="NE14" s="31"/>
-      <c r="NF14" s="31"/>
-      <c r="NG14" s="31"/>
-      <c r="NH14" s="31"/>
-      <c r="NI14" s="31"/>
-      <c r="NJ14" s="31"/>
-      <c r="NK14" s="31"/>
-      <c r="NL14" s="31"/>
-      <c r="NM14" s="31"/>
-      <c r="NN14" s="31"/>
-      <c r="NO14" s="31"/>
-      <c r="NP14" s="31"/>
-      <c r="NQ14" s="31"/>
-      <c r="NR14" s="31"/>
-      <c r="NS14" s="31"/>
-      <c r="NT14" s="31"/>
-      <c r="NU14" s="31"/>
-      <c r="NV14" s="31"/>
-      <c r="NW14" s="31"/>
-      <c r="NX14" s="31"/>
-      <c r="NY14" s="31"/>
-      <c r="NZ14" s="31"/>
-      <c r="OA14" s="31"/>
-      <c r="OB14" s="31"/>
-      <c r="OC14" s="31"/>
-      <c r="OD14" s="31"/>
-      <c r="OE14" s="31"/>
-      <c r="OF14" s="31"/>
-      <c r="OG14" s="31"/>
-      <c r="OH14" s="31"/>
-      <c r="OI14" s="31"/>
-      <c r="OJ14" s="31"/>
-      <c r="OK14" s="31"/>
-      <c r="OL14" s="31"/>
-      <c r="OM14" s="31"/>
-      <c r="ON14" s="31"/>
-      <c r="OO14" s="31"/>
-      <c r="OP14" s="31"/>
-      <c r="OQ14" s="31"/>
-      <c r="OR14" s="31"/>
-      <c r="OS14" s="31"/>
-      <c r="OT14" s="31"/>
-      <c r="OU14" s="31"/>
-      <c r="OV14" s="31"/>
-      <c r="OW14" s="31"/>
-      <c r="OX14" s="31"/>
-      <c r="OY14" s="31"/>
-      <c r="OZ14" s="31"/>
-      <c r="PA14" s="31"/>
-      <c r="PB14" s="31"/>
-      <c r="PC14" s="31"/>
-      <c r="PD14" s="31"/>
-      <c r="PE14" s="31"/>
-      <c r="PF14" s="31"/>
-      <c r="PG14" s="31"/>
-      <c r="PH14" s="31"/>
-      <c r="PI14" s="31"/>
-      <c r="PJ14" s="31"/>
-      <c r="PK14" s="31"/>
-      <c r="PL14" s="31"/>
-      <c r="PM14" s="31"/>
-      <c r="PN14" s="31"/>
-      <c r="PO14" s="31"/>
-      <c r="PP14" s="31"/>
-      <c r="PQ14" s="31"/>
-      <c r="PR14" s="31"/>
-      <c r="PS14" s="31"/>
-      <c r="PT14" s="31"/>
-      <c r="PU14" s="31"/>
-      <c r="PV14" s="31"/>
-      <c r="PW14" s="31"/>
-      <c r="PX14" s="31"/>
-      <c r="PY14" s="31"/>
-      <c r="PZ14" s="31"/>
-      <c r="QA14" s="31"/>
-      <c r="QB14" s="31"/>
-      <c r="QC14" s="31"/>
-      <c r="QD14" s="31"/>
-      <c r="QE14" s="31"/>
-      <c r="QF14" s="31"/>
-      <c r="QG14" s="31"/>
-      <c r="QH14" s="31"/>
-      <c r="QI14" s="31"/>
-      <c r="QJ14" s="31"/>
-      <c r="QK14" s="31"/>
-      <c r="QL14" s="31"/>
-      <c r="QM14" s="31"/>
-      <c r="QN14" s="31"/>
-      <c r="QO14" s="31"/>
-      <c r="QP14" s="31"/>
-      <c r="QQ14" s="31"/>
-      <c r="QR14" s="31"/>
-      <c r="QS14" s="31"/>
-      <c r="QT14" s="31"/>
-      <c r="QU14" s="31"/>
-      <c r="QV14" s="31"/>
-      <c r="QW14" s="31"/>
-      <c r="QX14" s="31"/>
-      <c r="QY14" s="31"/>
-      <c r="QZ14" s="31"/>
-      <c r="RA14" s="31"/>
-      <c r="RB14" s="31"/>
-      <c r="RC14" s="31"/>
-      <c r="RD14" s="31"/>
-      <c r="RE14" s="31"/>
-      <c r="RF14" s="31"/>
-      <c r="RG14" s="31"/>
-      <c r="RH14" s="31"/>
-      <c r="RI14" s="31"/>
-      <c r="RJ14" s="31"/>
-      <c r="RK14" s="31"/>
-      <c r="RL14" s="31"/>
-      <c r="RM14" s="31"/>
-      <c r="RN14" s="31"/>
-      <c r="RO14" s="31"/>
-      <c r="RP14" s="31"/>
-      <c r="RQ14" s="31"/>
-      <c r="RR14" s="31"/>
-      <c r="RS14" s="31"/>
-      <c r="RT14" s="31"/>
-      <c r="RU14" s="31"/>
-      <c r="RV14" s="31"/>
-      <c r="RW14" s="31"/>
-      <c r="RX14" s="31"/>
-      <c r="RY14" s="31"/>
-      <c r="RZ14" s="31"/>
-      <c r="SA14" s="31"/>
-      <c r="SB14" s="31"/>
-      <c r="SC14" s="31"/>
-      <c r="SD14" s="31"/>
-      <c r="SE14" s="31"/>
-      <c r="SF14" s="31"/>
-      <c r="SG14" s="31"/>
-      <c r="SH14" s="31"/>
-      <c r="SI14" s="31"/>
-      <c r="SJ14" s="31"/>
-      <c r="SK14" s="31"/>
-      <c r="SL14" s="31"/>
-      <c r="SM14" s="31"/>
-      <c r="SN14" s="31"/>
-      <c r="SO14" s="31"/>
-      <c r="SP14" s="31"/>
-      <c r="SQ14" s="31"/>
-      <c r="SR14" s="31"/>
-      <c r="SS14" s="31"/>
-      <c r="ST14" s="31"/>
-      <c r="SU14" s="31"/>
-      <c r="SV14" s="31"/>
-      <c r="SW14" s="31"/>
-      <c r="SX14" s="31"/>
-      <c r="SY14" s="31"/>
-      <c r="SZ14" s="31"/>
-      <c r="TA14" s="31"/>
-      <c r="TB14" s="31"/>
-      <c r="TC14" s="31"/>
-      <c r="TD14" s="31"/>
-      <c r="TE14" s="31"/>
-      <c r="TF14" s="31"/>
-      <c r="TG14" s="31"/>
-      <c r="TH14" s="31"/>
-      <c r="TI14" s="31"/>
-      <c r="TJ14" s="31"/>
-      <c r="TK14" s="31"/>
-      <c r="TL14" s="31"/>
-      <c r="TM14" s="31"/>
-      <c r="TN14" s="31"/>
-      <c r="TO14" s="31"/>
-      <c r="TP14" s="31"/>
-      <c r="TQ14" s="31"/>
-      <c r="TR14" s="31"/>
-      <c r="TS14" s="31"/>
-      <c r="TT14" s="31"/>
-      <c r="TU14" s="31"/>
-      <c r="TV14" s="31"/>
-      <c r="TW14" s="31"/>
-      <c r="TX14" s="31"/>
-      <c r="TY14" s="31"/>
-      <c r="TZ14" s="31"/>
-      <c r="UA14" s="31"/>
-      <c r="UB14" s="31"/>
-      <c r="UC14" s="31"/>
-      <c r="UD14" s="31"/>
-      <c r="UE14" s="31"/>
-      <c r="UF14" s="31"/>
-      <c r="UG14" s="31"/>
-      <c r="UH14" s="31"/>
-      <c r="UI14" s="31"/>
-      <c r="UJ14" s="31"/>
-      <c r="UK14" s="31"/>
-      <c r="UL14" s="31"/>
-      <c r="UM14" s="31"/>
-      <c r="UN14" s="31"/>
-      <c r="UO14" s="31"/>
-      <c r="UP14" s="31"/>
-      <c r="UQ14" s="31"/>
-      <c r="UR14" s="31"/>
-      <c r="US14" s="31"/>
-      <c r="UT14" s="31"/>
-      <c r="UU14" s="31"/>
-      <c r="UV14" s="31"/>
-      <c r="UW14" s="31"/>
-      <c r="UX14" s="31"/>
-      <c r="UY14" s="31"/>
-      <c r="UZ14" s="31"/>
-      <c r="VA14" s="31"/>
-      <c r="VB14" s="31"/>
-      <c r="VC14" s="31"/>
-      <c r="VD14" s="31"/>
-      <c r="VE14" s="31"/>
-      <c r="VF14" s="31"/>
-      <c r="VG14" s="31"/>
-      <c r="VH14" s="31"/>
-      <c r="VI14" s="31"/>
-      <c r="VJ14" s="31"/>
-      <c r="VK14" s="31"/>
-      <c r="VL14" s="31"/>
-      <c r="VM14" s="31"/>
-      <c r="VN14" s="31"/>
-      <c r="VO14" s="31"/>
-      <c r="VP14" s="31"/>
-      <c r="VQ14" s="31"/>
-      <c r="VR14" s="31"/>
-      <c r="VS14" s="31"/>
-      <c r="VT14" s="31"/>
-      <c r="VU14" s="31"/>
-      <c r="VV14" s="31"/>
-      <c r="VW14" s="31"/>
-      <c r="VX14" s="31"/>
-      <c r="VY14" s="31"/>
-      <c r="VZ14" s="31"/>
-      <c r="WA14" s="31"/>
-      <c r="WB14" s="31"/>
-      <c r="WC14" s="31"/>
-      <c r="WD14" s="31"/>
-      <c r="WE14" s="31"/>
-      <c r="WF14" s="31"/>
-      <c r="WG14" s="31"/>
-      <c r="WH14" s="31"/>
-      <c r="WI14" s="31"/>
-      <c r="WJ14" s="31"/>
-      <c r="WK14" s="31"/>
-      <c r="WL14" s="31"/>
-      <c r="WM14" s="31"/>
-      <c r="WN14" s="31"/>
-      <c r="WO14" s="31"/>
-      <c r="WP14" s="31"/>
-      <c r="WQ14" s="31"/>
-      <c r="WR14" s="31"/>
-      <c r="WS14" s="31"/>
-      <c r="WT14" s="31"/>
-      <c r="WU14" s="31"/>
-      <c r="WV14" s="31"/>
-      <c r="WW14" s="31"/>
-      <c r="WX14" s="31"/>
-      <c r="WY14" s="31"/>
-      <c r="WZ14" s="31"/>
-      <c r="XA14" s="31"/>
-      <c r="XB14" s="31"/>
-      <c r="XC14" s="31"/>
-      <c r="XD14" s="31"/>
-      <c r="XE14" s="31"/>
-      <c r="XF14" s="31"/>
-      <c r="XG14" s="31"/>
-      <c r="XH14" s="31"/>
-      <c r="XI14" s="31"/>
-      <c r="XJ14" s="31"/>
-      <c r="XK14" s="31"/>
-      <c r="XL14" s="31"/>
-      <c r="XM14" s="31"/>
-      <c r="XN14" s="31"/>
-      <c r="XO14" s="31"/>
-      <c r="XP14" s="31"/>
-      <c r="XQ14" s="31"/>
-      <c r="XR14" s="31"/>
-      <c r="XS14" s="31"/>
-      <c r="XT14" s="31"/>
-      <c r="XU14" s="31"/>
-      <c r="XV14" s="31"/>
-      <c r="XW14" s="31"/>
-      <c r="XX14" s="31"/>
-      <c r="XY14" s="31"/>
-      <c r="XZ14" s="31"/>
-      <c r="YA14" s="31"/>
-      <c r="YB14" s="31"/>
-      <c r="YC14" s="31"/>
-      <c r="YD14" s="31"/>
-      <c r="YE14" s="31"/>
-      <c r="YF14" s="31"/>
-      <c r="YG14" s="31"/>
-      <c r="YH14" s="31"/>
-      <c r="YI14" s="31"/>
-      <c r="YJ14" s="31"/>
-      <c r="YK14" s="31"/>
-      <c r="YL14" s="31"/>
-      <c r="YM14" s="31"/>
-      <c r="YN14" s="31"/>
-      <c r="YO14" s="31"/>
-      <c r="YP14" s="31"/>
-      <c r="YQ14" s="31"/>
-      <c r="YR14" s="31"/>
-      <c r="YS14" s="31"/>
-      <c r="YT14" s="31"/>
-      <c r="YU14" s="31"/>
-      <c r="YV14" s="31"/>
-      <c r="YW14" s="31"/>
-      <c r="YX14" s="31"/>
-      <c r="YY14" s="31"/>
-      <c r="YZ14" s="31"/>
-      <c r="ZA14" s="31"/>
-      <c r="ZB14" s="31"/>
-      <c r="ZC14" s="31"/>
-      <c r="ZD14" s="31"/>
-      <c r="ZE14" s="31"/>
-      <c r="ZF14" s="31"/>
-      <c r="ZG14" s="31"/>
-      <c r="ZH14" s="31"/>
-      <c r="ZI14" s="31"/>
-      <c r="ZJ14" s="31"/>
-      <c r="ZK14" s="31"/>
-      <c r="ZL14" s="31"/>
-      <c r="ZM14" s="31"/>
-      <c r="ZN14" s="31"/>
-      <c r="ZO14" s="31"/>
-      <c r="ZP14" s="31"/>
-      <c r="ZQ14" s="31"/>
-      <c r="ZR14" s="31"/>
-      <c r="ZS14" s="31"/>
-      <c r="ZT14" s="31"/>
-      <c r="ZU14" s="31"/>
-      <c r="ZV14" s="31"/>
-      <c r="ZW14" s="31"/>
-      <c r="ZX14" s="31"/>
-      <c r="ZY14" s="31"/>
-      <c r="ZZ14" s="31"/>
-      <c r="AAA14" s="31"/>
-      <c r="AAB14" s="31"/>
-      <c r="AAC14" s="31"/>
-      <c r="AAD14" s="31"/>
-      <c r="AAE14" s="31"/>
-      <c r="AAF14" s="31"/>
-      <c r="AAG14" s="31"/>
-      <c r="AAH14" s="31"/>
-      <c r="AAI14" s="31"/>
-      <c r="AAJ14" s="31"/>
-      <c r="AAK14" s="31"/>
-      <c r="AAL14" s="31"/>
-      <c r="AAM14" s="31"/>
-      <c r="AAN14" s="31"/>
-      <c r="AAO14" s="31"/>
-      <c r="AAP14" s="31"/>
-      <c r="AAQ14" s="31"/>
-      <c r="AAR14" s="31"/>
-      <c r="AAS14" s="31"/>
-      <c r="AAT14" s="31"/>
-      <c r="AAU14" s="31"/>
-      <c r="AAV14" s="31"/>
-      <c r="AAW14" s="31"/>
-      <c r="AAX14" s="31"/>
-      <c r="AAY14" s="31"/>
-      <c r="AAZ14" s="31"/>
-      <c r="ABA14" s="31"/>
-      <c r="ABB14" s="31"/>
-      <c r="ABC14" s="31"/>
-      <c r="ABD14" s="31"/>
-      <c r="ABE14" s="31"/>
-      <c r="ABF14" s="31"/>
-      <c r="ABG14" s="31"/>
-      <c r="ABH14" s="31"/>
-      <c r="ABI14" s="31"/>
-      <c r="ABJ14" s="31"/>
-      <c r="ABK14" s="31"/>
-      <c r="ABL14" s="31"/>
-      <c r="ABM14" s="31"/>
-      <c r="ABN14" s="31"/>
-      <c r="ABO14" s="31"/>
-      <c r="ABP14" s="31"/>
-      <c r="ABQ14" s="31"/>
-      <c r="ABR14" s="31"/>
-      <c r="ABS14" s="31"/>
-      <c r="ABT14" s="31"/>
-      <c r="ABU14" s="31"/>
-      <c r="ABV14" s="31"/>
-      <c r="ABW14" s="31"/>
-      <c r="ABX14" s="31"/>
-      <c r="ABY14" s="31"/>
-      <c r="ABZ14" s="31"/>
-      <c r="ACA14" s="31"/>
-      <c r="ACB14" s="31"/>
-      <c r="ACC14" s="31"/>
-      <c r="ACD14" s="31"/>
-      <c r="ACE14" s="31"/>
-      <c r="ACF14" s="31"/>
-      <c r="ACG14" s="31"/>
-      <c r="ACH14" s="31"/>
-      <c r="ACI14" s="31"/>
-      <c r="ACJ14" s="31"/>
-      <c r="ACK14" s="31"/>
-      <c r="ACL14" s="31"/>
-      <c r="ACM14" s="31"/>
-      <c r="ACN14" s="31"/>
-      <c r="ACO14" s="31"/>
-      <c r="ACP14" s="31"/>
-      <c r="ACQ14" s="31"/>
-      <c r="ACR14" s="31"/>
-      <c r="ACS14" s="31"/>
-      <c r="ACT14" s="31"/>
-      <c r="ACU14" s="31"/>
-      <c r="ACV14" s="31"/>
-      <c r="ACW14" s="31"/>
-      <c r="ACX14" s="31"/>
-      <c r="ACY14" s="31"/>
-      <c r="ACZ14" s="31"/>
-      <c r="ADA14" s="31"/>
-      <c r="ADB14" s="31"/>
-      <c r="ADC14" s="31"/>
-      <c r="ADD14" s="31"/>
-      <c r="ADE14" s="31"/>
-      <c r="ADF14" s="31"/>
-      <c r="ADG14" s="31"/>
-      <c r="ADH14" s="31"/>
-      <c r="ADI14" s="31"/>
-      <c r="ADJ14" s="31"/>
-      <c r="ADK14" s="31"/>
-      <c r="ADL14" s="31"/>
-      <c r="ADM14" s="31"/>
-      <c r="ADN14" s="31"/>
-      <c r="ADO14" s="31"/>
-      <c r="ADP14" s="31"/>
-      <c r="ADQ14" s="31"/>
-      <c r="ADR14" s="31"/>
-      <c r="ADS14" s="31"/>
-      <c r="ADT14" s="31"/>
-      <c r="ADU14" s="31"/>
-      <c r="ADV14" s="31"/>
-      <c r="ADW14" s="31"/>
-      <c r="ADX14" s="31"/>
-      <c r="ADY14" s="31"/>
-      <c r="ADZ14" s="31"/>
-      <c r="AEA14" s="31"/>
-      <c r="AEB14" s="31"/>
-      <c r="AEC14" s="31"/>
-      <c r="AED14" s="31"/>
-      <c r="AEE14" s="31"/>
-      <c r="AEF14" s="31"/>
-      <c r="AEG14" s="31"/>
-      <c r="AEH14" s="31"/>
-      <c r="AEI14" s="31"/>
-      <c r="AEJ14" s="31"/>
-      <c r="AEK14" s="31"/>
-      <c r="AEL14" s="31"/>
-      <c r="AEM14" s="31"/>
-      <c r="AEN14" s="31"/>
-      <c r="AEO14" s="31"/>
-      <c r="AEP14" s="31"/>
-      <c r="AEQ14" s="31"/>
-      <c r="AER14" s="31"/>
-      <c r="AES14" s="31"/>
-      <c r="AET14" s="31"/>
-      <c r="AEU14" s="31"/>
-      <c r="AEV14" s="31"/>
-      <c r="AEW14" s="31"/>
-      <c r="AEX14" s="31"/>
-      <c r="AEY14" s="31"/>
-      <c r="AEZ14" s="31"/>
-      <c r="AFA14" s="31"/>
-      <c r="AFB14" s="31"/>
-      <c r="AFC14" s="31"/>
-      <c r="AFD14" s="31"/>
-      <c r="AFE14" s="31"/>
-      <c r="AFF14" s="31"/>
-      <c r="AFG14" s="31"/>
-      <c r="AFH14" s="31"/>
-      <c r="AFI14" s="31"/>
-      <c r="AFJ14" s="31"/>
-      <c r="AFK14" s="31"/>
-      <c r="AFL14" s="31"/>
-      <c r="AFM14" s="31"/>
-      <c r="AFN14" s="31"/>
-      <c r="AFO14" s="31"/>
-      <c r="AFP14" s="31"/>
-      <c r="AFQ14" s="31"/>
-      <c r="AFR14" s="31"/>
-      <c r="AFS14" s="31"/>
-      <c r="AFT14" s="31"/>
-      <c r="AFU14" s="31"/>
-      <c r="AFV14" s="31"/>
-      <c r="AFW14" s="31"/>
-      <c r="AFX14" s="31"/>
-      <c r="AFY14" s="31"/>
-      <c r="AFZ14" s="31"/>
-      <c r="AGA14" s="31"/>
-      <c r="AGB14" s="31"/>
-      <c r="AGC14" s="31"/>
-      <c r="AGD14" s="31"/>
-      <c r="AGE14" s="31"/>
-      <c r="AGF14" s="31"/>
-      <c r="AGG14" s="31"/>
-      <c r="AGH14" s="31"/>
-      <c r="AGI14" s="31"/>
-      <c r="AGJ14" s="31"/>
-      <c r="AGK14" s="31"/>
-      <c r="AGL14" s="31"/>
-      <c r="AGM14" s="31"/>
-      <c r="AGN14" s="31"/>
-      <c r="AGO14" s="31"/>
-      <c r="AGP14" s="31"/>
-      <c r="AGQ14" s="31"/>
-      <c r="AGR14" s="31"/>
-      <c r="AGS14" s="31"/>
-      <c r="AGT14" s="31"/>
-      <c r="AGU14" s="31"/>
-      <c r="AGV14" s="31"/>
-      <c r="AGW14" s="31"/>
-      <c r="AGX14" s="31"/>
-      <c r="AGY14" s="31"/>
-      <c r="AGZ14" s="31"/>
-      <c r="AHA14" s="31"/>
-      <c r="AHB14" s="31"/>
-      <c r="AHC14" s="31"/>
-      <c r="AHD14" s="31"/>
-      <c r="AHE14" s="31"/>
-      <c r="AHF14" s="31"/>
-      <c r="AHG14" s="31"/>
-      <c r="AHH14" s="31"/>
-      <c r="AHI14" s="31"/>
-      <c r="AHJ14" s="31"/>
-      <c r="AHK14" s="31"/>
-      <c r="AHL14" s="31"/>
-      <c r="AHM14" s="31"/>
-      <c r="AHN14" s="31"/>
-      <c r="AHO14" s="31"/>
-      <c r="AHP14" s="31"/>
-      <c r="AHQ14" s="31"/>
-      <c r="AHR14" s="31"/>
-      <c r="AHS14" s="31"/>
-      <c r="AHT14" s="31"/>
-      <c r="AHU14" s="31"/>
-      <c r="AHV14" s="31"/>
-      <c r="AHW14" s="31"/>
-      <c r="AHX14" s="31"/>
-      <c r="AHY14" s="31"/>
-      <c r="AHZ14" s="31"/>
-      <c r="AIA14" s="31"/>
-      <c r="AIB14" s="31"/>
-      <c r="AIC14" s="31"/>
-      <c r="AID14" s="31"/>
-      <c r="AIE14" s="31"/>
-      <c r="AIF14" s="31"/>
-      <c r="AIG14" s="31"/>
-      <c r="AIH14" s="31"/>
-      <c r="AII14" s="31"/>
-      <c r="AIJ14" s="31"/>
-      <c r="AIK14" s="31"/>
-      <c r="AIL14" s="31"/>
-      <c r="AIM14" s="31"/>
-      <c r="AIN14" s="31"/>
-      <c r="AIO14" s="31"/>
-      <c r="AIP14" s="31"/>
-      <c r="AIQ14" s="31"/>
-      <c r="AIR14" s="31"/>
-      <c r="AIS14" s="31"/>
-      <c r="AIT14" s="31"/>
-      <c r="AIU14" s="31"/>
-      <c r="AIV14" s="31"/>
-      <c r="AIW14" s="31"/>
-      <c r="AIX14" s="31"/>
-      <c r="AIY14" s="31"/>
-      <c r="AIZ14" s="31"/>
-      <c r="AJA14" s="31"/>
-      <c r="AJB14" s="31"/>
-      <c r="AJC14" s="31"/>
-      <c r="AJD14" s="31"/>
-      <c r="AJE14" s="31"/>
-      <c r="AJF14" s="31"/>
-      <c r="AJG14" s="31"/>
-      <c r="AJH14" s="31"/>
-      <c r="AJI14" s="31"/>
-      <c r="AJJ14" s="31"/>
-      <c r="AJK14" s="31"/>
-      <c r="AJL14" s="31"/>
-      <c r="AJM14" s="31"/>
-      <c r="AJN14" s="31"/>
-      <c r="AJO14" s="31"/>
-      <c r="AJP14" s="31"/>
-      <c r="AJQ14" s="31"/>
-      <c r="AJR14" s="31"/>
-      <c r="AJS14" s="31"/>
-      <c r="AJT14" s="31"/>
-      <c r="AJU14" s="31"/>
-      <c r="AJV14" s="31"/>
-      <c r="AJW14" s="31"/>
-      <c r="AJX14" s="31"/>
-      <c r="AJY14" s="31"/>
-      <c r="AJZ14" s="31"/>
-      <c r="AKA14" s="31"/>
-      <c r="AKB14" s="31"/>
-      <c r="AKC14" s="31"/>
-      <c r="AKD14" s="31"/>
-      <c r="AKE14" s="31"/>
-      <c r="AKF14" s="31"/>
-      <c r="AKG14" s="31"/>
-      <c r="AKH14" s="31"/>
-      <c r="AKI14" s="31"/>
-      <c r="AKJ14" s="31"/>
-      <c r="AKK14" s="31"/>
-      <c r="AKL14" s="31"/>
-      <c r="AKM14" s="31"/>
-      <c r="AKN14" s="31"/>
-      <c r="AKO14" s="31"/>
-      <c r="AKP14" s="31"/>
-      <c r="AKQ14" s="31"/>
-      <c r="AKR14" s="31"/>
-      <c r="AKS14" s="31"/>
-      <c r="AKT14" s="31"/>
-      <c r="AKU14" s="31"/>
-      <c r="AKV14" s="31"/>
-      <c r="AKW14" s="31"/>
-      <c r="AKX14" s="31"/>
-      <c r="AKY14" s="31"/>
-      <c r="AKZ14" s="31"/>
-      <c r="ALA14" s="31"/>
-      <c r="ALB14" s="31"/>
-      <c r="ALC14" s="31"/>
-      <c r="ALD14" s="31"/>
-      <c r="ALE14" s="31"/>
-      <c r="ALF14" s="31"/>
-      <c r="ALG14" s="31"/>
-      <c r="ALH14" s="31"/>
-      <c r="ALI14" s="31"/>
-      <c r="ALJ14" s="31"/>
-      <c r="ALK14" s="31"/>
-      <c r="ALL14" s="31"/>
-      <c r="ALM14" s="31"/>
-      <c r="ALN14" s="31"/>
-      <c r="ALO14" s="31"/>
-      <c r="ALP14" s="31"/>
-      <c r="ALQ14" s="31"/>
-      <c r="ALR14" s="31"/>
-      <c r="ALS14" s="31"/>
-      <c r="ALT14" s="31"/>
-      <c r="ALU14" s="31"/>
-      <c r="ALV14" s="31"/>
-      <c r="ALW14" s="31"/>
-      <c r="ALX14" s="31"/>
-      <c r="ALY14" s="31"/>
-      <c r="ALZ14" s="31"/>
-      <c r="AMA14" s="31"/>
-      <c r="AMB14" s="31"/>
-      <c r="AMC14" s="31"/>
-      <c r="AMD14" s="31"/>
-      <c r="AME14" s="31"/>
-      <c r="AMF14" s="31"/>
-      <c r="AMG14" s="31"/>
-      <c r="AMH14" s="31"/>
-      <c r="AMI14" s="31"/>
+      <c r="W14" s="29"/>
+      <c r="Y14" s="29"/>
+      <c r="AA14" s="29"/>
+      <c r="AB14" s="29"/>
+      <c r="AC14" s="29"/>
+      <c r="AD14" s="29"/>
+      <c r="AE14" s="29"/>
+      <c r="AF14" s="29"/>
+      <c r="AG14" s="29"/>
+      <c r="AH14" s="29"/>
+      <c r="AI14" s="29"/>
+      <c r="AJ14" s="29"/>
+      <c r="AK14" s="29"/>
+      <c r="AL14" s="29"/>
+      <c r="AM14" s="29"/>
+      <c r="AN14" s="29"/>
+      <c r="AO14" s="29"/>
+      <c r="AP14" s="29"/>
+      <c r="AQ14" s="29"/>
+      <c r="AR14" s="29"/>
+      <c r="AS14" s="29"/>
+      <c r="AT14" s="29"/>
+      <c r="AU14" s="29"/>
+      <c r="AV14" s="29"/>
+      <c r="AW14" s="29"/>
+      <c r="AX14" s="29"/>
+      <c r="AY14" s="29"/>
+      <c r="AZ14" s="29"/>
+      <c r="BA14" s="29"/>
+      <c r="BB14" s="29"/>
+      <c r="BC14" s="29"/>
+      <c r="BD14" s="29"/>
+      <c r="BE14" s="29"/>
+      <c r="BF14" s="29"/>
+      <c r="BG14" s="29"/>
+      <c r="BH14" s="29"/>
+      <c r="BI14" s="29"/>
+      <c r="BJ14" s="29"/>
+      <c r="BK14" s="29"/>
+      <c r="BL14" s="29"/>
+      <c r="BM14" s="29"/>
+      <c r="BN14" s="29"/>
+      <c r="BO14" s="29"/>
+      <c r="BP14" s="29"/>
+      <c r="BQ14" s="29"/>
+      <c r="BR14" s="29"/>
+      <c r="BS14" s="29"/>
+      <c r="BT14" s="29"/>
+      <c r="BU14" s="29"/>
+      <c r="BV14" s="29"/>
+      <c r="BW14" s="29"/>
+      <c r="BX14" s="29"/>
+      <c r="BY14" s="29"/>
+      <c r="BZ14" s="29"/>
+      <c r="CA14" s="29"/>
+      <c r="CB14" s="29"/>
+      <c r="CC14" s="29"/>
+      <c r="CD14" s="29"/>
+      <c r="CE14" s="29"/>
+      <c r="CF14" s="29"/>
+      <c r="CG14" s="29"/>
+      <c r="CH14" s="29"/>
+      <c r="CI14" s="29"/>
+      <c r="CJ14" s="29"/>
+      <c r="CK14" s="29"/>
+      <c r="CL14" s="29"/>
+      <c r="CM14" s="29"/>
+      <c r="CN14" s="29"/>
+      <c r="CO14" s="29"/>
+      <c r="CP14" s="29"/>
+      <c r="CQ14" s="29"/>
+      <c r="CR14" s="29"/>
+      <c r="CS14" s="29"/>
+      <c r="CT14" s="29"/>
+      <c r="CU14" s="29"/>
+      <c r="CV14" s="29"/>
+      <c r="CW14" s="29"/>
+      <c r="CX14" s="29"/>
+      <c r="CY14" s="29"/>
+      <c r="CZ14" s="29"/>
+      <c r="DA14" s="29"/>
+      <c r="DB14" s="29"/>
+      <c r="DC14" s="29"/>
+      <c r="DD14" s="29"/>
+      <c r="DE14" s="29"/>
+      <c r="DF14" s="29"/>
+      <c r="DG14" s="29"/>
+      <c r="DH14" s="29"/>
+      <c r="DI14" s="29"/>
+      <c r="DJ14" s="29"/>
+      <c r="DK14" s="29"/>
+      <c r="DL14" s="29"/>
+      <c r="DM14" s="29"/>
+      <c r="DN14" s="29"/>
+      <c r="DO14" s="29"/>
+      <c r="DP14" s="29"/>
+      <c r="DQ14" s="29"/>
+      <c r="DR14" s="29"/>
+      <c r="DS14" s="29"/>
+      <c r="DT14" s="29"/>
+      <c r="DU14" s="29"/>
+      <c r="DV14" s="29"/>
+      <c r="DW14" s="29"/>
+      <c r="DX14" s="29"/>
+      <c r="DY14" s="29"/>
+      <c r="DZ14" s="29"/>
+      <c r="EA14" s="29"/>
+      <c r="EB14" s="29"/>
+      <c r="EC14" s="29"/>
+      <c r="ED14" s="29"/>
+      <c r="EE14" s="29"/>
+      <c r="EF14" s="29"/>
+      <c r="EG14" s="29"/>
+      <c r="EH14" s="29"/>
+      <c r="EI14" s="29"/>
+      <c r="EJ14" s="29"/>
+      <c r="EK14" s="29"/>
+      <c r="EL14" s="29"/>
+      <c r="EM14" s="29"/>
+      <c r="EN14" s="29"/>
+      <c r="EO14" s="29"/>
+      <c r="EP14" s="29"/>
+      <c r="EQ14" s="29"/>
+      <c r="ER14" s="29"/>
+      <c r="ES14" s="29"/>
+      <c r="ET14" s="29"/>
+      <c r="EU14" s="29"/>
+      <c r="EV14" s="29"/>
+      <c r="EW14" s="29"/>
+      <c r="EX14" s="29"/>
+      <c r="EY14" s="29"/>
+      <c r="EZ14" s="29"/>
+      <c r="FA14" s="29"/>
+      <c r="FB14" s="29"/>
+      <c r="FC14" s="29"/>
+      <c r="FD14" s="29"/>
+      <c r="FE14" s="29"/>
+      <c r="FF14" s="29"/>
+      <c r="FG14" s="29"/>
+      <c r="FH14" s="29"/>
+      <c r="FI14" s="29"/>
+      <c r="FJ14" s="29"/>
+      <c r="FK14" s="29"/>
+      <c r="FL14" s="29"/>
+      <c r="FM14" s="29"/>
+      <c r="FN14" s="29"/>
+      <c r="FO14" s="29"/>
+      <c r="FP14" s="29"/>
+      <c r="FQ14" s="29"/>
+      <c r="FR14" s="29"/>
+      <c r="FS14" s="29"/>
+      <c r="FT14" s="29"/>
+      <c r="FU14" s="29"/>
+      <c r="FV14" s="29"/>
+      <c r="FW14" s="29"/>
+      <c r="FX14" s="29"/>
+      <c r="FY14" s="29"/>
+      <c r="FZ14" s="29"/>
+      <c r="GA14" s="29"/>
+      <c r="GB14" s="29"/>
+      <c r="GC14" s="29"/>
+      <c r="GD14" s="29"/>
+      <c r="GE14" s="29"/>
+      <c r="GF14" s="29"/>
+      <c r="GG14" s="29"/>
+      <c r="GH14" s="29"/>
+      <c r="GI14" s="29"/>
+      <c r="GJ14" s="29"/>
+      <c r="GK14" s="29"/>
+      <c r="GL14" s="29"/>
+      <c r="GM14" s="29"/>
+      <c r="GN14" s="29"/>
+      <c r="GO14" s="29"/>
+      <c r="GP14" s="29"/>
+      <c r="GQ14" s="29"/>
+      <c r="GR14" s="29"/>
+      <c r="GS14" s="29"/>
+      <c r="GT14" s="29"/>
+      <c r="GU14" s="29"/>
+      <c r="GV14" s="29"/>
+      <c r="GW14" s="29"/>
+      <c r="GX14" s="29"/>
+      <c r="GY14" s="29"/>
+      <c r="GZ14" s="29"/>
+      <c r="HA14" s="29"/>
+      <c r="HB14" s="29"/>
+      <c r="HC14" s="29"/>
+      <c r="HD14" s="29"/>
+      <c r="HE14" s="29"/>
+      <c r="HF14" s="29"/>
+      <c r="HG14" s="29"/>
+      <c r="HH14" s="29"/>
+      <c r="HI14" s="29"/>
+      <c r="HJ14" s="29"/>
+      <c r="HK14" s="29"/>
+      <c r="HL14" s="29"/>
+      <c r="HM14" s="29"/>
+      <c r="HN14" s="29"/>
+      <c r="HO14" s="29"/>
+      <c r="HP14" s="29"/>
+      <c r="HQ14" s="29"/>
+      <c r="HR14" s="29"/>
+      <c r="HS14" s="29"/>
+      <c r="HT14" s="29"/>
+      <c r="HU14" s="29"/>
+      <c r="HV14" s="29"/>
+      <c r="HW14" s="29"/>
+      <c r="HX14" s="29"/>
+      <c r="HY14" s="29"/>
+      <c r="HZ14" s="29"/>
+      <c r="IA14" s="29"/>
+      <c r="IB14" s="29"/>
+      <c r="IC14" s="29"/>
+      <c r="ID14" s="29"/>
+      <c r="IE14" s="29"/>
+      <c r="IF14" s="29"/>
+      <c r="IG14" s="29"/>
+      <c r="IH14" s="29"/>
+      <c r="II14" s="29"/>
+      <c r="IJ14" s="29"/>
+      <c r="IK14" s="29"/>
+      <c r="IL14" s="29"/>
+      <c r="IM14" s="29"/>
+      <c r="IN14" s="29"/>
+      <c r="IO14" s="29"/>
+      <c r="IP14" s="29"/>
+      <c r="IQ14" s="29"/>
+      <c r="IR14" s="29"/>
+      <c r="IS14" s="29"/>
+      <c r="IT14" s="29"/>
+      <c r="IU14" s="29"/>
+      <c r="IV14" s="29"/>
+      <c r="IW14" s="29"/>
+      <c r="IX14" s="29"/>
+      <c r="IY14" s="29"/>
+      <c r="IZ14" s="29"/>
+      <c r="JA14" s="29"/>
+      <c r="JB14" s="29"/>
+      <c r="JC14" s="29"/>
+      <c r="JD14" s="29"/>
+      <c r="JE14" s="29"/>
+      <c r="JF14" s="29"/>
+      <c r="JG14" s="29"/>
+      <c r="JH14" s="29"/>
+      <c r="JI14" s="29"/>
+      <c r="JJ14" s="29"/>
+      <c r="JK14" s="29"/>
+      <c r="JL14" s="29"/>
+      <c r="JM14" s="29"/>
+      <c r="JN14" s="29"/>
+      <c r="JO14" s="29"/>
+      <c r="JP14" s="29"/>
+      <c r="JQ14" s="29"/>
+      <c r="JR14" s="29"/>
+      <c r="JS14" s="29"/>
+      <c r="JT14" s="29"/>
+      <c r="JU14" s="29"/>
+      <c r="JV14" s="29"/>
+      <c r="JW14" s="29"/>
+      <c r="JX14" s="29"/>
+      <c r="JY14" s="29"/>
+      <c r="JZ14" s="29"/>
+      <c r="KA14" s="29"/>
+      <c r="KB14" s="29"/>
+      <c r="KC14" s="29"/>
+      <c r="KD14" s="29"/>
+      <c r="KE14" s="29"/>
+      <c r="KF14" s="29"/>
+      <c r="KG14" s="29"/>
+      <c r="KH14" s="29"/>
+      <c r="KI14" s="29"/>
+      <c r="KJ14" s="29"/>
+      <c r="KK14" s="29"/>
+      <c r="KL14" s="29"/>
+      <c r="KM14" s="29"/>
+      <c r="KN14" s="29"/>
+      <c r="KO14" s="29"/>
+      <c r="KP14" s="29"/>
+      <c r="KQ14" s="29"/>
+      <c r="KR14" s="29"/>
+      <c r="KS14" s="29"/>
+      <c r="KT14" s="29"/>
+      <c r="KU14" s="29"/>
+      <c r="KV14" s="29"/>
+      <c r="KW14" s="29"/>
+      <c r="KX14" s="29"/>
+      <c r="KY14" s="29"/>
+      <c r="KZ14" s="29"/>
+      <c r="LA14" s="29"/>
+      <c r="LB14" s="29"/>
+      <c r="LC14" s="29"/>
+      <c r="LD14" s="29"/>
+      <c r="LE14" s="29"/>
+      <c r="LF14" s="29"/>
+      <c r="LG14" s="29"/>
+      <c r="LH14" s="29"/>
+      <c r="LI14" s="29"/>
+      <c r="LJ14" s="29"/>
+      <c r="LK14" s="29"/>
+      <c r="LL14" s="29"/>
+      <c r="LM14" s="29"/>
+      <c r="LN14" s="29"/>
+      <c r="LO14" s="29"/>
+      <c r="LP14" s="29"/>
+      <c r="LQ14" s="29"/>
+      <c r="LR14" s="29"/>
+      <c r="LS14" s="29"/>
+      <c r="LT14" s="29"/>
+      <c r="LU14" s="29"/>
+      <c r="LV14" s="29"/>
+      <c r="LW14" s="29"/>
+      <c r="LX14" s="29"/>
+      <c r="LY14" s="29"/>
+      <c r="LZ14" s="29"/>
+      <c r="MA14" s="29"/>
+      <c r="MB14" s="29"/>
+      <c r="MC14" s="29"/>
+      <c r="MD14" s="29"/>
+      <c r="ME14" s="29"/>
+      <c r="MF14" s="29"/>
+      <c r="MG14" s="29"/>
+      <c r="MH14" s="29"/>
+      <c r="MI14" s="29"/>
+      <c r="MJ14" s="29"/>
+      <c r="MK14" s="29"/>
+      <c r="ML14" s="29"/>
+      <c r="MM14" s="29"/>
+      <c r="MN14" s="29"/>
+      <c r="MO14" s="29"/>
+      <c r="MP14" s="29"/>
+      <c r="MQ14" s="29"/>
+      <c r="MR14" s="29"/>
+      <c r="MS14" s="29"/>
+      <c r="MT14" s="29"/>
+      <c r="MU14" s="29"/>
+      <c r="MV14" s="29"/>
+      <c r="MW14" s="29"/>
+      <c r="MX14" s="29"/>
+      <c r="MY14" s="29"/>
+      <c r="MZ14" s="29"/>
+      <c r="NA14" s="29"/>
+      <c r="NB14" s="29"/>
+      <c r="NC14" s="29"/>
+      <c r="ND14" s="29"/>
+      <c r="NE14" s="29"/>
+      <c r="NF14" s="29"/>
+      <c r="NG14" s="29"/>
+      <c r="NH14" s="29"/>
+      <c r="NI14" s="29"/>
+      <c r="NJ14" s="29"/>
+      <c r="NK14" s="29"/>
+      <c r="NL14" s="29"/>
+      <c r="NM14" s="29"/>
+      <c r="NN14" s="29"/>
+      <c r="NO14" s="29"/>
+      <c r="NP14" s="29"/>
+      <c r="NQ14" s="29"/>
+      <c r="NR14" s="29"/>
+      <c r="NS14" s="29"/>
+      <c r="NT14" s="29"/>
+      <c r="NU14" s="29"/>
+      <c r="NV14" s="29"/>
+      <c r="NW14" s="29"/>
+      <c r="NX14" s="29"/>
+      <c r="NY14" s="29"/>
+      <c r="NZ14" s="29"/>
+      <c r="OA14" s="29"/>
+      <c r="OB14" s="29"/>
+      <c r="OC14" s="29"/>
+      <c r="OD14" s="29"/>
+      <c r="OE14" s="29"/>
+      <c r="OF14" s="29"/>
+      <c r="OG14" s="29"/>
+      <c r="OH14" s="29"/>
+      <c r="OI14" s="29"/>
+      <c r="OJ14" s="29"/>
+      <c r="OK14" s="29"/>
+      <c r="OL14" s="29"/>
+      <c r="OM14" s="29"/>
+      <c r="ON14" s="29"/>
+      <c r="OO14" s="29"/>
+      <c r="OP14" s="29"/>
+      <c r="OQ14" s="29"/>
+      <c r="OR14" s="29"/>
+      <c r="OS14" s="29"/>
+      <c r="OT14" s="29"/>
+      <c r="OU14" s="29"/>
+      <c r="OV14" s="29"/>
+      <c r="OW14" s="29"/>
+      <c r="OX14" s="29"/>
+      <c r="OY14" s="29"/>
+      <c r="OZ14" s="29"/>
+      <c r="PA14" s="29"/>
+      <c r="PB14" s="29"/>
+      <c r="PC14" s="29"/>
+      <c r="PD14" s="29"/>
+      <c r="PE14" s="29"/>
+      <c r="PF14" s="29"/>
+      <c r="PG14" s="29"/>
+      <c r="PH14" s="29"/>
+      <c r="PI14" s="29"/>
+      <c r="PJ14" s="29"/>
+      <c r="PK14" s="29"/>
+      <c r="PL14" s="29"/>
+      <c r="PM14" s="29"/>
+      <c r="PN14" s="29"/>
+      <c r="PO14" s="29"/>
+      <c r="PP14" s="29"/>
+      <c r="PQ14" s="29"/>
+      <c r="PR14" s="29"/>
+      <c r="PS14" s="29"/>
+      <c r="PT14" s="29"/>
+      <c r="PU14" s="29"/>
+      <c r="PV14" s="29"/>
+      <c r="PW14" s="29"/>
+      <c r="PX14" s="29"/>
+      <c r="PY14" s="29"/>
+      <c r="PZ14" s="29"/>
+      <c r="QA14" s="29"/>
+      <c r="QB14" s="29"/>
+      <c r="QC14" s="29"/>
+      <c r="QD14" s="29"/>
+      <c r="QE14" s="29"/>
+      <c r="QF14" s="29"/>
+      <c r="QG14" s="29"/>
+      <c r="QH14" s="29"/>
+      <c r="QI14" s="29"/>
+      <c r="QJ14" s="29"/>
+      <c r="QK14" s="29"/>
+      <c r="QL14" s="29"/>
+      <c r="QM14" s="29"/>
+      <c r="QN14" s="29"/>
+      <c r="QO14" s="29"/>
+      <c r="QP14" s="29"/>
+      <c r="QQ14" s="29"/>
+      <c r="QR14" s="29"/>
+      <c r="QS14" s="29"/>
+      <c r="QT14" s="29"/>
+      <c r="QU14" s="29"/>
+      <c r="QV14" s="29"/>
+      <c r="QW14" s="29"/>
+      <c r="QX14" s="29"/>
+      <c r="QY14" s="29"/>
+      <c r="QZ14" s="29"/>
+      <c r="RA14" s="29"/>
+      <c r="RB14" s="29"/>
+      <c r="RC14" s="29"/>
+      <c r="RD14" s="29"/>
+      <c r="RE14" s="29"/>
+      <c r="RF14" s="29"/>
+      <c r="RG14" s="29"/>
+      <c r="RH14" s="29"/>
+      <c r="RI14" s="29"/>
+      <c r="RJ14" s="29"/>
+      <c r="RK14" s="29"/>
+      <c r="RL14" s="29"/>
+      <c r="RM14" s="29"/>
+      <c r="RN14" s="29"/>
+      <c r="RO14" s="29"/>
+      <c r="RP14" s="29"/>
+      <c r="RQ14" s="29"/>
+      <c r="RR14" s="29"/>
+      <c r="RS14" s="29"/>
+      <c r="RT14" s="29"/>
+      <c r="RU14" s="29"/>
+      <c r="RV14" s="29"/>
+      <c r="RW14" s="29"/>
+      <c r="RX14" s="29"/>
+      <c r="RY14" s="29"/>
+      <c r="RZ14" s="29"/>
+      <c r="SA14" s="29"/>
+      <c r="SB14" s="29"/>
+      <c r="SC14" s="29"/>
+      <c r="SD14" s="29"/>
+      <c r="SE14" s="29"/>
+      <c r="SF14" s="29"/>
+      <c r="SG14" s="29"/>
+      <c r="SH14" s="29"/>
+      <c r="SI14" s="29"/>
+      <c r="SJ14" s="29"/>
+      <c r="SK14" s="29"/>
+      <c r="SL14" s="29"/>
+      <c r="SM14" s="29"/>
+      <c r="SN14" s="29"/>
+      <c r="SO14" s="29"/>
+      <c r="SP14" s="29"/>
+      <c r="SQ14" s="29"/>
+      <c r="SR14" s="29"/>
+      <c r="SS14" s="29"/>
+      <c r="ST14" s="29"/>
+      <c r="SU14" s="29"/>
+      <c r="SV14" s="29"/>
+      <c r="SW14" s="29"/>
+      <c r="SX14" s="29"/>
+      <c r="SY14" s="29"/>
+      <c r="SZ14" s="29"/>
+      <c r="TA14" s="29"/>
+      <c r="TB14" s="29"/>
+      <c r="TC14" s="29"/>
+      <c r="TD14" s="29"/>
+      <c r="TE14" s="29"/>
+      <c r="TF14" s="29"/>
+      <c r="TG14" s="29"/>
+      <c r="TH14" s="29"/>
+      <c r="TI14" s="29"/>
+      <c r="TJ14" s="29"/>
+      <c r="TK14" s="29"/>
+      <c r="TL14" s="29"/>
+      <c r="TM14" s="29"/>
+      <c r="TN14" s="29"/>
+      <c r="TO14" s="29"/>
+      <c r="TP14" s="29"/>
+      <c r="TQ14" s="29"/>
+      <c r="TR14" s="29"/>
+      <c r="TS14" s="29"/>
+      <c r="TT14" s="29"/>
+      <c r="TU14" s="29"/>
+      <c r="TV14" s="29"/>
+      <c r="TW14" s="29"/>
+      <c r="TX14" s="29"/>
+      <c r="TY14" s="29"/>
+      <c r="TZ14" s="29"/>
+      <c r="UA14" s="29"/>
+      <c r="UB14" s="29"/>
+      <c r="UC14" s="29"/>
+      <c r="UD14" s="29"/>
+      <c r="UE14" s="29"/>
+      <c r="UF14" s="29"/>
+      <c r="UG14" s="29"/>
+      <c r="UH14" s="29"/>
+      <c r="UI14" s="29"/>
+      <c r="UJ14" s="29"/>
+      <c r="UK14" s="29"/>
+      <c r="UL14" s="29"/>
+      <c r="UM14" s="29"/>
+      <c r="UN14" s="29"/>
+      <c r="UO14" s="29"/>
+      <c r="UP14" s="29"/>
+      <c r="UQ14" s="29"/>
+      <c r="UR14" s="29"/>
+      <c r="US14" s="29"/>
+      <c r="UT14" s="29"/>
+      <c r="UU14" s="29"/>
+      <c r="UV14" s="29"/>
+      <c r="UW14" s="29"/>
+      <c r="UX14" s="29"/>
+      <c r="UY14" s="29"/>
+      <c r="UZ14" s="29"/>
+      <c r="VA14" s="29"/>
+      <c r="VB14" s="29"/>
+      <c r="VC14" s="29"/>
+      <c r="VD14" s="29"/>
+      <c r="VE14" s="29"/>
+      <c r="VF14" s="29"/>
+      <c r="VG14" s="29"/>
+      <c r="VH14" s="29"/>
+      <c r="VI14" s="29"/>
+      <c r="VJ14" s="29"/>
+      <c r="VK14" s="29"/>
+      <c r="VL14" s="29"/>
+      <c r="VM14" s="29"/>
+      <c r="VN14" s="29"/>
+      <c r="VO14" s="29"/>
+      <c r="VP14" s="29"/>
+      <c r="VQ14" s="29"/>
+      <c r="VR14" s="29"/>
+      <c r="VS14" s="29"/>
+      <c r="VT14" s="29"/>
+      <c r="VU14" s="29"/>
+      <c r="VV14" s="29"/>
+      <c r="VW14" s="29"/>
+      <c r="VX14" s="29"/>
+      <c r="VY14" s="29"/>
+      <c r="VZ14" s="29"/>
+      <c r="WA14" s="29"/>
+      <c r="WB14" s="29"/>
+      <c r="WC14" s="29"/>
+      <c r="WD14" s="29"/>
+      <c r="WE14" s="29"/>
+      <c r="WF14" s="29"/>
+      <c r="WG14" s="29"/>
+      <c r="WH14" s="29"/>
+      <c r="WI14" s="29"/>
+      <c r="WJ14" s="29"/>
+      <c r="WK14" s="29"/>
+      <c r="WL14" s="29"/>
+      <c r="WM14" s="29"/>
+      <c r="WN14" s="29"/>
+      <c r="WO14" s="29"/>
+      <c r="WP14" s="29"/>
+      <c r="WQ14" s="29"/>
+      <c r="WR14" s="29"/>
+      <c r="WS14" s="29"/>
+      <c r="WT14" s="29"/>
+      <c r="WU14" s="29"/>
+      <c r="WV14" s="29"/>
+      <c r="WW14" s="29"/>
+      <c r="WX14" s="29"/>
+      <c r="WY14" s="29"/>
+      <c r="WZ14" s="29"/>
+      <c r="XA14" s="29"/>
+      <c r="XB14" s="29"/>
+      <c r="XC14" s="29"/>
+      <c r="XD14" s="29"/>
+      <c r="XE14" s="29"/>
+      <c r="XF14" s="29"/>
+      <c r="XG14" s="29"/>
+      <c r="XH14" s="29"/>
+      <c r="XI14" s="29"/>
+      <c r="XJ14" s="29"/>
+      <c r="XK14" s="29"/>
+      <c r="XL14" s="29"/>
+      <c r="XM14" s="29"/>
+      <c r="XN14" s="29"/>
+      <c r="XO14" s="29"/>
+      <c r="XP14" s="29"/>
+      <c r="XQ14" s="29"/>
+      <c r="XR14" s="29"/>
+      <c r="XS14" s="29"/>
+      <c r="XT14" s="29"/>
+      <c r="XU14" s="29"/>
+      <c r="XV14" s="29"/>
+      <c r="XW14" s="29"/>
+      <c r="XX14" s="29"/>
+      <c r="XY14" s="29"/>
+      <c r="XZ14" s="29"/>
+      <c r="YA14" s="29"/>
+      <c r="YB14" s="29"/>
+      <c r="YC14" s="29"/>
+      <c r="YD14" s="29"/>
+      <c r="YE14" s="29"/>
+      <c r="YF14" s="29"/>
+      <c r="YG14" s="29"/>
+      <c r="YH14" s="29"/>
+      <c r="YI14" s="29"/>
+      <c r="YJ14" s="29"/>
+      <c r="YK14" s="29"/>
+      <c r="YL14" s="29"/>
+      <c r="YM14" s="29"/>
+      <c r="YN14" s="29"/>
+      <c r="YO14" s="29"/>
+      <c r="YP14" s="29"/>
+      <c r="YQ14" s="29"/>
+      <c r="YR14" s="29"/>
+      <c r="YS14" s="29"/>
+      <c r="YT14" s="29"/>
+      <c r="YU14" s="29"/>
+      <c r="YV14" s="29"/>
+      <c r="YW14" s="29"/>
+      <c r="YX14" s="29"/>
+      <c r="YY14" s="29"/>
+      <c r="YZ14" s="29"/>
+      <c r="ZA14" s="29"/>
+      <c r="ZB14" s="29"/>
+      <c r="ZC14" s="29"/>
+      <c r="ZD14" s="29"/>
+      <c r="ZE14" s="29"/>
+      <c r="ZF14" s="29"/>
+      <c r="ZG14" s="29"/>
+      <c r="ZH14" s="29"/>
+      <c r="ZI14" s="29"/>
+      <c r="ZJ14" s="29"/>
+      <c r="ZK14" s="29"/>
+      <c r="ZL14" s="29"/>
+      <c r="ZM14" s="29"/>
+      <c r="ZN14" s="29"/>
+      <c r="ZO14" s="29"/>
+      <c r="ZP14" s="29"/>
+      <c r="ZQ14" s="29"/>
+      <c r="ZR14" s="29"/>
+      <c r="ZS14" s="29"/>
+      <c r="ZT14" s="29"/>
+      <c r="ZU14" s="29"/>
+      <c r="ZV14" s="29"/>
+      <c r="ZW14" s="29"/>
+      <c r="ZX14" s="29"/>
+      <c r="ZY14" s="29"/>
+      <c r="ZZ14" s="29"/>
+      <c r="AAA14" s="29"/>
+      <c r="AAB14" s="29"/>
+      <c r="AAC14" s="29"/>
+      <c r="AAD14" s="29"/>
+      <c r="AAE14" s="29"/>
+      <c r="AAF14" s="29"/>
+      <c r="AAG14" s="29"/>
+      <c r="AAH14" s="29"/>
+      <c r="AAI14" s="29"/>
+      <c r="AAJ14" s="29"/>
+      <c r="AAK14" s="29"/>
+      <c r="AAL14" s="29"/>
+      <c r="AAM14" s="29"/>
+      <c r="AAN14" s="29"/>
+      <c r="AAO14" s="29"/>
+      <c r="AAP14" s="29"/>
+      <c r="AAQ14" s="29"/>
+      <c r="AAR14" s="29"/>
+      <c r="AAS14" s="29"/>
+      <c r="AAT14" s="29"/>
+      <c r="AAU14" s="29"/>
+      <c r="AAV14" s="29"/>
+      <c r="AAW14" s="29"/>
+      <c r="AAX14" s="29"/>
+      <c r="AAY14" s="29"/>
+      <c r="AAZ14" s="29"/>
+      <c r="ABA14" s="29"/>
+      <c r="ABB14" s="29"/>
+      <c r="ABC14" s="29"/>
+      <c r="ABD14" s="29"/>
+      <c r="ABE14" s="29"/>
+      <c r="ABF14" s="29"/>
+      <c r="ABG14" s="29"/>
+      <c r="ABH14" s="29"/>
+      <c r="ABI14" s="29"/>
+      <c r="ABJ14" s="29"/>
+      <c r="ABK14" s="29"/>
+      <c r="ABL14" s="29"/>
+      <c r="ABM14" s="29"/>
+      <c r="ABN14" s="29"/>
+      <c r="ABO14" s="29"/>
+      <c r="ABP14" s="29"/>
+      <c r="ABQ14" s="29"/>
+      <c r="ABR14" s="29"/>
+      <c r="ABS14" s="29"/>
+      <c r="ABT14" s="29"/>
+      <c r="ABU14" s="29"/>
+      <c r="ABV14" s="29"/>
+      <c r="ABW14" s="29"/>
+      <c r="ABX14" s="29"/>
+      <c r="ABY14" s="29"/>
+      <c r="ABZ14" s="29"/>
+      <c r="ACA14" s="29"/>
+      <c r="ACB14" s="29"/>
+      <c r="ACC14" s="29"/>
+      <c r="ACD14" s="29"/>
+      <c r="ACE14" s="29"/>
+      <c r="ACF14" s="29"/>
+      <c r="ACG14" s="29"/>
+      <c r="ACH14" s="29"/>
+      <c r="ACI14" s="29"/>
+      <c r="ACJ14" s="29"/>
+      <c r="ACK14" s="29"/>
+      <c r="ACL14" s="29"/>
+      <c r="ACM14" s="29"/>
+      <c r="ACN14" s="29"/>
+      <c r="ACO14" s="29"/>
+      <c r="ACP14" s="29"/>
+      <c r="ACQ14" s="29"/>
+      <c r="ACR14" s="29"/>
+      <c r="ACS14" s="29"/>
+      <c r="ACT14" s="29"/>
+      <c r="ACU14" s="29"/>
+      <c r="ACV14" s="29"/>
+      <c r="ACW14" s="29"/>
+      <c r="ACX14" s="29"/>
+      <c r="ACY14" s="29"/>
+      <c r="ACZ14" s="29"/>
+      <c r="ADA14" s="29"/>
+      <c r="ADB14" s="29"/>
+      <c r="ADC14" s="29"/>
+      <c r="ADD14" s="29"/>
+      <c r="ADE14" s="29"/>
+      <c r="ADF14" s="29"/>
+      <c r="ADG14" s="29"/>
+      <c r="ADH14" s="29"/>
+      <c r="ADI14" s="29"/>
+      <c r="ADJ14" s="29"/>
+      <c r="ADK14" s="29"/>
+      <c r="ADL14" s="29"/>
+      <c r="ADM14" s="29"/>
+      <c r="ADN14" s="29"/>
+      <c r="ADO14" s="29"/>
+      <c r="ADP14" s="29"/>
+      <c r="ADQ14" s="29"/>
+      <c r="ADR14" s="29"/>
+      <c r="ADS14" s="29"/>
+      <c r="ADT14" s="29"/>
+      <c r="ADU14" s="29"/>
+      <c r="ADV14" s="29"/>
+      <c r="ADW14" s="29"/>
+      <c r="ADX14" s="29"/>
+      <c r="ADY14" s="29"/>
+      <c r="ADZ14" s="29"/>
+      <c r="AEA14" s="29"/>
+      <c r="AEB14" s="29"/>
+      <c r="AEC14" s="29"/>
+      <c r="AED14" s="29"/>
+      <c r="AEE14" s="29"/>
+      <c r="AEF14" s="29"/>
+      <c r="AEG14" s="29"/>
+      <c r="AEH14" s="29"/>
+      <c r="AEI14" s="29"/>
+      <c r="AEJ14" s="29"/>
+      <c r="AEK14" s="29"/>
+      <c r="AEL14" s="29"/>
+      <c r="AEM14" s="29"/>
+      <c r="AEN14" s="29"/>
+      <c r="AEO14" s="29"/>
+      <c r="AEP14" s="29"/>
+      <c r="AEQ14" s="29"/>
+      <c r="AER14" s="29"/>
+      <c r="AES14" s="29"/>
+      <c r="AET14" s="29"/>
+      <c r="AEU14" s="29"/>
+      <c r="AEV14" s="29"/>
+      <c r="AEW14" s="29"/>
+      <c r="AEX14" s="29"/>
+      <c r="AEY14" s="29"/>
+      <c r="AEZ14" s="29"/>
+      <c r="AFA14" s="29"/>
+      <c r="AFB14" s="29"/>
+      <c r="AFC14" s="29"/>
+      <c r="AFD14" s="29"/>
+      <c r="AFE14" s="29"/>
+      <c r="AFF14" s="29"/>
+      <c r="AFG14" s="29"/>
+      <c r="AFH14" s="29"/>
+      <c r="AFI14" s="29"/>
+      <c r="AFJ14" s="29"/>
+      <c r="AFK14" s="29"/>
+      <c r="AFL14" s="29"/>
+      <c r="AFM14" s="29"/>
+      <c r="AFN14" s="29"/>
+      <c r="AFO14" s="29"/>
+      <c r="AFP14" s="29"/>
+      <c r="AFQ14" s="29"/>
+      <c r="AFR14" s="29"/>
+      <c r="AFS14" s="29"/>
+      <c r="AFT14" s="29"/>
+      <c r="AFU14" s="29"/>
+      <c r="AFV14" s="29"/>
+      <c r="AFW14" s="29"/>
+      <c r="AFX14" s="29"/>
+      <c r="AFY14" s="29"/>
+      <c r="AFZ14" s="29"/>
+      <c r="AGA14" s="29"/>
+      <c r="AGB14" s="29"/>
+      <c r="AGC14" s="29"/>
+      <c r="AGD14" s="29"/>
+      <c r="AGE14" s="29"/>
+      <c r="AGF14" s="29"/>
+      <c r="AGG14" s="29"/>
+      <c r="AGH14" s="29"/>
+      <c r="AGI14" s="29"/>
+      <c r="AGJ14" s="29"/>
+      <c r="AGK14" s="29"/>
+      <c r="AGL14" s="29"/>
+      <c r="AGM14" s="29"/>
+      <c r="AGN14" s="29"/>
+      <c r="AGO14" s="29"/>
+      <c r="AGP14" s="29"/>
+      <c r="AGQ14" s="29"/>
+      <c r="AGR14" s="29"/>
+      <c r="AGS14" s="29"/>
+      <c r="AGT14" s="29"/>
+      <c r="AGU14" s="29"/>
+      <c r="AGV14" s="29"/>
+      <c r="AGW14" s="29"/>
+      <c r="AGX14" s="29"/>
+      <c r="AGY14" s="29"/>
+      <c r="AGZ14" s="29"/>
+      <c r="AHA14" s="29"/>
+      <c r="AHB14" s="29"/>
+      <c r="AHC14" s="29"/>
+      <c r="AHD14" s="29"/>
+      <c r="AHE14" s="29"/>
+      <c r="AHF14" s="29"/>
+      <c r="AHG14" s="29"/>
+      <c r="AHH14" s="29"/>
+      <c r="AHI14" s="29"/>
+      <c r="AHJ14" s="29"/>
+      <c r="AHK14" s="29"/>
+      <c r="AHL14" s="29"/>
+      <c r="AHM14" s="29"/>
+      <c r="AHN14" s="29"/>
+      <c r="AHO14" s="29"/>
+      <c r="AHP14" s="29"/>
+      <c r="AHQ14" s="29"/>
+      <c r="AHR14" s="29"/>
+      <c r="AHS14" s="29"/>
+      <c r="AHT14" s="29"/>
+      <c r="AHU14" s="29"/>
+      <c r="AHV14" s="29"/>
+      <c r="AHW14" s="29"/>
+      <c r="AHX14" s="29"/>
+      <c r="AHY14" s="29"/>
+      <c r="AHZ14" s="29"/>
+      <c r="AIA14" s="29"/>
+      <c r="AIB14" s="29"/>
+      <c r="AIC14" s="29"/>
+      <c r="AID14" s="29"/>
+      <c r="AIE14" s="29"/>
+      <c r="AIF14" s="29"/>
+      <c r="AIG14" s="29"/>
+      <c r="AIH14" s="29"/>
+      <c r="AII14" s="29"/>
+      <c r="AIJ14" s="29"/>
+      <c r="AIK14" s="29"/>
+      <c r="AIL14" s="29"/>
+      <c r="AIM14" s="29"/>
+      <c r="AIN14" s="29"/>
+      <c r="AIO14" s="29"/>
+      <c r="AIP14" s="29"/>
+      <c r="AIQ14" s="29"/>
+      <c r="AIR14" s="29"/>
+      <c r="AIS14" s="29"/>
+      <c r="AIT14" s="29"/>
+      <c r="AIU14" s="29"/>
+      <c r="AIV14" s="29"/>
+      <c r="AIW14" s="29"/>
+      <c r="AIX14" s="29"/>
+      <c r="AIY14" s="29"/>
+      <c r="AIZ14" s="29"/>
+      <c r="AJA14" s="29"/>
+      <c r="AJB14" s="29"/>
+      <c r="AJC14" s="29"/>
+      <c r="AJD14" s="29"/>
+      <c r="AJE14" s="29"/>
+      <c r="AJF14" s="29"/>
+      <c r="AJG14" s="29"/>
+      <c r="AJH14" s="29"/>
+      <c r="AJI14" s="29"/>
+      <c r="AJJ14" s="29"/>
+      <c r="AJK14" s="29"/>
+      <c r="AJL14" s="29"/>
+      <c r="AJM14" s="29"/>
+      <c r="AJN14" s="29"/>
+      <c r="AJO14" s="29"/>
+      <c r="AJP14" s="29"/>
+      <c r="AJQ14" s="29"/>
+      <c r="AJR14" s="29"/>
+      <c r="AJS14" s="29"/>
+      <c r="AJT14" s="29"/>
+      <c r="AJU14" s="29"/>
+      <c r="AJV14" s="29"/>
+      <c r="AJW14" s="29"/>
+      <c r="AJX14" s="29"/>
+      <c r="AJY14" s="29"/>
+      <c r="AJZ14" s="29"/>
+      <c r="AKA14" s="29"/>
+      <c r="AKB14" s="29"/>
+      <c r="AKC14" s="29"/>
+      <c r="AKD14" s="29"/>
+      <c r="AKE14" s="29"/>
+      <c r="AKF14" s="29"/>
+      <c r="AKG14" s="29"/>
+      <c r="AKH14" s="29"/>
+      <c r="AKI14" s="29"/>
+      <c r="AKJ14" s="29"/>
+      <c r="AKK14" s="29"/>
+      <c r="AKL14" s="29"/>
+      <c r="AKM14" s="29"/>
+      <c r="AKN14" s="29"/>
+      <c r="AKO14" s="29"/>
+      <c r="AKP14" s="29"/>
+      <c r="AKQ14" s="29"/>
+      <c r="AKR14" s="29"/>
+      <c r="AKS14" s="29"/>
+      <c r="AKT14" s="29"/>
+      <c r="AKU14" s="29"/>
+      <c r="AKV14" s="29"/>
+      <c r="AKW14" s="29"/>
+      <c r="AKX14" s="29"/>
+      <c r="AKY14" s="29"/>
+      <c r="AKZ14" s="29"/>
+      <c r="ALA14" s="29"/>
+      <c r="ALB14" s="29"/>
+      <c r="ALC14" s="29"/>
+      <c r="ALD14" s="29"/>
+      <c r="ALE14" s="29"/>
+      <c r="ALF14" s="29"/>
+      <c r="ALG14" s="29"/>
+      <c r="ALH14" s="29"/>
+      <c r="ALI14" s="29"/>
+      <c r="ALJ14" s="29"/>
+      <c r="ALK14" s="29"/>
+      <c r="ALL14" s="29"/>
+      <c r="ALM14" s="29"/>
+      <c r="ALN14" s="29"/>
+      <c r="ALO14" s="29"/>
+      <c r="ALP14" s="29"/>
+      <c r="ALQ14" s="29"/>
+      <c r="ALR14" s="29"/>
+      <c r="ALS14" s="29"/>
+      <c r="ALT14" s="29"/>
+      <c r="ALU14" s="29"/>
+      <c r="ALV14" s="29"/>
+      <c r="ALW14" s="29"/>
+      <c r="ALX14" s="29"/>
+      <c r="ALY14" s="29"/>
+      <c r="ALZ14" s="29"/>
+      <c r="AMA14" s="29"/>
+      <c r="AMB14" s="29"/>
+      <c r="AMC14" s="29"/>
+      <c r="AMD14" s="29"/>
+      <c r="AME14" s="29"/>
+      <c r="AMF14" s="29"/>
+      <c r="AMG14" s="29"/>
+      <c r="AMH14" s="29"/>
+      <c r="AMI14" s="29"/>
     </row>
     <row r="15" s="8" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="n">
@@ -3898,13 +3890,13 @@
       <c r="C15" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="26" t="s">
         <v>73</v>
       </c>
       <c r="E15" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F15" s="28" t="n">
+      <c r="F15" s="14" t="n">
         <v>156842</v>
       </c>
       <c r="G15" s="8" t="n">
@@ -3969,13 +3961,13 @@
       <c r="C16" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>75</v>
       </c>
       <c r="E16" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="F16" s="28" t="n">
+      <c r="F16" s="14" t="n">
         <v>157127</v>
       </c>
       <c r="G16" s="8" t="n">
@@ -4042,13 +4034,13 @@
       <c r="C17" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="26" t="s">
         <v>77</v>
       </c>
       <c r="E17" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="28" t="n">
+      <c r="F17" s="14" t="n">
         <v>311953</v>
       </c>
       <c r="G17" s="8" t="n">
@@ -4113,13 +4105,13 @@
       <c r="C18" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="26" t="s">
         <v>79</v>
       </c>
       <c r="E18" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="F18" s="28" t="n">
+      <c r="F18" s="14" t="n">
         <v>192626</v>
       </c>
       <c r="G18" s="2" t="n">
@@ -5171,13 +5163,13 @@
       <c r="C19" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="26" t="s">
         <v>81</v>
       </c>
       <c r="E19" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="F19" s="28" t="n">
+      <c r="F19" s="14" t="n">
         <v>195139</v>
       </c>
       <c r="G19" s="1" t="n">
@@ -5227,13 +5219,13 @@
       <c r="C20" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="26" t="s">
         <v>83</v>
       </c>
       <c r="E20" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="F20" s="28" t="n">
+      <c r="F20" s="14" t="n">
         <v>155187</v>
       </c>
       <c r="G20" s="1" t="n">
@@ -5283,13 +5275,13 @@
       <c r="C21" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="26" t="s">
         <v>85</v>
       </c>
       <c r="E21" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="F21" s="28" t="n">
+      <c r="F21" s="14" t="n">
         <v>156952</v>
       </c>
       <c r="G21" s="1" t="n">
@@ -5339,13 +5331,13 @@
       <c r="C22" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="26" t="s">
         <v>87</v>
       </c>
       <c r="E22" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="F22" s="28" t="n">
+      <c r="F22" s="14" t="n">
         <v>156959</v>
       </c>
       <c r="G22" s="1" t="n">
@@ -5395,13 +5387,13 @@
       <c r="C23" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="26" t="s">
         <v>89</v>
       </c>
       <c r="E23" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="F23" s="28" t="n">
+      <c r="F23" s="14" t="n">
         <v>194484</v>
       </c>
       <c r="G23" s="1" t="n">
@@ -5451,13 +5443,13 @@
       <c r="C24" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="26" t="s">
         <v>91</v>
       </c>
       <c r="E24" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="F24" s="28" t="n">
+      <c r="F24" s="14" t="n">
         <v>151885</v>
       </c>
       <c r="G24" s="1" t="n">
@@ -5512,13 +5504,13 @@
       <c r="C25" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="D25" s="26" t="s">
         <v>93</v>
       </c>
       <c r="E25" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="F25" s="28" t="n">
+      <c r="F25" s="14" t="n">
         <v>156764</v>
       </c>
       <c r="G25" s="8" t="n">
@@ -5573,13 +5565,13 @@
       <c r="C26" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="26" t="s">
         <v>95</v>
       </c>
       <c r="E26" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="F26" s="28" t="n">
+      <c r="F26" s="14" t="n">
         <v>156809</v>
       </c>
       <c r="G26" s="8" t="n">
@@ -5634,13 +5626,13 @@
       <c r="C27" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="26" t="s">
         <v>97</v>
       </c>
       <c r="E27" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="F27" s="28" t="n">
+      <c r="F27" s="14" t="n">
         <v>157271</v>
       </c>
       <c r="G27" s="2" t="n">
@@ -5695,13 +5687,13 @@
       <c r="C28" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="26" t="s">
         <v>99</v>
       </c>
       <c r="E28" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="F28" s="28" t="n">
+      <c r="F28" s="14" t="n">
         <v>155742</v>
       </c>
       <c r="G28" s="1" t="n">
@@ -5756,13 +5748,13 @@
       <c r="C29" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="26" t="s">
         <v>101</v>
       </c>
       <c r="E29" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F29" s="28" t="n">
+      <c r="F29" s="14" t="n">
         <v>151835</v>
       </c>
       <c r="H29" s="1" t="n">
@@ -5814,13 +5806,13 @@
       <c r="C30" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="26" t="s">
         <v>103</v>
       </c>
       <c r="E30" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F30" s="28" t="n">
+      <c r="F30" s="14" t="n">
         <v>192832</v>
       </c>
       <c r="H30" s="1" t="n">
@@ -5872,13 +5864,13 @@
       <c r="C31" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="27" t="s">
+      <c r="D31" s="26" t="s">
         <v>105</v>
       </c>
       <c r="E31" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F31" s="28" t="n">
+      <c r="F31" s="14" t="n">
         <v>192643</v>
       </c>
       <c r="H31" s="1" t="n">
@@ -5930,13 +5922,13 @@
       <c r="C32" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="D32" s="26" t="s">
         <v>107</v>
       </c>
       <c r="E32" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F32" s="28" t="n">
+      <c r="F32" s="14" t="n">
         <v>311954</v>
       </c>
       <c r="H32" s="1" t="n">
@@ -5988,13 +5980,13 @@
       <c r="C33" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="26" t="s">
         <v>109</v>
       </c>
       <c r="E33" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F33" s="28" t="n">
+      <c r="F33" s="14" t="n">
         <v>195287</v>
       </c>
       <c r="H33" s="1" t="n">
@@ -6046,13 +6038,13 @@
       <c r="C34" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D34" s="27" t="s">
+      <c r="D34" s="26" t="s">
         <v>111</v>
       </c>
       <c r="E34" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="F34" s="28" t="n">
+      <c r="F34" s="14" t="n">
         <v>151886</v>
       </c>
       <c r="H34" s="1" t="n">
@@ -6104,13 +6096,13 @@
       <c r="C35" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="26" t="s">
         <v>113</v>
       </c>
       <c r="E35" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="F35" s="28" t="n">
+      <c r="F35" s="14" t="n">
         <v>180478</v>
       </c>
       <c r="H35" s="1" t="n">
@@ -6162,13 +6154,13 @@
       <c r="C36" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="26" t="s">
         <v>115</v>
       </c>
       <c r="E36" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="F36" s="28" t="n">
+      <c r="F36" s="14" t="n">
         <v>179413</v>
       </c>
       <c r="H36" s="1" t="n">
@@ -6220,13 +6212,13 @@
       <c r="C37" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="26" t="s">
         <v>117</v>
       </c>
       <c r="E37" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="F37" s="28" t="n">
+      <c r="F37" s="14" t="n">
         <v>142306</v>
       </c>
       <c r="H37" s="1" t="n">
@@ -6278,13 +6270,13 @@
       <c r="C38" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="26" t="s">
         <v>119</v>
       </c>
       <c r="E38" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="F38" s="28" t="n">
+      <c r="F38" s="14" t="n">
         <v>142300</v>
       </c>
       <c r="H38" s="1" t="n">
@@ -6336,13 +6328,13 @@
       <c r="C39" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="27" t="s">
+      <c r="D39" s="26" t="s">
         <v>121</v>
       </c>
       <c r="E39" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F39" s="28" t="n">
+      <c r="F39" s="14" t="n">
         <v>151157</v>
       </c>
       <c r="H39" s="1" t="n">
@@ -6394,13 +6386,13 @@
       <c r="C40" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D40" s="27" t="s">
+      <c r="D40" s="26" t="s">
         <v>123</v>
       </c>
       <c r="E40" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F40" s="28" t="n">
+      <c r="F40" s="14" t="n">
         <v>196958</v>
       </c>
       <c r="H40" s="1" t="n">
@@ -6452,13 +6444,13 @@
       <c r="C41" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="D41" s="27" t="s">
+      <c r="D41" s="26" t="s">
         <v>125</v>
       </c>
       <c r="E41" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F41" s="28" t="n">
+      <c r="F41" s="14" t="n">
         <v>142396</v>
       </c>
       <c r="H41" s="1" t="n">
@@ -6510,13 +6502,13 @@
       <c r="C42" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D42" s="27" t="s">
+      <c r="D42" s="26" t="s">
         <v>127</v>
       </c>
       <c r="E42" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F42" s="28" t="n">
+      <c r="F42" s="14" t="n">
         <v>137844</v>
       </c>
       <c r="H42" s="1" t="n">
@@ -6568,13 +6560,13 @@
       <c r="C43" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="27" t="s">
+      <c r="D43" s="26" t="s">
         <v>129</v>
       </c>
       <c r="E43" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F43" s="28" t="n">
+      <c r="F43" s="14" t="n">
         <v>142153</v>
       </c>
       <c r="H43" s="1" t="n">

</xml_diff>

<commit_message>
feat：update stage config change and excel
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Monster_怪物表.xlsx
+++ b/nevergiveup/Excel/Monster_怪物表.xlsx
@@ -487,7 +487,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,13 +503,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF4000"/>
-        <bgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF5429"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00A933"/>
         <bgColor rgb="FF008000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5429"/>
+        <bgColor rgb="FFFF4000"/>
       </patternFill>
     </fill>
   </fills>
@@ -561,7 +567,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -714,6 +720,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,7 +737,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -770,7 +780,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF4000"/>
+      <rgbColor rgb="FFFF5429"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -900,9 +910,9 @@
   <dimension ref="A1:AMI376"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="D19" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" ySplit="0" topLeftCell="N19" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="topRight" activeCell="C44" activeCellId="0" sqref="C44"/>
+      <selection pane="topRight" activeCell="S40" activeCellId="0" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4985,8 +4995,8 @@
       <c r="G31" s="2" t="n">
         <v>281015</v>
       </c>
-      <c r="H31" s="2" t="n">
-        <v>600</v>
+      <c r="H31" s="38" t="n">
+        <v>300</v>
       </c>
       <c r="I31" s="2" t="n">
         <v>105</v>
@@ -5024,11 +5034,11 @@
       <c r="T31" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="U31" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="V31" s="2" t="n">
-        <v>50</v>
+      <c r="U31" s="38" t="n">
+        <v>100</v>
+      </c>
+      <c r="V31" s="38" t="n">
+        <v>0</v>
       </c>
       <c r="X31" s="10"/>
       <c r="Z31" s="10"/>
@@ -5052,8 +5062,8 @@
       <c r="G32" s="2" t="n">
         <v>281015</v>
       </c>
-      <c r="H32" s="2" t="n">
-        <v>700</v>
+      <c r="H32" s="38" t="n">
+        <v>500</v>
       </c>
       <c r="I32" s="2" t="n">
         <v>105</v>
@@ -5091,11 +5101,11 @@
       <c r="T32" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="U32" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="V32" s="2" t="n">
-        <v>50</v>
+      <c r="U32" s="38" t="n">
+        <v>200</v>
+      </c>
+      <c r="V32" s="38" t="n">
+        <v>0</v>
       </c>
       <c r="X32" s="10"/>
       <c r="Z32" s="10"/>
@@ -5630,11 +5640,11 @@
       <c r="T40" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="U40" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="V40" s="2" t="n">
-        <v>100</v>
+      <c r="U40" s="38" t="n">
+        <v>200</v>
+      </c>
+      <c r="V40" s="38" t="n">
+        <v>200</v>
       </c>
       <c r="X40" s="10"/>
       <c r="Z40" s="10"/>

</xml_diff>

<commit_message>
feat：update world1 stage change
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Monster_怪物表.xlsx
+++ b/nevergiveup/Excel/Monster_怪物表.xlsx
@@ -909,10 +909,10 @@
   </sheetPr>
   <dimension ref="A1:AMI376"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="N19" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="topRight" activeCell="S40" activeCellId="0" sqref="S40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="0" topLeftCell="D16" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topRight" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat：update world3 easy stageconfig
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Monster_怪物表.xlsx
+++ b/nevergiveup/Excel/Monster_怪物表.xlsx
@@ -919,10 +919,10 @@
   </sheetPr>
   <dimension ref="A1:AMI376"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="D4" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="topRight" activeCell="K16" activeCellId="0" sqref="K16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="0" topLeftCell="D10" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topRight" activeCell="D25" activeCellId="0" sqref="25:25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4639,11 +4639,11 @@
       <c r="T25" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="U25" s="2" t="n">
-        <v>70</v>
-      </c>
-      <c r="V25" s="2" t="n">
-        <v>70</v>
+      <c r="U25" s="26" t="n">
+        <v>150</v>
+      </c>
+      <c r="V25" s="26" t="n">
+        <v>0</v>
       </c>
       <c r="X25" s="10"/>
       <c r="Z25" s="10"/>

</xml_diff>

<commit_message>
feat：update monster excel and stage config
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Monster_怪物表.xlsx
+++ b/nevergiveup/Excel/Monster_怪物表.xlsx
@@ -922,7 +922,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="0" topLeftCell="D10" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="topRight" activeCell="D25" activeCellId="0" sqref="25:25"/>
+      <selection pane="topRight" activeCell="K20" activeCellId="0" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4737,8 +4737,8 @@
       <c r="H27" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="I27" s="2" t="n">
-        <v>75</v>
+      <c r="I27" s="37" t="n">
+        <v>50</v>
       </c>
       <c r="J27" s="13" t="n">
         <v>107535</v>
@@ -5276,8 +5276,8 @@
       <c r="H35" s="2" t="n">
         <v>1200</v>
       </c>
-      <c r="I35" s="2" t="n">
-        <v>90</v>
+      <c r="I35" s="37" t="n">
+        <v>30</v>
       </c>
       <c r="J35" s="13" t="n">
         <v>107535</v>
@@ -5312,11 +5312,11 @@
       <c r="T35" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="U35" s="2" t="n">
-        <v>70</v>
-      </c>
-      <c r="V35" s="2" t="n">
-        <v>70</v>
+      <c r="U35" s="37" t="n">
+        <v>300</v>
+      </c>
+      <c r="V35" s="37" t="n">
+        <v>30</v>
       </c>
       <c r="X35" s="10"/>
       <c r="Z35" s="10"/>

</xml_diff>

<commit_message>
feat：update world5 easy change
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Monster_怪物表.xlsx
+++ b/nevergiveup/Excel/Monster_怪物表.xlsx
@@ -919,10 +919,10 @@
   </sheetPr>
   <dimension ref="A1:AMI376"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="D10" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="topRight" activeCell="K20" activeCellId="0" sqref="K20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="0" topLeftCell="D13" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topRight" activeCell="D35" activeCellId="0" sqref="35:35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5449,11 +5449,11 @@
       <c r="T37" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="U37" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="V37" s="2" t="n">
-        <v>50</v>
+      <c r="U37" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" s="37" t="n">
+        <v>45</v>
       </c>
       <c r="X37" s="10"/>
       <c r="Z37" s="10"/>
@@ -5480,8 +5480,8 @@
       <c r="H38" s="2" t="n">
         <v>700</v>
       </c>
-      <c r="I38" s="2" t="n">
-        <v>105</v>
+      <c r="I38" s="37" t="n">
+        <v>90</v>
       </c>
       <c r="J38" s="13" t="n">
         <v>107535</v>
@@ -5516,11 +5516,11 @@
       <c r="T38" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="U38" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="V38" s="2" t="n">
-        <v>50</v>
+      <c r="U38" s="37" t="n">
+        <v>10</v>
+      </c>
+      <c r="V38" s="37" t="n">
+        <v>90</v>
       </c>
       <c r="X38" s="10"/>
       <c r="Z38" s="10"/>

</xml_diff>

<commit_message>
fix: dead anim time
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Monster_怪物表.xlsx
+++ b/nevergiveup/Excel/Monster_怪物表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30708" windowHeight="14100" tabRatio="500"/>
+    <workbookView windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -596,10 +596,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -652,7 +652,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -660,21 +660,21 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -682,7 +682,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -690,7 +690,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -698,7 +698,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -706,7 +706,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -714,14 +714,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -729,7 +729,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -737,7 +737,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -745,14 +745,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -760,42 +760,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1192,11 +1192,11 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1486,55 +1486,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -1940,12 +1940,12 @@
   <dimension ref="A1:AMJ373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A3" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <selection pane="bottomLeft" activeCell="T5" sqref="T5:T70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="7.25" style="4" customWidth="1"/>
     <col min="2" max="2" width="5.9" style="4" customWidth="1"/>
@@ -2257,7 +2257,7 @@
       <c r="Y4" s="10"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" s="1" customFormat="1" ht="16.2" spans="1:33">
+    <row r="5" s="1" customFormat="1" spans="1:33">
       <c r="A5" s="10">
         <v>1001</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>285139</v>
       </c>
       <c r="T5" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U5" s="1">
         <v>3</v>
@@ -2333,7 +2333,7 @@
       <c r="AD5" s="53"/>
       <c r="AG5" s="53"/>
     </row>
-    <row r="6" s="1" customFormat="1" ht="16.2" spans="1:27">
+    <row r="6" s="1" customFormat="1" spans="1:27">
       <c r="A6" s="10">
         <v>1002</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>285139</v>
       </c>
       <c r="T6" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U6" s="1">
         <v>3</v>
@@ -2407,7 +2407,7 @@
       <c r="Y6" s="52"/>
       <c r="AA6" s="52"/>
     </row>
-    <row r="7" s="1" customFormat="1" ht="16.2" spans="1:33">
+    <row r="7" s="1" customFormat="1" spans="1:33">
       <c r="A7" s="10">
         <v>1003</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>20291</v>
       </c>
       <c r="T7" s="1">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="U7" s="1">
         <v>3</v>
@@ -2484,7 +2484,7 @@
       <c r="AD7" s="53"/>
       <c r="AG7" s="53"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="16.2" spans="1:27">
+    <row r="8" s="1" customFormat="1" spans="1:27">
       <c r="A8" s="10">
         <v>1004</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>285395</v>
       </c>
       <c r="T8" s="1">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="U8" s="1">
         <v>3</v>
@@ -2558,7 +2558,7 @@
       <c r="Y8" s="52"/>
       <c r="AA8" s="52"/>
     </row>
-    <row r="9" s="1" customFormat="1" ht="16.2" spans="1:27">
+    <row r="9" s="1" customFormat="1" spans="1:27">
       <c r="A9" s="10">
         <v>1005</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>285139</v>
       </c>
       <c r="T9" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U9" s="1">
         <v>3</v>
@@ -2632,7 +2632,7 @@
       <c r="Y9" s="52"/>
       <c r="AA9" s="52"/>
     </row>
-    <row r="10" s="1" customFormat="1" ht="16.2" spans="1:27">
+    <row r="10" s="1" customFormat="1" spans="1:27">
       <c r="A10" s="10">
         <v>1006</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>285139</v>
       </c>
       <c r="T10" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U10" s="1">
         <v>3</v>
@@ -2763,7 +2763,7 @@
         <v>281693</v>
       </c>
       <c r="T11" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U11" s="1">
         <v>3</v>
@@ -2832,8 +2832,8 @@
       <c r="S12" s="18">
         <v>281693</v>
       </c>
-      <c r="T12" s="17">
-        <v>1.5</v>
+      <c r="T12" s="1">
+        <v>0.8</v>
       </c>
       <c r="U12" s="17">
         <v>3</v>
@@ -3900,7 +3900,7 @@
         <v>281693</v>
       </c>
       <c r="T13" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U13" s="1">
         <v>3</v>
@@ -3972,7 +3972,7 @@
         <v>281693</v>
       </c>
       <c r="T14" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U14" s="1">
         <v>3</v>
@@ -4983,7 +4983,7 @@
       <c r="AMI14" s="25"/>
       <c r="AMJ14" s="25"/>
     </row>
-    <row r="15" s="1" customFormat="1" ht="16.2" spans="1:27">
+    <row r="15" s="1" customFormat="1" spans="1:27">
       <c r="A15" s="1">
         <v>1011</v>
       </c>
@@ -5039,7 +5039,7 @@
         <v>281693</v>
       </c>
       <c r="T15" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U15" s="1">
         <v>3</v>
@@ -5054,7 +5054,7 @@
       <c r="Y15" s="52"/>
       <c r="AA15" s="52"/>
     </row>
-    <row r="16" s="1" customFormat="1" ht="16.2" spans="1:33">
+    <row r="16" s="1" customFormat="1" spans="1:33">
       <c r="A16" s="1">
         <v>1012</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>281693</v>
       </c>
       <c r="T16" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U16" s="1">
         <v>3</v>
@@ -5129,7 +5129,7 @@
       <c r="AD16" s="53"/>
       <c r="AG16" s="53"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="16.2" spans="1:27">
+    <row r="17" s="1" customFormat="1" spans="1:27">
       <c r="A17" s="1">
         <v>1013</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>281693</v>
       </c>
       <c r="T17" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U17" s="1">
         <v>3</v>
@@ -5256,7 +5256,7 @@
         <v>281693</v>
       </c>
       <c r="T18" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U18" s="1">
         <v>3</v>
@@ -5327,7 +5327,7 @@
         <v>281693</v>
       </c>
       <c r="T19" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U19" s="1">
         <v>3</v>
@@ -5396,7 +5396,7 @@
         <v>281693</v>
       </c>
       <c r="T20" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U20" s="1">
         <v>3</v>
@@ -5465,7 +5465,7 @@
         <v>281693</v>
       </c>
       <c r="T21" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U21" s="1">
         <v>3</v>
@@ -5534,7 +5534,7 @@
         <v>281693</v>
       </c>
       <c r="T22" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U22" s="1">
         <v>3</v>
@@ -5603,7 +5603,7 @@
         <v>281693</v>
       </c>
       <c r="T23" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U23" s="1">
         <v>3</v>
@@ -5674,7 +5674,7 @@
         <v>281693</v>
       </c>
       <c r="T24" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U24" s="1">
         <v>3</v>
@@ -5745,7 +5745,7 @@
         <v>281693</v>
       </c>
       <c r="T25" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U25" s="1">
         <v>3</v>
@@ -5816,7 +5816,7 @@
         <v>281693</v>
       </c>
       <c r="T26" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U26" s="1">
         <v>3</v>
@@ -5887,7 +5887,7 @@
         <v>281693</v>
       </c>
       <c r="T27" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U27" s="1">
         <v>3</v>
@@ -5960,7 +5960,7 @@
         <v>281693</v>
       </c>
       <c r="T28" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U28" s="1">
         <v>3</v>
@@ -6031,7 +6031,7 @@
         <v>281693</v>
       </c>
       <c r="T29" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U29" s="1">
         <v>3</v>
@@ -6102,7 +6102,7 @@
         <v>281693</v>
       </c>
       <c r="T30" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U30" s="1">
         <v>3</v>
@@ -6173,7 +6173,7 @@
         <v>281693</v>
       </c>
       <c r="T31" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U31" s="1">
         <v>3</v>
@@ -6244,7 +6244,7 @@
         <v>281693</v>
       </c>
       <c r="T32" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U32" s="1">
         <v>3</v>
@@ -6315,7 +6315,7 @@
         <v>281693</v>
       </c>
       <c r="T33" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U33" s="1">
         <v>3</v>
@@ -6386,7 +6386,7 @@
         <v>281693</v>
       </c>
       <c r="T34" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U34" s="1">
         <v>3</v>
@@ -6457,7 +6457,7 @@
         <v>281693</v>
       </c>
       <c r="T35" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U35" s="1">
         <v>3</v>
@@ -6528,7 +6528,7 @@
         <v>281693</v>
       </c>
       <c r="T36" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U36" s="1">
         <v>3</v>
@@ -6601,7 +6601,7 @@
         <v>281693</v>
       </c>
       <c r="T37" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U37" s="1">
         <v>3</v>
@@ -6672,7 +6672,7 @@
         <v>281693</v>
       </c>
       <c r="T38" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U38" s="1">
         <v>3</v>
@@ -6743,7 +6743,7 @@
         <v>281693</v>
       </c>
       <c r="T39" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U39" s="1">
         <v>3</v>
@@ -6814,7 +6814,7 @@
         <v>281693</v>
       </c>
       <c r="T40" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U40" s="1">
         <v>3</v>
@@ -6885,7 +6885,7 @@
         <v>281693</v>
       </c>
       <c r="T41" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U41" s="1">
         <v>3</v>
@@ -6956,7 +6956,7 @@
         <v>281693</v>
       </c>
       <c r="T42" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U42" s="1">
         <v>3</v>
@@ -7030,7 +7030,7 @@
         <v>281693</v>
       </c>
       <c r="T43" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U43" s="1">
         <v>3</v>
@@ -7045,7 +7045,7 @@
       <c r="Y43" s="10"/>
       <c r="AA43" s="10"/>
     </row>
-    <row r="44" ht="16.35" spans="1:1024">
+    <row r="44" ht="17.25" spans="1:1024">
       <c r="A44" s="31">
         <v>1040</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>281693</v>
       </c>
       <c r="T44" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U44" s="1">
         <v>3</v>
@@ -8117,7 +8117,7 @@
       <c r="AMI44" s="1"/>
       <c r="AMJ44" s="1"/>
     </row>
-    <row r="45" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="45" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A45" s="36">
         <v>1041</v>
       </c>
@@ -8174,7 +8174,7 @@
         <v>281693</v>
       </c>
       <c r="T45" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U45" s="1">
         <v>3</v>
@@ -8191,7 +8191,7 @@
       <c r="Y45" s="10"/>
       <c r="AA45" s="10"/>
     </row>
-    <row r="46" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="46" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A46" s="36">
         <v>1042</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>281693</v>
       </c>
       <c r="T46" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U46" s="1">
         <v>3</v>
@@ -8263,7 +8263,7 @@
       <c r="Y46" s="10"/>
       <c r="AA46" s="10"/>
     </row>
-    <row r="47" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="47" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A47" s="39">
         <v>1043</v>
       </c>
@@ -8320,7 +8320,7 @@
         <v>281693</v>
       </c>
       <c r="T47" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U47" s="1">
         <v>3</v>
@@ -8335,7 +8335,7 @@
       <c r="Y47" s="10"/>
       <c r="AA47" s="10"/>
     </row>
-    <row r="48" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="48" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A48" s="36">
         <v>1044</v>
       </c>
@@ -8392,7 +8392,7 @@
         <v>281693</v>
       </c>
       <c r="T48" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U48" s="1">
         <v>3</v>
@@ -8407,7 +8407,7 @@
       <c r="Y48" s="10"/>
       <c r="AA48" s="10"/>
     </row>
-    <row r="49" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="49" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A49" s="31">
         <v>1045</v>
       </c>
@@ -8463,8 +8463,8 @@
       <c r="S49" s="48">
         <v>281693</v>
       </c>
-      <c r="T49" s="31">
-        <v>1.5</v>
+      <c r="T49" s="1">
+        <v>0.8</v>
       </c>
       <c r="U49" s="31">
         <v>3</v>
@@ -8479,7 +8479,7 @@
       <c r="Y49" s="10"/>
       <c r="AA49" s="10"/>
     </row>
-    <row r="50" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="50" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A50" s="36">
         <v>1046</v>
       </c>
@@ -8536,7 +8536,7 @@
         <v>281693</v>
       </c>
       <c r="T50" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U50" s="1">
         <v>3</v>
@@ -8551,7 +8551,7 @@
       <c r="Y50" s="10"/>
       <c r="AA50" s="10"/>
     </row>
-    <row r="51" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="51" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A51" s="36">
         <v>1047</v>
       </c>
@@ -8608,7 +8608,7 @@
         <v>281693</v>
       </c>
       <c r="T51" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U51" s="1">
         <v>3</v>
@@ -8623,7 +8623,7 @@
       <c r="Y51" s="10"/>
       <c r="AA51" s="10"/>
     </row>
-    <row r="52" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="52" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A52" s="36">
         <v>1048</v>
       </c>
@@ -8680,7 +8680,7 @@
         <v>281693</v>
       </c>
       <c r="T52" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U52" s="1">
         <v>3</v>
@@ -8695,7 +8695,7 @@
       <c r="Y52" s="10"/>
       <c r="AA52" s="10"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="53" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A53" s="31">
         <v>1049</v>
       </c>
@@ -8751,8 +8751,8 @@
       <c r="S53" s="48">
         <v>281693</v>
       </c>
-      <c r="T53" s="31">
-        <v>1.5</v>
+      <c r="T53" s="1">
+        <v>0.8</v>
       </c>
       <c r="U53" s="31">
         <v>3</v>
@@ -8769,7 +8769,7 @@
       <c r="Y53" s="10"/>
       <c r="AA53" s="10"/>
     </row>
-    <row r="54" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="54" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A54" s="31">
         <v>1050</v>
       </c>
@@ -8828,7 +8828,7 @@
         <v>281693</v>
       </c>
       <c r="T54" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U54" s="1">
         <v>3</v>
@@ -8843,7 +8843,7 @@
       <c r="Y54" s="10"/>
       <c r="AA54" s="10"/>
     </row>
-    <row r="55" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="55" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A55" s="36">
         <v>1051</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>281693</v>
       </c>
       <c r="T55" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U55" s="1">
         <v>3</v>
@@ -8915,7 +8915,7 @@
       <c r="Y55" s="10"/>
       <c r="AA55" s="10"/>
     </row>
-    <row r="56" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="56" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A56" s="36">
         <v>1052</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>281693</v>
       </c>
       <c r="T56" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U56" s="1">
         <v>3</v>
@@ -8987,7 +8987,7 @@
       <c r="Y56" s="10"/>
       <c r="AA56" s="10"/>
     </row>
-    <row r="57" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="57" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A57" s="31">
         <v>1053</v>
       </c>
@@ -9044,7 +9044,7 @@
         <v>281693</v>
       </c>
       <c r="T57" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U57" s="1">
         <v>3</v>
@@ -9059,7 +9059,7 @@
       <c r="Y57" s="10"/>
       <c r="AA57" s="10"/>
     </row>
-    <row r="58" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="58" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A58" s="36">
         <v>1054</v>
       </c>
@@ -9116,7 +9116,7 @@
         <v>281693</v>
       </c>
       <c r="T58" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U58" s="1">
         <v>3</v>
@@ -9131,7 +9131,7 @@
       <c r="Y58" s="10"/>
       <c r="AA58" s="10"/>
     </row>
-    <row r="59" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="59" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A59" s="36">
         <v>1055</v>
       </c>
@@ -9188,7 +9188,7 @@
         <v>281693</v>
       </c>
       <c r="T59" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U59" s="1">
         <v>3</v>
@@ -9203,7 +9203,7 @@
       <c r="Y59" s="10"/>
       <c r="AA59" s="10"/>
     </row>
-    <row r="60" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="60" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A60" s="36">
         <v>1056</v>
       </c>
@@ -9260,7 +9260,7 @@
         <v>281693</v>
       </c>
       <c r="T60" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U60" s="1">
         <v>3</v>
@@ -9275,7 +9275,7 @@
       <c r="Y60" s="10"/>
       <c r="AA60" s="10"/>
     </row>
-    <row r="61" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="61" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A61" s="36">
         <v>1057</v>
       </c>
@@ -9332,7 +9332,7 @@
         <v>281693</v>
       </c>
       <c r="T61" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U61" s="1">
         <v>3</v>
@@ -9347,7 +9347,7 @@
       <c r="Y61" s="10"/>
       <c r="AA61" s="10"/>
     </row>
-    <row r="62" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="62" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A62" s="31">
         <v>1058</v>
       </c>
@@ -9404,7 +9404,7 @@
         <v>285139</v>
       </c>
       <c r="T62" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U62" s="1">
         <v>3</v>
@@ -9419,11 +9419,10 @@
       <c r="Y62" s="10"/>
       <c r="AA62" s="10"/>
     </row>
-    <row r="63" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="63" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A63" s="36">
         <v>1059</v>
       </c>
-      <c r="B63" s="1"/>
       <c r="C63" s="11" t="s">
         <v>170</v>
       </c>
@@ -9476,7 +9475,7 @@
         <v>281693</v>
       </c>
       <c r="T63" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U63" s="1">
         <v>3</v>
@@ -9493,7 +9492,7 @@
       <c r="Y63" s="10"/>
       <c r="AA63" s="10"/>
     </row>
-    <row r="64" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="64" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A64" s="41">
         <v>1060</v>
       </c>
@@ -9549,7 +9548,7 @@
         <v>281693</v>
       </c>
       <c r="T64" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U64" s="1">
         <v>3</v>
@@ -9564,7 +9563,7 @@
       <c r="Y64" s="10"/>
       <c r="AA64" s="10"/>
     </row>
-    <row r="65" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="65" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A65" s="1">
         <v>1061</v>
       </c>
@@ -9620,7 +9619,7 @@
         <v>281693</v>
       </c>
       <c r="T65" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U65" s="1">
         <v>3</v>
@@ -9635,7 +9634,7 @@
       <c r="Y65" s="10"/>
       <c r="AA65" s="10"/>
     </row>
-    <row r="66" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="66" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A66" s="36">
         <v>1062</v>
       </c>
@@ -9691,7 +9690,7 @@
         <v>281693</v>
       </c>
       <c r="T66" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U66" s="1">
         <v>3</v>
@@ -9708,7 +9707,7 @@
       <c r="Y66" s="10"/>
       <c r="AA66" s="10"/>
     </row>
-    <row r="67" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="67" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A67" s="36">
         <v>1063</v>
       </c>
@@ -9764,7 +9763,7 @@
         <v>281693</v>
       </c>
       <c r="T67" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U67" s="1">
         <v>3</v>
@@ -9779,7 +9778,7 @@
       <c r="Y67" s="10"/>
       <c r="AA67" s="10"/>
     </row>
-    <row r="68" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="68" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A68" s="1">
         <v>1064</v>
       </c>
@@ -9835,7 +9834,7 @@
         <v>281693</v>
       </c>
       <c r="T68" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U68" s="1">
         <v>3</v>
@@ -9850,7 +9849,7 @@
       <c r="Y68" s="10"/>
       <c r="AA68" s="10"/>
     </row>
-    <row r="69" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="69" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A69" s="1">
         <v>1065</v>
       </c>
@@ -9906,7 +9905,7 @@
         <v>281693</v>
       </c>
       <c r="T69" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U69" s="1">
         <v>3</v>
@@ -9921,7 +9920,7 @@
       <c r="Y69" s="10"/>
       <c r="AA69" s="10"/>
     </row>
-    <row r="70" s="1" customFormat="1" ht="16.35" spans="1:27">
+    <row r="70" s="1" customFormat="1" ht="17.25" spans="1:27">
       <c r="A70" s="1">
         <v>1066</v>
       </c>
@@ -9979,8 +9978,8 @@
       <c r="S70" s="48">
         <v>281693</v>
       </c>
-      <c r="T70" s="31">
-        <v>1.5</v>
+      <c r="T70" s="1">
+        <v>0.8</v>
       </c>
       <c r="U70" s="31">
         <v>3</v>

</xml_diff>

<commit_message>
Revert "feat: update config"
This reverts commit 80653133351b9e0659da116a6c54cd4f932e6cce.
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Monster_怪物表.xlsx
+++ b/nevergiveup/Excel/Monster_怪物表.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PGE\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE26AF91-0FA2-4AE2-B59B-D492D931ADC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C8BADE-D191-4CE7-99C2-CAC6321AC8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37284" yWindow="2352" windowWidth="23040" windowHeight="12120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -402,6 +400,9 @@
     <t>Monster_name_33</t>
   </si>
   <si>
+    <t>青年地精</t>
+  </si>
+  <si>
     <t>Monster_name_34</t>
   </si>
   <si>
@@ -453,6 +454,9 @@
     <t>Monster_name_42</t>
   </si>
   <si>
+    <t>三头犬</t>
+  </si>
+  <si>
     <t>Monster_name_43</t>
   </si>
   <si>
@@ -589,19 +593,13 @@
   </si>
   <si>
     <t>太阳神</t>
-  </si>
-  <si>
-    <t>女天使</t>
-  </si>
-  <si>
-    <t>外星人</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -611,6 +609,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -618,29 +617,40 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -889,7 +899,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -1298,39 +1308,39 @@
   <dimension ref="A1:AMJ373"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.19921875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="5.8984375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="17.8984375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="7.25" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.875" style="4" customWidth="1"/>
     <col min="4" max="4" width="10" style="4" customWidth="1"/>
-    <col min="5" max="5" width="8.796875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8.75" style="4" customWidth="1"/>
     <col min="6" max="7" width="10" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="11.375" style="5" customWidth="1"/>
     <col min="9" max="10" width="7.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="12.59765625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="7.59765625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="12.625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="7.625" style="4" customWidth="1"/>
     <col min="13" max="13" width="13.5" style="5" customWidth="1"/>
-    <col min="14" max="14" width="11.59765625" customWidth="1"/>
-    <col min="15" max="15" width="9.69921875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.625" customWidth="1"/>
+    <col min="15" max="15" width="9.75" style="4" customWidth="1"/>
     <col min="16" max="16" width="21" style="4" customWidth="1"/>
     <col min="17" max="17" width="9.5" style="4" customWidth="1"/>
-    <col min="18" max="18" width="17.3984375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="17.375" style="4" customWidth="1"/>
     <col min="19" max="19" width="9.5" style="4" customWidth="1"/>
     <col min="20" max="20" width="12.5" style="4" customWidth="1"/>
-    <col min="21" max="21" width="12.8984375" style="4" customWidth="1"/>
+    <col min="21" max="21" width="12.875" style="4" customWidth="1"/>
     <col min="22" max="22" width="11" style="5"/>
-    <col min="23" max="23" width="15.59765625" style="5" customWidth="1"/>
-    <col min="24" max="24" width="23.09765625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.625" style="5" customWidth="1"/>
+    <col min="24" max="24" width="23.125" style="4" customWidth="1"/>
     <col min="26" max="26" width="11" style="4"/>
     <col min="28" max="1024" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="26.25" customHeight="1">
+    <row r="1" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1420,7 +1430,7 @@
       <c r="AM1" s="6"/>
       <c r="AN1" s="6"/>
     </row>
-    <row r="2" spans="1:1024" ht="24.75" customHeight="1">
+    <row r="2" spans="1:1024" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1510,7 +1520,7 @@
       <c r="AM2" s="6"/>
       <c r="AN2" s="6"/>
     </row>
-    <row r="3" spans="1:1024" ht="95.25" customHeight="1">
+    <row r="3" spans="1:1024" ht="95.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
@@ -1600,7 +1610,7 @@
       <c r="AM3" s="6"/>
       <c r="AN3" s="6"/>
     </row>
-    <row r="4" spans="1:1024" s="1" customFormat="1">
+    <row r="4" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C4" s="1" t="s">
         <v>53</v>
       </c>
@@ -1614,7 +1624,7 @@
       <c r="Y4" s="9"/>
       <c r="AA4" s="9"/>
     </row>
-    <row r="5" spans="1:1024" s="1" customFormat="1" ht="16.2">
+    <row r="5" spans="1:1024" s="1" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>1001</v>
       </c>
@@ -1670,7 +1680,7 @@
         <v>285139</v>
       </c>
       <c r="T5" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U5" s="1">
         <v>3</v>
@@ -1690,7 +1700,7 @@
       <c r="AD5" s="44"/>
       <c r="AG5" s="44"/>
     </row>
-    <row r="6" spans="1:1024" s="1" customFormat="1" ht="16.2">
+    <row r="6" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>1002</v>
       </c>
@@ -1749,7 +1759,7 @@
         <v>285139</v>
       </c>
       <c r="T6" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U6" s="1">
         <v>3</v>
@@ -1764,7 +1774,7 @@
       <c r="Y6" s="43"/>
       <c r="AA6" s="43"/>
     </row>
-    <row r="7" spans="1:1024" s="1" customFormat="1" ht="16.2">
+    <row r="7" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>1003</v>
       </c>
@@ -1823,7 +1833,7 @@
         <v>20291</v>
       </c>
       <c r="T7" s="1">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="U7" s="1">
         <v>3</v>
@@ -1841,7 +1851,7 @@
       <c r="AD7" s="44"/>
       <c r="AG7" s="44"/>
     </row>
-    <row r="8" spans="1:1024" s="1" customFormat="1" ht="16.2">
+    <row r="8" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>1004</v>
       </c>
@@ -1900,7 +1910,7 @@
         <v>285395</v>
       </c>
       <c r="T8" s="1">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="U8" s="1">
         <v>3</v>
@@ -1915,7 +1925,7 @@
       <c r="Y8" s="43"/>
       <c r="AA8" s="43"/>
     </row>
-    <row r="9" spans="1:1024" s="1" customFormat="1" ht="16.2">
+    <row r="9" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>1005</v>
       </c>
@@ -1974,7 +1984,7 @@
         <v>285139</v>
       </c>
       <c r="T9" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U9" s="1">
         <v>3</v>
@@ -1989,7 +1999,7 @@
       <c r="Y9" s="43"/>
       <c r="AA9" s="43"/>
     </row>
-    <row r="10" spans="1:1024" s="1" customFormat="1" ht="16.2">
+    <row r="10" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>1006</v>
       </c>
@@ -2048,7 +2058,7 @@
         <v>285139</v>
       </c>
       <c r="T10" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U10" s="1">
         <v>3</v>
@@ -2063,7 +2073,7 @@
       <c r="Y10" s="43"/>
       <c r="AA10" s="43"/>
     </row>
-    <row r="11" spans="1:1024">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1007</v>
       </c>
@@ -2120,7 +2130,7 @@
         <v>281693</v>
       </c>
       <c r="T11" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U11" s="1">
         <v>3</v>
@@ -2133,7 +2143,7 @@
       </c>
       <c r="X11" s="36"/>
     </row>
-    <row r="12" spans="1:1024" s="2" customFormat="1">
+    <row r="12" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <v>1008</v>
       </c>
@@ -2154,7 +2164,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I12" s="37">
         <v>500</v>
@@ -2189,8 +2199,8 @@
       <c r="S12" s="17">
         <v>281693</v>
       </c>
-      <c r="T12" s="16">
-        <v>1.5</v>
+      <c r="T12" s="1">
+        <v>0.8</v>
       </c>
       <c r="U12" s="16">
         <v>3</v>
@@ -3201,7 +3211,7 @@
       <c r="AMI12" s="17"/>
       <c r="AMJ12" s="17"/>
     </row>
-    <row r="13" spans="1:1024">
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1009</v>
       </c>
@@ -3257,7 +3267,7 @@
         <v>281693</v>
       </c>
       <c r="T13" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U13" s="1">
         <v>3</v>
@@ -3270,7 +3280,7 @@
       </c>
       <c r="X13" s="36"/>
     </row>
-    <row r="14" spans="1:1024" s="3" customFormat="1" ht="20.25" customHeight="1">
+    <row r="14" spans="1:1024" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23">
         <v>1010</v>
       </c>
@@ -3329,7 +3339,7 @@
         <v>281693</v>
       </c>
       <c r="T14" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U14" s="1">
         <v>3</v>
@@ -4340,7 +4350,7 @@
       <c r="AMI14" s="24"/>
       <c r="AMJ14" s="24"/>
     </row>
-    <row r="15" spans="1:1024" s="1" customFormat="1" ht="16.2">
+    <row r="15" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1011</v>
       </c>
@@ -4360,7 +4370,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I15" s="5">
         <v>700</v>
@@ -4396,7 +4406,7 @@
         <v>281693</v>
       </c>
       <c r="T15" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U15" s="1">
         <v>3</v>
@@ -4411,7 +4421,7 @@
       <c r="Y15" s="43"/>
       <c r="AA15" s="43"/>
     </row>
-    <row r="16" spans="1:1024" s="1" customFormat="1" ht="16.2">
+    <row r="16" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1012</v>
       </c>
@@ -4468,7 +4478,7 @@
         <v>281693</v>
       </c>
       <c r="T16" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U16" s="1">
         <v>3</v>
@@ -4486,7 +4496,7 @@
       <c r="AD16" s="44"/>
       <c r="AG16" s="44"/>
     </row>
-    <row r="17" spans="1:27" s="1" customFormat="1" ht="16.2">
+    <row r="17" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>1013</v>
       </c>
@@ -4542,7 +4552,7 @@
         <v>281693</v>
       </c>
       <c r="T17" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U17" s="1">
         <v>3</v>
@@ -4557,7 +4567,7 @@
       <c r="Y17" s="43"/>
       <c r="AA17" s="43"/>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>1014</v>
       </c>
@@ -4613,7 +4623,7 @@
         <v>281693</v>
       </c>
       <c r="T18" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U18" s="1">
         <v>3</v>
@@ -4628,7 +4638,7 @@
         <v>5001</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1015</v>
       </c>
@@ -4684,7 +4694,7 @@
         <v>281693</v>
       </c>
       <c r="T19" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U19" s="1">
         <v>3</v>
@@ -4697,7 +4707,7 @@
       </c>
       <c r="X19" s="36"/>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1016</v>
       </c>
@@ -4753,7 +4763,7 @@
         <v>281693</v>
       </c>
       <c r="T20" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U20" s="1">
         <v>3</v>
@@ -4766,7 +4776,7 @@
       </c>
       <c r="X20" s="36"/>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1017</v>
       </c>
@@ -4822,7 +4832,7 @@
         <v>281693</v>
       </c>
       <c r="T21" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U21" s="1">
         <v>3</v>
@@ -4835,7 +4845,7 @@
       </c>
       <c r="X21" s="36"/>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>1018</v>
       </c>
@@ -4891,7 +4901,7 @@
         <v>281693</v>
       </c>
       <c r="T22" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U22" s="1">
         <v>3</v>
@@ -4904,7 +4914,7 @@
       </c>
       <c r="X22" s="36"/>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>1019</v>
       </c>
@@ -4924,7 +4934,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="5">
-        <v>268725</v>
+        <v>268562</v>
       </c>
       <c r="I23" s="5">
         <v>2000</v>
@@ -4960,7 +4970,7 @@
         <v>281693</v>
       </c>
       <c r="T23" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U23" s="1">
         <v>3</v>
@@ -4975,7 +4985,7 @@
         <v>5002</v>
       </c>
     </row>
-    <row r="24" spans="1:27" s="1" customFormat="1">
+    <row r="24" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>1020</v>
       </c>
@@ -5031,7 +5041,7 @@
         <v>281693</v>
       </c>
       <c r="T24" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U24" s="1">
         <v>3</v>
@@ -5046,7 +5056,7 @@
       <c r="Y24" s="9"/>
       <c r="AA24" s="9"/>
     </row>
-    <row r="25" spans="1:27" s="1" customFormat="1">
+    <row r="25" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>1021</v>
       </c>
@@ -5102,7 +5112,7 @@
         <v>281693</v>
       </c>
       <c r="T25" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U25" s="1">
         <v>3</v>
@@ -5117,7 +5127,7 @@
       <c r="Y25" s="9"/>
       <c r="AA25" s="9"/>
     </row>
-    <row r="26" spans="1:27" s="1" customFormat="1">
+    <row r="26" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>1022</v>
       </c>
@@ -5173,7 +5183,7 @@
         <v>281693</v>
       </c>
       <c r="T26" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U26" s="1">
         <v>3</v>
@@ -5188,7 +5198,7 @@
       <c r="Y26" s="9"/>
       <c r="AA26" s="9"/>
     </row>
-    <row r="27" spans="1:27" s="1" customFormat="1">
+    <row r="27" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>1023</v>
       </c>
@@ -5244,7 +5254,7 @@
         <v>281693</v>
       </c>
       <c r="T27" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U27" s="1">
         <v>3</v>
@@ -5261,7 +5271,7 @@
       <c r="Y27" s="9"/>
       <c r="AA27" s="9"/>
     </row>
-    <row r="28" spans="1:27" s="1" customFormat="1">
+    <row r="28" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>1024</v>
       </c>
@@ -5317,7 +5327,7 @@
         <v>281693</v>
       </c>
       <c r="T28" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U28" s="1">
         <v>3</v>
@@ -5332,7 +5342,7 @@
       <c r="Y28" s="9"/>
       <c r="AA28" s="9"/>
     </row>
-    <row r="29" spans="1:27" s="1" customFormat="1">
+    <row r="29" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>1025</v>
       </c>
@@ -5352,7 +5362,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I29" s="5">
         <v>500</v>
@@ -5388,7 +5398,7 @@
         <v>281693</v>
       </c>
       <c r="T29" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U29" s="1">
         <v>3</v>
@@ -5403,7 +5413,7 @@
       <c r="Y29" s="9"/>
       <c r="AA29" s="9"/>
     </row>
-    <row r="30" spans="1:27" s="1" customFormat="1">
+    <row r="30" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>1026</v>
       </c>
@@ -5423,7 +5433,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I30" s="5">
         <v>2000</v>
@@ -5459,7 +5469,7 @@
         <v>281693</v>
       </c>
       <c r="T30" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U30" s="1">
         <v>3</v>
@@ -5474,7 +5484,7 @@
       <c r="Y30" s="9"/>
       <c r="AA30" s="9"/>
     </row>
-    <row r="31" spans="1:27" s="1" customFormat="1">
+    <row r="31" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>1027</v>
       </c>
@@ -5494,7 +5504,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I31" s="40">
         <v>300</v>
@@ -5530,7 +5540,7 @@
         <v>281693</v>
       </c>
       <c r="T31" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U31" s="1">
         <v>3</v>
@@ -5545,7 +5555,7 @@
       <c r="Y31" s="9"/>
       <c r="AA31" s="9"/>
     </row>
-    <row r="32" spans="1:27" s="1" customFormat="1">
+    <row r="32" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>1028</v>
       </c>
@@ -5565,7 +5575,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I32" s="40">
         <v>500</v>
@@ -5601,7 +5611,7 @@
         <v>281693</v>
       </c>
       <c r="T32" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U32" s="1">
         <v>3</v>
@@ -5616,7 +5626,7 @@
       <c r="Y32" s="9"/>
       <c r="AA32" s="9"/>
     </row>
-    <row r="33" spans="1:1024" s="1" customFormat="1">
+    <row r="33" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>1029</v>
       </c>
@@ -5636,7 +5646,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I33" s="5">
         <v>1200</v>
@@ -5672,7 +5682,7 @@
         <v>281693</v>
       </c>
       <c r="T33" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U33" s="1">
         <v>3</v>
@@ -5687,7 +5697,7 @@
       <c r="Y33" s="9"/>
       <c r="AA33" s="9"/>
     </row>
-    <row r="34" spans="1:1024" s="1" customFormat="1">
+    <row r="34" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>1030</v>
       </c>
@@ -5707,7 +5717,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I34" s="5">
         <v>500</v>
@@ -5743,7 +5753,7 @@
         <v>281693</v>
       </c>
       <c r="T34" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U34" s="1">
         <v>3</v>
@@ -5758,7 +5768,7 @@
       <c r="Y34" s="9"/>
       <c r="AA34" s="9"/>
     </row>
-    <row r="35" spans="1:1024" s="1" customFormat="1">
+    <row r="35" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>1031</v>
       </c>
@@ -5778,7 +5788,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I35" s="5">
         <v>1200</v>
@@ -5814,7 +5824,7 @@
         <v>281693</v>
       </c>
       <c r="T35" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U35" s="1">
         <v>3</v>
@@ -5829,7 +5839,7 @@
       <c r="Y35" s="9"/>
       <c r="AA35" s="9"/>
     </row>
-    <row r="36" spans="1:1024" s="1" customFormat="1">
+    <row r="36" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>1032</v>
       </c>
@@ -5849,7 +5859,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I36" s="5">
         <v>2000</v>
@@ -5885,7 +5895,7 @@
         <v>281693</v>
       </c>
       <c r="T36" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U36" s="1">
         <v>3</v>
@@ -5902,7 +5912,7 @@
       <c r="Y36" s="9"/>
       <c r="AA36" s="9"/>
     </row>
-    <row r="37" spans="1:1024" s="1" customFormat="1">
+    <row r="37" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>1033</v>
       </c>
@@ -5922,7 +5932,7 @@
         <v>2</v>
       </c>
       <c r="H37" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I37" s="5">
         <v>600</v>
@@ -5958,7 +5968,7 @@
         <v>281693</v>
       </c>
       <c r="T37" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U37" s="1">
         <v>3</v>
@@ -5973,7 +5983,7 @@
       <c r="Y37" s="9"/>
       <c r="AA37" s="9"/>
     </row>
-    <row r="38" spans="1:1024" s="1" customFormat="1">
+    <row r="38" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>1034</v>
       </c>
@@ -5981,19 +5991,19 @@
         <v>120</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>185</v>
+        <v>121</v>
       </c>
       <c r="E38" s="1">
         <v>6</v>
       </c>
       <c r="F38" s="12">
-        <v>142880</v>
+        <v>142300</v>
       </c>
       <c r="G38" s="12">
         <v>2</v>
       </c>
       <c r="H38" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I38" s="5">
         <v>700</v>
@@ -6029,7 +6039,7 @@
         <v>281693</v>
       </c>
       <c r="T38" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U38" s="1">
         <v>3</v>
@@ -6044,15 +6054,15 @@
       <c r="Y38" s="9"/>
       <c r="AA38" s="9"/>
     </row>
-    <row r="39" spans="1:1024" s="1" customFormat="1">
+    <row r="39" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>1035</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -6064,7 +6074,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I39" s="5">
         <v>400</v>
@@ -6100,7 +6110,7 @@
         <v>281693</v>
       </c>
       <c r="T39" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U39" s="1">
         <v>3</v>
@@ -6115,15 +6125,15 @@
       <c r="Y39" s="9"/>
       <c r="AA39" s="9"/>
     </row>
-    <row r="40" spans="1:1024" s="1" customFormat="1">
+    <row r="40" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>1036</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -6135,7 +6145,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I40" s="5">
         <v>2000</v>
@@ -6171,7 +6181,7 @@
         <v>281693</v>
       </c>
       <c r="T40" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U40" s="1">
         <v>3</v>
@@ -6186,15 +6196,15 @@
       <c r="Y40" s="9"/>
       <c r="AA40" s="9"/>
     </row>
-    <row r="41" spans="1:1024" s="1" customFormat="1">
+    <row r="41" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>1037</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -6206,7 +6216,7 @@
         <v>2</v>
       </c>
       <c r="H41" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I41" s="5">
         <v>1200</v>
@@ -6242,7 +6252,7 @@
         <v>281693</v>
       </c>
       <c r="T41" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U41" s="1">
         <v>3</v>
@@ -6257,15 +6267,15 @@
       <c r="Y41" s="9"/>
       <c r="AA41" s="9"/>
     </row>
-    <row r="42" spans="1:1024" s="1" customFormat="1">
+    <row r="42" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>1038</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -6277,7 +6287,7 @@
         <v>2</v>
       </c>
       <c r="H42" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I42" s="5">
         <v>700</v>
@@ -6313,7 +6323,7 @@
         <v>281693</v>
       </c>
       <c r="T42" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U42" s="1">
         <v>3</v>
@@ -6328,7 +6338,7 @@
       <c r="Y42" s="9"/>
       <c r="AA42" s="9"/>
     </row>
-    <row r="43" spans="1:1024" s="1" customFormat="1">
+    <row r="43" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>1039</v>
       </c>
@@ -6336,10 +6346,10 @@
         <v>1</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
@@ -6351,7 +6361,7 @@
         <v>2</v>
       </c>
       <c r="H43" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I43" s="5">
         <v>500</v>
@@ -6387,7 +6397,7 @@
         <v>281693</v>
       </c>
       <c r="T43" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U43" s="1">
         <v>3</v>
@@ -6402,7 +6412,7 @@
       <c r="Y43" s="9"/>
       <c r="AA43" s="9"/>
     </row>
-    <row r="44" spans="1:1024">
+    <row r="44" spans="1:1024" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>1040</v>
       </c>
@@ -6410,10 +6420,10 @@
         <v>1</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
@@ -6425,7 +6435,7 @@
         <v>1</v>
       </c>
       <c r="H44" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I44" s="5">
         <v>500</v>
@@ -6461,7 +6471,7 @@
         <v>281693</v>
       </c>
       <c r="T44" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U44" s="1">
         <v>3</v>
@@ -7474,15 +7484,15 @@
       <c r="AMI44" s="1"/>
       <c r="AMJ44" s="1"/>
     </row>
-    <row r="45" spans="1:1024" s="1" customFormat="1">
+    <row r="45" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>1041</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E45" s="1">
         <v>4</v>
@@ -7494,7 +7504,7 @@
         <v>1</v>
       </c>
       <c r="H45" s="32">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I45" s="5">
         <v>2000</v>
@@ -7530,7 +7540,7 @@
         <v>281693</v>
       </c>
       <c r="T45" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U45" s="1">
         <v>3</v>
@@ -7547,15 +7557,15 @@
       <c r="Y45" s="9"/>
       <c r="AA45" s="9"/>
     </row>
-    <row r="46" spans="1:1024" s="1" customFormat="1">
+    <row r="46" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>1042</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E46" s="1">
         <v>5</v>
@@ -7603,7 +7613,7 @@
         <v>281693</v>
       </c>
       <c r="T46" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U46" s="1">
         <v>3</v>
@@ -7617,27 +7627,27 @@
       <c r="Y46" s="9"/>
       <c r="AA46" s="9"/>
     </row>
-    <row r="47" spans="1:1024" s="1" customFormat="1">
+    <row r="47" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="33">
         <v>1043</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>184</v>
+        <v>139</v>
       </c>
       <c r="E47" s="1">
         <v>4</v>
       </c>
       <c r="F47" s="31">
-        <v>137837</v>
+        <v>174697</v>
       </c>
       <c r="G47" s="1">
         <v>1</v>
       </c>
       <c r="H47" s="5">
-        <v>303165</v>
+        <v>150774</v>
       </c>
       <c r="I47" s="5">
         <v>500</v>
@@ -7673,7 +7683,7 @@
         <v>281693</v>
       </c>
       <c r="T47" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U47" s="1">
         <v>3</v>
@@ -7687,15 +7697,15 @@
       <c r="Y47" s="9"/>
       <c r="AA47" s="9"/>
     </row>
-    <row r="48" spans="1:1024" s="1" customFormat="1">
+    <row r="48" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>1044</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E48" s="1">
         <v>4</v>
@@ -7743,7 +7753,7 @@
         <v>281693</v>
       </c>
       <c r="T48" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U48" s="1">
         <v>3</v>
@@ -7757,15 +7767,15 @@
       <c r="Y48" s="9"/>
       <c r="AA48" s="9"/>
     </row>
-    <row r="49" spans="1:27" s="1" customFormat="1">
+    <row r="49" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>1045</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E49" s="1">
         <v>4</v>
@@ -7777,7 +7787,7 @@
         <v>1</v>
       </c>
       <c r="H49" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I49" s="5">
         <v>300</v>
@@ -7813,7 +7823,7 @@
         <v>281693</v>
       </c>
       <c r="T49" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U49" s="1">
         <v>3</v>
@@ -7827,15 +7837,15 @@
       <c r="Y49" s="9"/>
       <c r="AA49" s="9"/>
     </row>
-    <row r="50" spans="1:27" s="1" customFormat="1">
+    <row r="50" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>1046</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E50" s="1">
         <v>3</v>
@@ -7847,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="H50" s="5">
-        <v>268725</v>
+        <v>268562</v>
       </c>
       <c r="I50" s="5">
         <v>1200</v>
@@ -7883,7 +7893,7 @@
         <v>281693</v>
       </c>
       <c r="T50" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U50" s="1">
         <v>3</v>
@@ -7897,15 +7907,15 @@
       <c r="Y50" s="9"/>
       <c r="AA50" s="9"/>
     </row>
-    <row r="51" spans="1:27" s="1" customFormat="1">
+    <row r="51" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>1047</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E51" s="1">
         <v>6</v>
@@ -7917,7 +7927,7 @@
         <v>2</v>
       </c>
       <c r="H51" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I51" s="5">
         <v>600</v>
@@ -7953,7 +7963,7 @@
         <v>281693</v>
       </c>
       <c r="T51" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U51" s="1">
         <v>3</v>
@@ -7967,15 +7977,15 @@
       <c r="Y51" s="9"/>
       <c r="AA51" s="9"/>
     </row>
-    <row r="52" spans="1:27" s="1" customFormat="1">
+    <row r="52" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>1048</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E52" s="1">
         <v>6</v>
@@ -7987,7 +7997,7 @@
         <v>1</v>
       </c>
       <c r="H52" s="5">
-        <v>268725</v>
+        <v>268562</v>
       </c>
       <c r="I52" s="5">
         <v>500</v>
@@ -8023,7 +8033,7 @@
         <v>281693</v>
       </c>
       <c r="T52" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U52" s="1">
         <v>3</v>
@@ -8037,15 +8047,15 @@
       <c r="Y52" s="9"/>
       <c r="AA52" s="9"/>
     </row>
-    <row r="53" spans="1:27" s="1" customFormat="1">
+    <row r="53" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>1049</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E53" s="1">
         <v>2</v>
@@ -8093,7 +8103,7 @@
         <v>281693</v>
       </c>
       <c r="T53" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U53" s="1">
         <v>3</v>
@@ -8110,7 +8120,7 @@
       <c r="Y53" s="9"/>
       <c r="AA53" s="9"/>
     </row>
-    <row r="54" spans="1:27" s="1" customFormat="1">
+    <row r="54" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>1050</v>
       </c>
@@ -8118,10 +8128,10 @@
         <v>2</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E54" s="1">
         <v>2</v>
@@ -8169,7 +8179,7 @@
         <v>281693</v>
       </c>
       <c r="T54" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U54" s="1">
         <v>3</v>
@@ -8183,15 +8193,15 @@
       <c r="Y54" s="9"/>
       <c r="AA54" s="9"/>
     </row>
-    <row r="55" spans="1:27" s="1" customFormat="1">
+    <row r="55" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>1051</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E55" s="1">
         <v>5</v>
@@ -8203,7 +8213,7 @@
         <v>2</v>
       </c>
       <c r="H55" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I55" s="5">
         <v>500</v>
@@ -8239,7 +8249,7 @@
         <v>281693</v>
       </c>
       <c r="T55" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U55" s="1">
         <v>3</v>
@@ -8253,15 +8263,15 @@
       <c r="Y55" s="9"/>
       <c r="AA55" s="9"/>
     </row>
-    <row r="56" spans="1:27" s="1" customFormat="1">
+    <row r="56" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>1052</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E56" s="1">
         <v>2</v>
@@ -8309,7 +8319,7 @@
         <v>281693</v>
       </c>
       <c r="T56" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U56" s="1">
         <v>3</v>
@@ -8323,15 +8333,15 @@
       <c r="Y56" s="9"/>
       <c r="AA56" s="9"/>
     </row>
-    <row r="57" spans="1:27" s="1" customFormat="1">
+    <row r="57" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>1053</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E57" s="1">
         <v>1</v>
@@ -8343,7 +8353,7 @@
         <v>2</v>
       </c>
       <c r="H57" s="5">
-        <v>268725</v>
+        <v>268562</v>
       </c>
       <c r="I57" s="5">
         <v>300</v>
@@ -8379,7 +8389,7 @@
         <v>281693</v>
       </c>
       <c r="T57" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U57" s="1">
         <v>3</v>
@@ -8393,15 +8403,15 @@
       <c r="Y57" s="9"/>
       <c r="AA57" s="9"/>
     </row>
-    <row r="58" spans="1:27" s="1" customFormat="1">
+    <row r="58" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>1054</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E58" s="1">
         <v>6</v>
@@ -8449,7 +8459,7 @@
         <v>281693</v>
       </c>
       <c r="T58" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U58" s="1">
         <v>3</v>
@@ -8463,15 +8473,15 @@
       <c r="Y58" s="9"/>
       <c r="AA58" s="9"/>
     </row>
-    <row r="59" spans="1:27" s="1" customFormat="1">
+    <row r="59" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>1055</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D59" s="31" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E59" s="1">
         <v>3</v>
@@ -8483,7 +8493,7 @@
         <v>2</v>
       </c>
       <c r="H59" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I59" s="5">
         <v>500</v>
@@ -8519,7 +8529,7 @@
         <v>281693</v>
       </c>
       <c r="T59" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U59" s="1">
         <v>3</v>
@@ -8533,15 +8543,15 @@
       <c r="Y59" s="9"/>
       <c r="AA59" s="9"/>
     </row>
-    <row r="60" spans="1:27" s="1" customFormat="1">
+    <row r="60" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>1056</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D60" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E60" s="1">
         <v>2</v>
@@ -8589,7 +8599,7 @@
         <v>281693</v>
       </c>
       <c r="T60" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U60" s="1">
         <v>3</v>
@@ -8603,15 +8613,15 @@
       <c r="Y60" s="9"/>
       <c r="AA60" s="9"/>
     </row>
-    <row r="61" spans="1:27" s="1" customFormat="1">
+    <row r="61" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>1057</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E61" s="1">
         <v>1</v>
@@ -8623,7 +8633,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I61" s="5">
         <v>500</v>
@@ -8659,7 +8669,7 @@
         <v>281693</v>
       </c>
       <c r="T61" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U61" s="1">
         <v>3</v>
@@ -8673,15 +8683,15 @@
       <c r="Y61" s="9"/>
       <c r="AA61" s="9"/>
     </row>
-    <row r="62" spans="1:27" s="1" customFormat="1">
+    <row r="62" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>1058</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E62" s="1">
         <v>5</v>
@@ -8708,7 +8718,7 @@
         <v>1</v>
       </c>
       <c r="M62" s="5">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="N62" s="1">
         <v>500</v>
@@ -8729,7 +8739,7 @@
         <v>285139</v>
       </c>
       <c r="T62" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U62" s="1">
         <v>3</v>
@@ -8743,15 +8753,15 @@
       <c r="Y62" s="9"/>
       <c r="AA62" s="9"/>
     </row>
-    <row r="63" spans="1:27" s="1" customFormat="1">
+    <row r="63" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>1059</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -8799,7 +8809,7 @@
         <v>281693</v>
       </c>
       <c r="T63" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U63" s="1">
         <v>3</v>
@@ -8816,15 +8826,15 @@
       <c r="Y63" s="9"/>
       <c r="AA63" s="9"/>
     </row>
-    <row r="64" spans="1:27" s="1" customFormat="1">
+    <row r="64" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="34">
         <v>1060</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E64" s="1">
         <v>6</v>
@@ -8836,7 +8846,7 @@
         <v>1</v>
       </c>
       <c r="H64" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I64" s="5">
         <v>600</v>
@@ -8872,7 +8882,7 @@
         <v>281693</v>
       </c>
       <c r="T64" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U64" s="1">
         <v>3</v>
@@ -8886,15 +8896,15 @@
       <c r="Y64" s="9"/>
       <c r="AA64" s="9"/>
     </row>
-    <row r="65" spans="1:27" s="1" customFormat="1">
+    <row r="65" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>1061</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D65" s="31" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E65" s="1">
         <v>4</v>
@@ -8906,7 +8916,7 @@
         <v>1</v>
       </c>
       <c r="H65" s="5">
-        <v>303165</v>
+        <v>281015</v>
       </c>
       <c r="I65" s="5">
         <v>400</v>
@@ -8942,7 +8952,7 @@
         <v>281693</v>
       </c>
       <c r="T65" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U65" s="1">
         <v>3</v>
@@ -8956,15 +8966,15 @@
       <c r="Y65" s="9"/>
       <c r="AA65" s="9"/>
     </row>
-    <row r="66" spans="1:27" s="1" customFormat="1">
+    <row r="66" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>1062</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D66" s="45" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E66" s="46">
         <v>3</v>
@@ -9012,7 +9022,7 @@
         <v>281693</v>
       </c>
       <c r="T66" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U66" s="1">
         <v>3</v>
@@ -9029,15 +9039,15 @@
       <c r="Y66" s="9"/>
       <c r="AA66" s="9"/>
     </row>
-    <row r="67" spans="1:27" s="1" customFormat="1">
+    <row r="67" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>1063</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D67" s="45" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E67" s="46">
         <v>4</v>
@@ -9085,7 +9095,7 @@
         <v>281693</v>
       </c>
       <c r="T67" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U67" s="1">
         <v>3</v>
@@ -9099,15 +9109,15 @@
       <c r="Y67" s="9"/>
       <c r="AA67" s="9"/>
     </row>
-    <row r="68" spans="1:27" s="1" customFormat="1">
+    <row r="68" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>1064</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E68" s="1">
         <v>3</v>
@@ -9119,7 +9129,7 @@
         <v>1</v>
       </c>
       <c r="H68" s="5">
-        <v>268725</v>
+        <v>268562</v>
       </c>
       <c r="I68" s="5">
         <v>700</v>
@@ -9155,7 +9165,7 @@
         <v>281693</v>
       </c>
       <c r="T68" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U68" s="1">
         <v>3</v>
@@ -9169,15 +9179,15 @@
       <c r="Y68" s="9"/>
       <c r="AA68" s="9"/>
     </row>
-    <row r="69" spans="1:27" s="1" customFormat="1">
+    <row r="69" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>1065</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E69" s="1">
         <v>5</v>
@@ -9189,7 +9199,7 @@
         <v>1</v>
       </c>
       <c r="H69" s="5">
-        <v>268725</v>
+        <v>268562</v>
       </c>
       <c r="I69" s="5">
         <v>600</v>
@@ -9225,7 +9235,7 @@
         <v>281693</v>
       </c>
       <c r="T69" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U69" s="1">
         <v>3</v>
@@ -9239,7 +9249,7 @@
       <c r="Y69" s="9"/>
       <c r="AA69" s="9"/>
     </row>
-    <row r="70" spans="1:27" s="1" customFormat="1">
+    <row r="70" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>1066</v>
       </c>
@@ -9247,10 +9257,10 @@
         <v>2</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E70" s="1">
         <v>1</v>
@@ -9298,7 +9308,7 @@
         <v>281693</v>
       </c>
       <c r="T70" s="1">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="U70" s="1">
         <v>3</v>
@@ -9312,7 +9322,7 @@
       <c r="Y70" s="9"/>
       <c r="AA70" s="9"/>
     </row>
-    <row r="71" spans="1:27" s="1" customFormat="1">
+    <row r="71" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
@@ -9323,7 +9333,7 @@
       <c r="Y71" s="9"/>
       <c r="AA71" s="9"/>
     </row>
-    <row r="72" spans="1:27" s="1" customFormat="1">
+    <row r="72" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
@@ -9334,7 +9344,7 @@
       <c r="Y72" s="9"/>
       <c r="AA72" s="9"/>
     </row>
-    <row r="73" spans="1:27" s="1" customFormat="1">
+    <row r="73" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
@@ -9345,7 +9355,7 @@
       <c r="Y73" s="9"/>
       <c r="AA73" s="9"/>
     </row>
-    <row r="74" spans="1:27" s="1" customFormat="1">
+    <row r="74" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
@@ -9356,7 +9366,7 @@
       <c r="Y74" s="9"/>
       <c r="AA74" s="9"/>
     </row>
-    <row r="75" spans="1:27" s="1" customFormat="1">
+    <row r="75" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
@@ -9367,7 +9377,7 @@
       <c r="Y75" s="9"/>
       <c r="AA75" s="9"/>
     </row>
-    <row r="76" spans="1:27" s="1" customFormat="1">
+    <row r="76" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
@@ -9378,7 +9388,7 @@
       <c r="Y76" s="9"/>
       <c r="AA76" s="9"/>
     </row>
-    <row r="77" spans="1:27" s="1" customFormat="1">
+    <row r="77" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
@@ -9389,7 +9399,7 @@
       <c r="Y77" s="9"/>
       <c r="AA77" s="9"/>
     </row>
-    <row r="78" spans="1:27" s="1" customFormat="1">
+    <row r="78" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
@@ -9400,7 +9410,7 @@
       <c r="Y78" s="9"/>
       <c r="AA78" s="9"/>
     </row>
-    <row r="79" spans="1:27" s="1" customFormat="1">
+    <row r="79" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="5"/>
@@ -9411,7 +9421,7 @@
       <c r="Y79" s="9"/>
       <c r="AA79" s="9"/>
     </row>
-    <row r="80" spans="1:27" s="1" customFormat="1">
+    <row r="80" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="5"/>
@@ -9422,7 +9432,7 @@
       <c r="Y80" s="9"/>
       <c r="AA80" s="9"/>
     </row>
-    <row r="81" spans="8:27" s="1" customFormat="1">
+    <row r="81" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
@@ -9433,7 +9443,7 @@
       <c r="Y81" s="9"/>
       <c r="AA81" s="9"/>
     </row>
-    <row r="82" spans="8:27" s="1" customFormat="1">
+    <row r="82" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
@@ -9444,7 +9454,7 @@
       <c r="Y82" s="9"/>
       <c r="AA82" s="9"/>
     </row>
-    <row r="83" spans="8:27" s="1" customFormat="1">
+    <row r="83" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
@@ -9455,7 +9465,7 @@
       <c r="Y83" s="9"/>
       <c r="AA83" s="9"/>
     </row>
-    <row r="84" spans="8:27" s="1" customFormat="1">
+    <row r="84" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
       <c r="J84" s="5"/>
@@ -9466,7 +9476,7 @@
       <c r="Y84" s="9"/>
       <c r="AA84" s="9"/>
     </row>
-    <row r="85" spans="8:27" s="1" customFormat="1">
+    <row r="85" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
       <c r="J85" s="5"/>
@@ -9477,7 +9487,7 @@
       <c r="Y85" s="9"/>
       <c r="AA85" s="9"/>
     </row>
-    <row r="86" spans="8:27" s="1" customFormat="1">
+    <row r="86" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
       <c r="J86" s="5"/>
@@ -9488,7 +9498,7 @@
       <c r="Y86" s="9"/>
       <c r="AA86" s="9"/>
     </row>
-    <row r="87" spans="8:27" s="1" customFormat="1">
+    <row r="87" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
       <c r="J87" s="5"/>
@@ -9499,7 +9509,7 @@
       <c r="Y87" s="9"/>
       <c r="AA87" s="9"/>
     </row>
-    <row r="88" spans="8:27" s="1" customFormat="1">
+    <row r="88" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
       <c r="J88" s="5"/>
@@ -9510,7 +9520,7 @@
       <c r="Y88" s="9"/>
       <c r="AA88" s="9"/>
     </row>
-    <row r="89" spans="8:27" s="1" customFormat="1">
+    <row r="89" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
       <c r="J89" s="5"/>
@@ -9521,7 +9531,7 @@
       <c r="Y89" s="9"/>
       <c r="AA89" s="9"/>
     </row>
-    <row r="90" spans="8:27" s="1" customFormat="1">
+    <row r="90" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
       <c r="J90" s="5"/>
@@ -9532,7 +9542,7 @@
       <c r="Y90" s="9"/>
       <c r="AA90" s="9"/>
     </row>
-    <row r="91" spans="8:27" s="1" customFormat="1">
+    <row r="91" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
       <c r="J91" s="5"/>
@@ -9543,7 +9553,7 @@
       <c r="Y91" s="9"/>
       <c r="AA91" s="9"/>
     </row>
-    <row r="92" spans="8:27" s="1" customFormat="1">
+    <row r="92" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
       <c r="J92" s="5"/>
@@ -9554,7 +9564,7 @@
       <c r="Y92" s="9"/>
       <c r="AA92" s="9"/>
     </row>
-    <row r="93" spans="8:27" s="1" customFormat="1">
+    <row r="93" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
       <c r="J93" s="5"/>
@@ -9565,7 +9575,7 @@
       <c r="Y93" s="9"/>
       <c r="AA93" s="9"/>
     </row>
-    <row r="94" spans="8:27" s="1" customFormat="1">
+    <row r="94" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
       <c r="J94" s="5"/>
@@ -9576,7 +9586,7 @@
       <c r="Y94" s="9"/>
       <c r="AA94" s="9"/>
     </row>
-    <row r="95" spans="8:27" s="1" customFormat="1">
+    <row r="95" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
       <c r="J95" s="5"/>
@@ -9587,7 +9597,7 @@
       <c r="Y95" s="9"/>
       <c r="AA95" s="9"/>
     </row>
-    <row r="96" spans="8:27" s="1" customFormat="1">
+    <row r="96" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
       <c r="J96" s="5"/>
@@ -9598,7 +9608,7 @@
       <c r="Y96" s="9"/>
       <c r="AA96" s="9"/>
     </row>
-    <row r="97" spans="8:27" s="1" customFormat="1">
+    <row r="97" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
       <c r="J97" s="5"/>
@@ -9609,7 +9619,7 @@
       <c r="Y97" s="9"/>
       <c r="AA97" s="9"/>
     </row>
-    <row r="98" spans="8:27" s="1" customFormat="1">
+    <row r="98" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
       <c r="J98" s="5"/>
@@ -9620,7 +9630,7 @@
       <c r="Y98" s="9"/>
       <c r="AA98" s="9"/>
     </row>
-    <row r="99" spans="8:27" s="1" customFormat="1">
+    <row r="99" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H99" s="5"/>
       <c r="I99" s="5"/>
       <c r="J99" s="5"/>
@@ -9631,7 +9641,7 @@
       <c r="Y99" s="9"/>
       <c r="AA99" s="9"/>
     </row>
-    <row r="100" spans="8:27" s="1" customFormat="1">
+    <row r="100" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H100" s="5"/>
       <c r="I100" s="5"/>
       <c r="J100" s="5"/>
@@ -9642,7 +9652,7 @@
       <c r="Y100" s="9"/>
       <c r="AA100" s="9"/>
     </row>
-    <row r="101" spans="8:27" s="1" customFormat="1">
+    <row r="101" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H101" s="5"/>
       <c r="I101" s="5"/>
       <c r="J101" s="5"/>
@@ -9653,7 +9663,7 @@
       <c r="Y101" s="9"/>
       <c r="AA101" s="9"/>
     </row>
-    <row r="102" spans="8:27" s="1" customFormat="1">
+    <row r="102" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H102" s="5"/>
       <c r="I102" s="5"/>
       <c r="J102" s="5"/>
@@ -9664,7 +9674,7 @@
       <c r="Y102" s="9"/>
       <c r="AA102" s="9"/>
     </row>
-    <row r="103" spans="8:27" s="1" customFormat="1">
+    <row r="103" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H103" s="5"/>
       <c r="I103" s="5"/>
       <c r="J103" s="5"/>
@@ -9675,7 +9685,7 @@
       <c r="Y103" s="9"/>
       <c r="AA103" s="9"/>
     </row>
-    <row r="104" spans="8:27" s="1" customFormat="1">
+    <row r="104" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H104" s="5"/>
       <c r="I104" s="5"/>
       <c r="J104" s="5"/>
@@ -9686,7 +9696,7 @@
       <c r="Y104" s="9"/>
       <c r="AA104" s="9"/>
     </row>
-    <row r="105" spans="8:27" s="1" customFormat="1">
+    <row r="105" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H105" s="5"/>
       <c r="I105" s="5"/>
       <c r="J105" s="5"/>
@@ -9697,7 +9707,7 @@
       <c r="Y105" s="9"/>
       <c r="AA105" s="9"/>
     </row>
-    <row r="106" spans="8:27" s="1" customFormat="1">
+    <row r="106" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
       <c r="J106" s="5"/>
@@ -9708,7 +9718,7 @@
       <c r="Y106" s="9"/>
       <c r="AA106" s="9"/>
     </row>
-    <row r="107" spans="8:27" s="1" customFormat="1">
+    <row r="107" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H107" s="5"/>
       <c r="I107" s="5"/>
       <c r="J107" s="5"/>
@@ -9719,7 +9729,7 @@
       <c r="Y107" s="9"/>
       <c r="AA107" s="9"/>
     </row>
-    <row r="108" spans="8:27" s="1" customFormat="1">
+    <row r="108" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H108" s="5"/>
       <c r="I108" s="5"/>
       <c r="J108" s="5"/>
@@ -9730,7 +9740,7 @@
       <c r="Y108" s="9"/>
       <c r="AA108" s="9"/>
     </row>
-    <row r="109" spans="8:27" s="1" customFormat="1">
+    <row r="109" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H109" s="5"/>
       <c r="I109" s="5"/>
       <c r="J109" s="5"/>
@@ -9741,7 +9751,7 @@
       <c r="Y109" s="9"/>
       <c r="AA109" s="9"/>
     </row>
-    <row r="110" spans="8:27" s="1" customFormat="1">
+    <row r="110" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H110" s="5"/>
       <c r="I110" s="5"/>
       <c r="J110" s="5"/>
@@ -9752,7 +9762,7 @@
       <c r="Y110" s="9"/>
       <c r="AA110" s="9"/>
     </row>
-    <row r="111" spans="8:27" s="1" customFormat="1">
+    <row r="111" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H111" s="5"/>
       <c r="I111" s="5"/>
       <c r="J111" s="5"/>
@@ -9763,7 +9773,7 @@
       <c r="Y111" s="9"/>
       <c r="AA111" s="9"/>
     </row>
-    <row r="112" spans="8:27" s="1" customFormat="1">
+    <row r="112" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H112" s="5"/>
       <c r="I112" s="5"/>
       <c r="J112" s="5"/>
@@ -9774,7 +9784,7 @@
       <c r="Y112" s="9"/>
       <c r="AA112" s="9"/>
     </row>
-    <row r="113" spans="8:27" s="1" customFormat="1">
+    <row r="113" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H113" s="5"/>
       <c r="I113" s="5"/>
       <c r="J113" s="5"/>
@@ -9785,7 +9795,7 @@
       <c r="Y113" s="9"/>
       <c r="AA113" s="9"/>
     </row>
-    <row r="114" spans="8:27" s="1" customFormat="1">
+    <row r="114" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H114" s="5"/>
       <c r="I114" s="5"/>
       <c r="J114" s="5"/>
@@ -9796,7 +9806,7 @@
       <c r="Y114" s="9"/>
       <c r="AA114" s="9"/>
     </row>
-    <row r="115" spans="8:27" s="1" customFormat="1">
+    <row r="115" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H115" s="5"/>
       <c r="I115" s="5"/>
       <c r="J115" s="5"/>
@@ -9807,7 +9817,7 @@
       <c r="Y115" s="9"/>
       <c r="AA115" s="9"/>
     </row>
-    <row r="116" spans="8:27" s="1" customFormat="1">
+    <row r="116" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H116" s="5"/>
       <c r="I116" s="5"/>
       <c r="J116" s="5"/>
@@ -9818,7 +9828,7 @@
       <c r="Y116" s="9"/>
       <c r="AA116" s="9"/>
     </row>
-    <row r="117" spans="8:27" s="1" customFormat="1">
+    <row r="117" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H117" s="5"/>
       <c r="I117" s="5"/>
       <c r="J117" s="5"/>
@@ -9829,7 +9839,7 @@
       <c r="Y117" s="9"/>
       <c r="AA117" s="9"/>
     </row>
-    <row r="118" spans="8:27" s="1" customFormat="1">
+    <row r="118" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H118" s="5"/>
       <c r="I118" s="5"/>
       <c r="J118" s="5"/>
@@ -9840,7 +9850,7 @@
       <c r="Y118" s="9"/>
       <c r="AA118" s="9"/>
     </row>
-    <row r="119" spans="8:27" s="1" customFormat="1">
+    <row r="119" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H119" s="5"/>
       <c r="I119" s="5"/>
       <c r="J119" s="5"/>
@@ -9851,7 +9861,7 @@
       <c r="Y119" s="9"/>
       <c r="AA119" s="9"/>
     </row>
-    <row r="120" spans="8:27" s="1" customFormat="1">
+    <row r="120" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H120" s="5"/>
       <c r="I120" s="5"/>
       <c r="J120" s="5"/>
@@ -9862,7 +9872,7 @@
       <c r="Y120" s="9"/>
       <c r="AA120" s="9"/>
     </row>
-    <row r="121" spans="8:27" s="1" customFormat="1">
+    <row r="121" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H121" s="5"/>
       <c r="I121" s="5"/>
       <c r="J121" s="5"/>
@@ -9873,7 +9883,7 @@
       <c r="Y121" s="9"/>
       <c r="AA121" s="9"/>
     </row>
-    <row r="122" spans="8:27" s="1" customFormat="1">
+    <row r="122" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H122" s="5"/>
       <c r="I122" s="5"/>
       <c r="J122" s="5"/>
@@ -9884,7 +9894,7 @@
       <c r="Y122" s="9"/>
       <c r="AA122" s="9"/>
     </row>
-    <row r="123" spans="8:27" s="1" customFormat="1">
+    <row r="123" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H123" s="5"/>
       <c r="I123" s="5"/>
       <c r="J123" s="5"/>
@@ -9895,7 +9905,7 @@
       <c r="Y123" s="9"/>
       <c r="AA123" s="9"/>
     </row>
-    <row r="124" spans="8:27" s="1" customFormat="1">
+    <row r="124" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H124" s="5"/>
       <c r="I124" s="5"/>
       <c r="J124" s="5"/>
@@ -9906,7 +9916,7 @@
       <c r="Y124" s="9"/>
       <c r="AA124" s="9"/>
     </row>
-    <row r="125" spans="8:27" s="1" customFormat="1">
+    <row r="125" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H125" s="5"/>
       <c r="I125" s="5"/>
       <c r="J125" s="5"/>
@@ -9917,7 +9927,7 @@
       <c r="Y125" s="9"/>
       <c r="AA125" s="9"/>
     </row>
-    <row r="126" spans="8:27" s="1" customFormat="1">
+    <row r="126" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H126" s="5"/>
       <c r="I126" s="5"/>
       <c r="J126" s="5"/>
@@ -9928,7 +9938,7 @@
       <c r="Y126" s="9"/>
       <c r="AA126" s="9"/>
     </row>
-    <row r="127" spans="8:27" s="1" customFormat="1">
+    <row r="127" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H127" s="5"/>
       <c r="I127" s="5"/>
       <c r="J127" s="5"/>
@@ -9939,7 +9949,7 @@
       <c r="Y127" s="9"/>
       <c r="AA127" s="9"/>
     </row>
-    <row r="128" spans="8:27" s="1" customFormat="1">
+    <row r="128" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H128" s="5"/>
       <c r="I128" s="5"/>
       <c r="J128" s="5"/>
@@ -9950,7 +9960,7 @@
       <c r="Y128" s="9"/>
       <c r="AA128" s="9"/>
     </row>
-    <row r="129" spans="8:27" s="1" customFormat="1">
+    <row r="129" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H129" s="5"/>
       <c r="I129" s="5"/>
       <c r="J129" s="5"/>
@@ -9961,7 +9971,7 @@
       <c r="Y129" s="9"/>
       <c r="AA129" s="9"/>
     </row>
-    <row r="130" spans="8:27" s="1" customFormat="1">
+    <row r="130" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H130" s="5"/>
       <c r="I130" s="5"/>
       <c r="J130" s="5"/>
@@ -9972,7 +9982,7 @@
       <c r="Y130" s="9"/>
       <c r="AA130" s="9"/>
     </row>
-    <row r="131" spans="8:27" s="1" customFormat="1">
+    <row r="131" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H131" s="5"/>
       <c r="I131" s="5"/>
       <c r="J131" s="5"/>
@@ -9983,7 +9993,7 @@
       <c r="Y131" s="9"/>
       <c r="AA131" s="9"/>
     </row>
-    <row r="132" spans="8:27" s="1" customFormat="1">
+    <row r="132" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H132" s="5"/>
       <c r="I132" s="5"/>
       <c r="J132" s="5"/>
@@ -9994,7 +10004,7 @@
       <c r="Y132" s="9"/>
       <c r="AA132" s="9"/>
     </row>
-    <row r="133" spans="8:27" s="1" customFormat="1">
+    <row r="133" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H133" s="5"/>
       <c r="I133" s="5"/>
       <c r="J133" s="5"/>
@@ -10005,7 +10015,7 @@
       <c r="Y133" s="9"/>
       <c r="AA133" s="9"/>
     </row>
-    <row r="134" spans="8:27" s="1" customFormat="1">
+    <row r="134" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H134" s="5"/>
       <c r="I134" s="5"/>
       <c r="J134" s="5"/>
@@ -10016,7 +10026,7 @@
       <c r="Y134" s="9"/>
       <c r="AA134" s="9"/>
     </row>
-    <row r="135" spans="8:27" s="1" customFormat="1">
+    <row r="135" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H135" s="5"/>
       <c r="I135" s="5"/>
       <c r="J135" s="5"/>
@@ -10027,7 +10037,7 @@
       <c r="Y135" s="9"/>
       <c r="AA135" s="9"/>
     </row>
-    <row r="136" spans="8:27" s="1" customFormat="1">
+    <row r="136" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H136" s="5"/>
       <c r="I136" s="5"/>
       <c r="J136" s="5"/>
@@ -10038,7 +10048,7 @@
       <c r="Y136" s="9"/>
       <c r="AA136" s="9"/>
     </row>
-    <row r="137" spans="8:27" s="1" customFormat="1">
+    <row r="137" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H137" s="5"/>
       <c r="I137" s="5"/>
       <c r="J137" s="5"/>
@@ -10049,7 +10059,7 @@
       <c r="Y137" s="9"/>
       <c r="AA137" s="9"/>
     </row>
-    <row r="138" spans="8:27" s="1" customFormat="1">
+    <row r="138" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H138" s="5"/>
       <c r="I138" s="5"/>
       <c r="J138" s="5"/>
@@ -10060,7 +10070,7 @@
       <c r="Y138" s="9"/>
       <c r="AA138" s="9"/>
     </row>
-    <row r="139" spans="8:27" s="1" customFormat="1">
+    <row r="139" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H139" s="5"/>
       <c r="I139" s="5"/>
       <c r="J139" s="5"/>
@@ -10071,7 +10081,7 @@
       <c r="Y139" s="9"/>
       <c r="AA139" s="9"/>
     </row>
-    <row r="140" spans="8:27" s="1" customFormat="1">
+    <row r="140" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H140" s="5"/>
       <c r="I140" s="5"/>
       <c r="J140" s="5"/>
@@ -10082,7 +10092,7 @@
       <c r="Y140" s="9"/>
       <c r="AA140" s="9"/>
     </row>
-    <row r="141" spans="8:27" s="1" customFormat="1">
+    <row r="141" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H141" s="5"/>
       <c r="I141" s="5"/>
       <c r="J141" s="5"/>
@@ -10093,7 +10103,7 @@
       <c r="Y141" s="9"/>
       <c r="AA141" s="9"/>
     </row>
-    <row r="142" spans="8:27" s="1" customFormat="1">
+    <row r="142" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H142" s="5"/>
       <c r="I142" s="5"/>
       <c r="J142" s="5"/>
@@ -10104,7 +10114,7 @@
       <c r="Y142" s="9"/>
       <c r="AA142" s="9"/>
     </row>
-    <row r="143" spans="8:27" s="1" customFormat="1">
+    <row r="143" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H143" s="5"/>
       <c r="I143" s="5"/>
       <c r="J143" s="5"/>
@@ -10115,7 +10125,7 @@
       <c r="Y143" s="9"/>
       <c r="AA143" s="9"/>
     </row>
-    <row r="144" spans="8:27" s="1" customFormat="1">
+    <row r="144" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H144" s="5"/>
       <c r="I144" s="5"/>
       <c r="J144" s="5"/>
@@ -10126,7 +10136,7 @@
       <c r="Y144" s="9"/>
       <c r="AA144" s="9"/>
     </row>
-    <row r="145" spans="8:27" s="1" customFormat="1">
+    <row r="145" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H145" s="5"/>
       <c r="I145" s="5"/>
       <c r="J145" s="5"/>
@@ -10137,7 +10147,7 @@
       <c r="Y145" s="9"/>
       <c r="AA145" s="9"/>
     </row>
-    <row r="146" spans="8:27" s="1" customFormat="1">
+    <row r="146" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H146" s="5"/>
       <c r="I146" s="5"/>
       <c r="J146" s="5"/>
@@ -10148,7 +10158,7 @@
       <c r="Y146" s="9"/>
       <c r="AA146" s="9"/>
     </row>
-    <row r="147" spans="8:27" s="1" customFormat="1">
+    <row r="147" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H147" s="5"/>
       <c r="I147" s="5"/>
       <c r="J147" s="5"/>
@@ -10159,7 +10169,7 @@
       <c r="Y147" s="9"/>
       <c r="AA147" s="9"/>
     </row>
-    <row r="148" spans="8:27" s="1" customFormat="1">
+    <row r="148" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H148" s="5"/>
       <c r="I148" s="5"/>
       <c r="J148" s="5"/>
@@ -10170,7 +10180,7 @@
       <c r="Y148" s="9"/>
       <c r="AA148" s="9"/>
     </row>
-    <row r="149" spans="8:27" s="1" customFormat="1">
+    <row r="149" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H149" s="5"/>
       <c r="I149" s="5"/>
       <c r="J149" s="5"/>
@@ -10181,7 +10191,7 @@
       <c r="Y149" s="9"/>
       <c r="AA149" s="9"/>
     </row>
-    <row r="150" spans="8:27" s="1" customFormat="1">
+    <row r="150" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H150" s="5"/>
       <c r="I150" s="5"/>
       <c r="J150" s="5"/>
@@ -10192,7 +10202,7 @@
       <c r="Y150" s="9"/>
       <c r="AA150" s="9"/>
     </row>
-    <row r="151" spans="8:27" s="1" customFormat="1">
+    <row r="151" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H151" s="5"/>
       <c r="I151" s="5"/>
       <c r="J151" s="5"/>
@@ -10203,7 +10213,7 @@
       <c r="Y151" s="9"/>
       <c r="AA151" s="9"/>
     </row>
-    <row r="152" spans="8:27" s="1" customFormat="1">
+    <row r="152" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H152" s="5"/>
       <c r="I152" s="5"/>
       <c r="J152" s="5"/>
@@ -10214,7 +10224,7 @@
       <c r="Y152" s="9"/>
       <c r="AA152" s="9"/>
     </row>
-    <row r="153" spans="8:27" s="1" customFormat="1">
+    <row r="153" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H153" s="5"/>
       <c r="I153" s="5"/>
       <c r="J153" s="5"/>
@@ -10225,7 +10235,7 @@
       <c r="Y153" s="9"/>
       <c r="AA153" s="9"/>
     </row>
-    <row r="154" spans="8:27" s="1" customFormat="1">
+    <row r="154" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H154" s="5"/>
       <c r="I154" s="5"/>
       <c r="J154" s="5"/>
@@ -10236,7 +10246,7 @@
       <c r="Y154" s="9"/>
       <c r="AA154" s="9"/>
     </row>
-    <row r="155" spans="8:27" s="1" customFormat="1">
+    <row r="155" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H155" s="5"/>
       <c r="I155" s="5"/>
       <c r="J155" s="5"/>
@@ -10247,7 +10257,7 @@
       <c r="Y155" s="9"/>
       <c r="AA155" s="9"/>
     </row>
-    <row r="156" spans="8:27" s="1" customFormat="1">
+    <row r="156" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H156" s="5"/>
       <c r="I156" s="5"/>
       <c r="J156" s="5"/>
@@ -10258,7 +10268,7 @@
       <c r="Y156" s="9"/>
       <c r="AA156" s="9"/>
     </row>
-    <row r="157" spans="8:27" s="1" customFormat="1">
+    <row r="157" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H157" s="5"/>
       <c r="I157" s="5"/>
       <c r="J157" s="5"/>
@@ -10269,7 +10279,7 @@
       <c r="Y157" s="9"/>
       <c r="AA157" s="9"/>
     </row>
-    <row r="158" spans="8:27" s="1" customFormat="1">
+    <row r="158" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H158" s="5"/>
       <c r="I158" s="5"/>
       <c r="J158" s="5"/>
@@ -10280,7 +10290,7 @@
       <c r="Y158" s="9"/>
       <c r="AA158" s="9"/>
     </row>
-    <row r="159" spans="8:27" s="1" customFormat="1">
+    <row r="159" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H159" s="5"/>
       <c r="I159" s="5"/>
       <c r="J159" s="5"/>
@@ -10291,7 +10301,7 @@
       <c r="Y159" s="9"/>
       <c r="AA159" s="9"/>
     </row>
-    <row r="160" spans="8:27" s="1" customFormat="1">
+    <row r="160" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H160" s="5"/>
       <c r="I160" s="5"/>
       <c r="J160" s="5"/>
@@ -10302,7 +10312,7 @@
       <c r="Y160" s="9"/>
       <c r="AA160" s="9"/>
     </row>
-    <row r="161" spans="8:27" s="1" customFormat="1">
+    <row r="161" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H161" s="5"/>
       <c r="I161" s="5"/>
       <c r="J161" s="5"/>
@@ -10313,7 +10323,7 @@
       <c r="Y161" s="9"/>
       <c r="AA161" s="9"/>
     </row>
-    <row r="162" spans="8:27" s="1" customFormat="1">
+    <row r="162" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H162" s="5"/>
       <c r="I162" s="5"/>
       <c r="J162" s="5"/>
@@ -10324,7 +10334,7 @@
       <c r="Y162" s="9"/>
       <c r="AA162" s="9"/>
     </row>
-    <row r="163" spans="8:27" s="1" customFormat="1">
+    <row r="163" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H163" s="5"/>
       <c r="I163" s="5"/>
       <c r="J163" s="5"/>
@@ -10335,7 +10345,7 @@
       <c r="Y163" s="9"/>
       <c r="AA163" s="9"/>
     </row>
-    <row r="164" spans="8:27" s="1" customFormat="1">
+    <row r="164" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H164" s="5"/>
       <c r="I164" s="5"/>
       <c r="J164" s="5"/>
@@ -10346,7 +10356,7 @@
       <c r="Y164" s="9"/>
       <c r="AA164" s="9"/>
     </row>
-    <row r="165" spans="8:27" s="1" customFormat="1">
+    <row r="165" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H165" s="5"/>
       <c r="I165" s="5"/>
       <c r="J165" s="5"/>
@@ -10357,7 +10367,7 @@
       <c r="Y165" s="9"/>
       <c r="AA165" s="9"/>
     </row>
-    <row r="166" spans="8:27" s="1" customFormat="1">
+    <row r="166" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H166" s="5"/>
       <c r="I166" s="5"/>
       <c r="J166" s="5"/>
@@ -10368,7 +10378,7 @@
       <c r="Y166" s="9"/>
       <c r="AA166" s="9"/>
     </row>
-    <row r="167" spans="8:27" s="1" customFormat="1">
+    <row r="167" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H167" s="5"/>
       <c r="I167" s="5"/>
       <c r="J167" s="5"/>
@@ -10379,7 +10389,7 @@
       <c r="Y167" s="9"/>
       <c r="AA167" s="9"/>
     </row>
-    <row r="168" spans="8:27" s="1" customFormat="1">
+    <row r="168" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H168" s="5"/>
       <c r="I168" s="5"/>
       <c r="J168" s="5"/>
@@ -10390,7 +10400,7 @@
       <c r="Y168" s="9"/>
       <c r="AA168" s="9"/>
     </row>
-    <row r="169" spans="8:27" s="1" customFormat="1">
+    <row r="169" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H169" s="5"/>
       <c r="I169" s="5"/>
       <c r="J169" s="5"/>
@@ -10401,7 +10411,7 @@
       <c r="Y169" s="9"/>
       <c r="AA169" s="9"/>
     </row>
-    <row r="170" spans="8:27" s="1" customFormat="1">
+    <row r="170" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H170" s="5"/>
       <c r="I170" s="5"/>
       <c r="J170" s="5"/>
@@ -10412,7 +10422,7 @@
       <c r="Y170" s="9"/>
       <c r="AA170" s="9"/>
     </row>
-    <row r="171" spans="8:27" s="1" customFormat="1">
+    <row r="171" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H171" s="5"/>
       <c r="I171" s="5"/>
       <c r="J171" s="5"/>
@@ -10423,7 +10433,7 @@
       <c r="Y171" s="9"/>
       <c r="AA171" s="9"/>
     </row>
-    <row r="172" spans="8:27" s="1" customFormat="1">
+    <row r="172" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H172" s="5"/>
       <c r="I172" s="5"/>
       <c r="J172" s="5"/>
@@ -10434,7 +10444,7 @@
       <c r="Y172" s="9"/>
       <c r="AA172" s="9"/>
     </row>
-    <row r="173" spans="8:27" s="1" customFormat="1">
+    <row r="173" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H173" s="5"/>
       <c r="I173" s="5"/>
       <c r="J173" s="5"/>
@@ -10445,7 +10455,7 @@
       <c r="Y173" s="9"/>
       <c r="AA173" s="9"/>
     </row>
-    <row r="174" spans="8:27" s="1" customFormat="1">
+    <row r="174" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H174" s="5"/>
       <c r="I174" s="5"/>
       <c r="J174" s="5"/>
@@ -10456,7 +10466,7 @@
       <c r="Y174" s="9"/>
       <c r="AA174" s="9"/>
     </row>
-    <row r="175" spans="8:27" s="1" customFormat="1">
+    <row r="175" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H175" s="5"/>
       <c r="I175" s="5"/>
       <c r="J175" s="5"/>
@@ -10467,7 +10477,7 @@
       <c r="Y175" s="9"/>
       <c r="AA175" s="9"/>
     </row>
-    <row r="176" spans="8:27" s="1" customFormat="1">
+    <row r="176" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H176" s="5"/>
       <c r="I176" s="5"/>
       <c r="J176" s="5"/>
@@ -10478,7 +10488,7 @@
       <c r="Y176" s="9"/>
       <c r="AA176" s="9"/>
     </row>
-    <row r="177" spans="8:27" s="1" customFormat="1">
+    <row r="177" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H177" s="5"/>
       <c r="I177" s="5"/>
       <c r="J177" s="5"/>
@@ -10489,7 +10499,7 @@
       <c r="Y177" s="9"/>
       <c r="AA177" s="9"/>
     </row>
-    <row r="178" spans="8:27" s="1" customFormat="1">
+    <row r="178" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H178" s="5"/>
       <c r="I178" s="5"/>
       <c r="J178" s="5"/>
@@ -10500,7 +10510,7 @@
       <c r="Y178" s="9"/>
       <c r="AA178" s="9"/>
     </row>
-    <row r="179" spans="8:27" s="1" customFormat="1">
+    <row r="179" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H179" s="5"/>
       <c r="I179" s="5"/>
       <c r="J179" s="5"/>
@@ -10511,7 +10521,7 @@
       <c r="Y179" s="9"/>
       <c r="AA179" s="9"/>
     </row>
-    <row r="180" spans="8:27" s="1" customFormat="1">
+    <row r="180" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H180" s="5"/>
       <c r="I180" s="5"/>
       <c r="J180" s="5"/>
@@ -10522,7 +10532,7 @@
       <c r="Y180" s="9"/>
       <c r="AA180" s="9"/>
     </row>
-    <row r="181" spans="8:27" s="1" customFormat="1">
+    <row r="181" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H181" s="5"/>
       <c r="I181" s="5"/>
       <c r="J181" s="5"/>
@@ -10533,7 +10543,7 @@
       <c r="Y181" s="9"/>
       <c r="AA181" s="9"/>
     </row>
-    <row r="182" spans="8:27" s="1" customFormat="1">
+    <row r="182" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H182" s="5"/>
       <c r="I182" s="5"/>
       <c r="J182" s="5"/>
@@ -10544,7 +10554,7 @@
       <c r="Y182" s="9"/>
       <c r="AA182" s="9"/>
     </row>
-    <row r="183" spans="8:27" s="1" customFormat="1">
+    <row r="183" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H183" s="5"/>
       <c r="I183" s="5"/>
       <c r="J183" s="5"/>
@@ -10555,7 +10565,7 @@
       <c r="Y183" s="9"/>
       <c r="AA183" s="9"/>
     </row>
-    <row r="184" spans="8:27" s="1" customFormat="1">
+    <row r="184" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H184" s="5"/>
       <c r="I184" s="5"/>
       <c r="J184" s="5"/>
@@ -10566,7 +10576,7 @@
       <c r="Y184" s="9"/>
       <c r="AA184" s="9"/>
     </row>
-    <row r="185" spans="8:27" s="1" customFormat="1">
+    <row r="185" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H185" s="5"/>
       <c r="I185" s="5"/>
       <c r="J185" s="5"/>
@@ -10577,7 +10587,7 @@
       <c r="Y185" s="9"/>
       <c r="AA185" s="9"/>
     </row>
-    <row r="186" spans="8:27" s="1" customFormat="1">
+    <row r="186" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H186" s="5"/>
       <c r="I186" s="5"/>
       <c r="J186" s="5"/>
@@ -10588,7 +10598,7 @@
       <c r="Y186" s="9"/>
       <c r="AA186" s="9"/>
     </row>
-    <row r="187" spans="8:27" s="1" customFormat="1">
+    <row r="187" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H187" s="5"/>
       <c r="I187" s="5"/>
       <c r="J187" s="5"/>
@@ -10599,7 +10609,7 @@
       <c r="Y187" s="9"/>
       <c r="AA187" s="9"/>
     </row>
-    <row r="188" spans="8:27" s="1" customFormat="1">
+    <row r="188" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H188" s="5"/>
       <c r="I188" s="5"/>
       <c r="J188" s="5"/>
@@ -10610,7 +10620,7 @@
       <c r="Y188" s="9"/>
       <c r="AA188" s="9"/>
     </row>
-    <row r="189" spans="8:27" s="1" customFormat="1">
+    <row r="189" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H189" s="5"/>
       <c r="I189" s="5"/>
       <c r="J189" s="5"/>
@@ -10621,7 +10631,7 @@
       <c r="Y189" s="9"/>
       <c r="AA189" s="9"/>
     </row>
-    <row r="190" spans="8:27" s="1" customFormat="1">
+    <row r="190" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H190" s="5"/>
       <c r="I190" s="5"/>
       <c r="J190" s="5"/>
@@ -10632,7 +10642,7 @@
       <c r="Y190" s="9"/>
       <c r="AA190" s="9"/>
     </row>
-    <row r="191" spans="8:27" s="1" customFormat="1">
+    <row r="191" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H191" s="5"/>
       <c r="I191" s="5"/>
       <c r="J191" s="5"/>
@@ -10643,7 +10653,7 @@
       <c r="Y191" s="9"/>
       <c r="AA191" s="9"/>
     </row>
-    <row r="192" spans="8:27" s="1" customFormat="1">
+    <row r="192" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H192" s="5"/>
       <c r="I192" s="5"/>
       <c r="J192" s="5"/>
@@ -10654,7 +10664,7 @@
       <c r="Y192" s="9"/>
       <c r="AA192" s="9"/>
     </row>
-    <row r="193" spans="8:27" s="1" customFormat="1">
+    <row r="193" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H193" s="5"/>
       <c r="I193" s="5"/>
       <c r="J193" s="5"/>
@@ -10665,7 +10675,7 @@
       <c r="Y193" s="9"/>
       <c r="AA193" s="9"/>
     </row>
-    <row r="194" spans="8:27" s="1" customFormat="1">
+    <row r="194" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H194" s="5"/>
       <c r="I194" s="5"/>
       <c r="J194" s="5"/>
@@ -10676,7 +10686,7 @@
       <c r="Y194" s="9"/>
       <c r="AA194" s="9"/>
     </row>
-    <row r="195" spans="8:27" s="1" customFormat="1">
+    <row r="195" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H195" s="5"/>
       <c r="I195" s="5"/>
       <c r="J195" s="5"/>
@@ -10687,7 +10697,7 @@
       <c r="Y195" s="9"/>
       <c r="AA195" s="9"/>
     </row>
-    <row r="196" spans="8:27" s="1" customFormat="1">
+    <row r="196" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H196" s="5"/>
       <c r="I196" s="5"/>
       <c r="J196" s="5"/>
@@ -10698,7 +10708,7 @@
       <c r="Y196" s="9"/>
       <c r="AA196" s="9"/>
     </row>
-    <row r="197" spans="8:27" s="1" customFormat="1">
+    <row r="197" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H197" s="5"/>
       <c r="I197" s="5"/>
       <c r="J197" s="5"/>
@@ -10709,7 +10719,7 @@
       <c r="Y197" s="9"/>
       <c r="AA197" s="9"/>
     </row>
-    <row r="198" spans="8:27" s="1" customFormat="1">
+    <row r="198" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H198" s="5"/>
       <c r="I198" s="5"/>
       <c r="J198" s="5"/>
@@ -10720,7 +10730,7 @@
       <c r="Y198" s="9"/>
       <c r="AA198" s="9"/>
     </row>
-    <row r="199" spans="8:27" s="1" customFormat="1">
+    <row r="199" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H199" s="5"/>
       <c r="I199" s="5"/>
       <c r="J199" s="5"/>
@@ -10731,7 +10741,7 @@
       <c r="Y199" s="9"/>
       <c r="AA199" s="9"/>
     </row>
-    <row r="200" spans="8:27" s="1" customFormat="1">
+    <row r="200" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H200" s="5"/>
       <c r="I200" s="5"/>
       <c r="J200" s="5"/>
@@ -10742,7 +10752,7 @@
       <c r="Y200" s="9"/>
       <c r="AA200" s="9"/>
     </row>
-    <row r="201" spans="8:27" s="1" customFormat="1">
+    <row r="201" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H201" s="5"/>
       <c r="I201" s="5"/>
       <c r="J201" s="5"/>
@@ -10753,7 +10763,7 @@
       <c r="Y201" s="9"/>
       <c r="AA201" s="9"/>
     </row>
-    <row r="202" spans="8:27" s="1" customFormat="1">
+    <row r="202" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H202" s="5"/>
       <c r="I202" s="5"/>
       <c r="J202" s="5"/>
@@ -10764,7 +10774,7 @@
       <c r="Y202" s="9"/>
       <c r="AA202" s="9"/>
     </row>
-    <row r="203" spans="8:27" s="1" customFormat="1">
+    <row r="203" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H203" s="5"/>
       <c r="I203" s="5"/>
       <c r="J203" s="5"/>
@@ -10775,7 +10785,7 @@
       <c r="Y203" s="9"/>
       <c r="AA203" s="9"/>
     </row>
-    <row r="204" spans="8:27" s="1" customFormat="1">
+    <row r="204" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H204" s="5"/>
       <c r="I204" s="5"/>
       <c r="J204" s="5"/>
@@ -10786,7 +10796,7 @@
       <c r="Y204" s="9"/>
       <c r="AA204" s="9"/>
     </row>
-    <row r="205" spans="8:27" s="1" customFormat="1">
+    <row r="205" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H205" s="5"/>
       <c r="I205" s="5"/>
       <c r="J205" s="5"/>
@@ -10797,7 +10807,7 @@
       <c r="Y205" s="9"/>
       <c r="AA205" s="9"/>
     </row>
-    <row r="206" spans="8:27" s="1" customFormat="1">
+    <row r="206" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H206" s="5"/>
       <c r="I206" s="5"/>
       <c r="J206" s="5"/>
@@ -10808,7 +10818,7 @@
       <c r="Y206" s="9"/>
       <c r="AA206" s="9"/>
     </row>
-    <row r="207" spans="8:27" s="1" customFormat="1">
+    <row r="207" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H207" s="5"/>
       <c r="I207" s="5"/>
       <c r="J207" s="5"/>
@@ -10819,7 +10829,7 @@
       <c r="Y207" s="9"/>
       <c r="AA207" s="9"/>
     </row>
-    <row r="208" spans="8:27" s="1" customFormat="1">
+    <row r="208" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H208" s="5"/>
       <c r="I208" s="5"/>
       <c r="J208" s="5"/>
@@ -10830,7 +10840,7 @@
       <c r="Y208" s="9"/>
       <c r="AA208" s="9"/>
     </row>
-    <row r="209" spans="8:27" s="1" customFormat="1">
+    <row r="209" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H209" s="5"/>
       <c r="I209" s="5"/>
       <c r="J209" s="5"/>
@@ -10841,7 +10851,7 @@
       <c r="Y209" s="9"/>
       <c r="AA209" s="9"/>
     </row>
-    <row r="210" spans="8:27" s="1" customFormat="1">
+    <row r="210" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H210" s="5"/>
       <c r="I210" s="5"/>
       <c r="J210" s="5"/>
@@ -10852,7 +10862,7 @@
       <c r="Y210" s="9"/>
       <c r="AA210" s="9"/>
     </row>
-    <row r="211" spans="8:27" s="1" customFormat="1">
+    <row r="211" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H211" s="5"/>
       <c r="I211" s="5"/>
       <c r="J211" s="5"/>
@@ -10863,7 +10873,7 @@
       <c r="Y211" s="9"/>
       <c r="AA211" s="9"/>
     </row>
-    <row r="212" spans="8:27" s="1" customFormat="1">
+    <row r="212" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H212" s="5"/>
       <c r="I212" s="5"/>
       <c r="J212" s="5"/>
@@ -10874,7 +10884,7 @@
       <c r="Y212" s="9"/>
       <c r="AA212" s="9"/>
     </row>
-    <row r="213" spans="8:27" s="1" customFormat="1">
+    <row r="213" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H213" s="5"/>
       <c r="I213" s="5"/>
       <c r="J213" s="5"/>
@@ -10885,7 +10895,7 @@
       <c r="Y213" s="9"/>
       <c r="AA213" s="9"/>
     </row>
-    <row r="214" spans="8:27" s="1" customFormat="1">
+    <row r="214" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H214" s="5"/>
       <c r="I214" s="5"/>
       <c r="J214" s="5"/>
@@ -10896,7 +10906,7 @@
       <c r="Y214" s="9"/>
       <c r="AA214" s="9"/>
     </row>
-    <row r="215" spans="8:27" s="1" customFormat="1">
+    <row r="215" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H215" s="5"/>
       <c r="I215" s="5"/>
       <c r="J215" s="5"/>
@@ -10907,7 +10917,7 @@
       <c r="Y215" s="9"/>
       <c r="AA215" s="9"/>
     </row>
-    <row r="216" spans="8:27" s="1" customFormat="1">
+    <row r="216" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H216" s="5"/>
       <c r="I216" s="5"/>
       <c r="J216" s="5"/>
@@ -10918,7 +10928,7 @@
       <c r="Y216" s="9"/>
       <c r="AA216" s="9"/>
     </row>
-    <row r="217" spans="8:27" s="1" customFormat="1">
+    <row r="217" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H217" s="5"/>
       <c r="I217" s="5"/>
       <c r="J217" s="5"/>
@@ -10929,7 +10939,7 @@
       <c r="Y217" s="9"/>
       <c r="AA217" s="9"/>
     </row>
-    <row r="218" spans="8:27" s="1" customFormat="1">
+    <row r="218" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H218" s="5"/>
       <c r="I218" s="5"/>
       <c r="J218" s="5"/>
@@ -10940,7 +10950,7 @@
       <c r="Y218" s="9"/>
       <c r="AA218" s="9"/>
     </row>
-    <row r="219" spans="8:27" s="1" customFormat="1">
+    <row r="219" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H219" s="5"/>
       <c r="I219" s="5"/>
       <c r="J219" s="5"/>
@@ -10951,7 +10961,7 @@
       <c r="Y219" s="9"/>
       <c r="AA219" s="9"/>
     </row>
-    <row r="220" spans="8:27" s="1" customFormat="1">
+    <row r="220" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H220" s="5"/>
       <c r="I220" s="5"/>
       <c r="J220" s="5"/>
@@ -10962,7 +10972,7 @@
       <c r="Y220" s="9"/>
       <c r="AA220" s="9"/>
     </row>
-    <row r="221" spans="8:27" s="1" customFormat="1">
+    <row r="221" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H221" s="5"/>
       <c r="I221" s="5"/>
       <c r="J221" s="5"/>
@@ -10973,7 +10983,7 @@
       <c r="Y221" s="9"/>
       <c r="AA221" s="9"/>
     </row>
-    <row r="222" spans="8:27" s="1" customFormat="1">
+    <row r="222" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H222" s="5"/>
       <c r="I222" s="5"/>
       <c r="J222" s="5"/>
@@ -10984,7 +10994,7 @@
       <c r="Y222" s="9"/>
       <c r="AA222" s="9"/>
     </row>
-    <row r="223" spans="8:27" s="1" customFormat="1">
+    <row r="223" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H223" s="5"/>
       <c r="I223" s="5"/>
       <c r="J223" s="5"/>
@@ -10995,7 +11005,7 @@
       <c r="Y223" s="9"/>
       <c r="AA223" s="9"/>
     </row>
-    <row r="224" spans="8:27" s="1" customFormat="1">
+    <row r="224" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H224" s="5"/>
       <c r="I224" s="5"/>
       <c r="J224" s="5"/>
@@ -11006,7 +11016,7 @@
       <c r="Y224" s="9"/>
       <c r="AA224" s="9"/>
     </row>
-    <row r="225" spans="8:27" s="1" customFormat="1">
+    <row r="225" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H225" s="5"/>
       <c r="I225" s="5"/>
       <c r="J225" s="5"/>
@@ -11017,7 +11027,7 @@
       <c r="Y225" s="9"/>
       <c r="AA225" s="9"/>
     </row>
-    <row r="226" spans="8:27" s="1" customFormat="1">
+    <row r="226" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H226" s="5"/>
       <c r="I226" s="5"/>
       <c r="J226" s="5"/>
@@ -11028,7 +11038,7 @@
       <c r="Y226" s="9"/>
       <c r="AA226" s="9"/>
     </row>
-    <row r="227" spans="8:27" s="1" customFormat="1">
+    <row r="227" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H227" s="5"/>
       <c r="I227" s="5"/>
       <c r="J227" s="5"/>
@@ -11039,7 +11049,7 @@
       <c r="Y227" s="9"/>
       <c r="AA227" s="9"/>
     </row>
-    <row r="228" spans="8:27" s="1" customFormat="1">
+    <row r="228" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H228" s="5"/>
       <c r="I228" s="5"/>
       <c r="J228" s="5"/>
@@ -11050,7 +11060,7 @@
       <c r="Y228" s="9"/>
       <c r="AA228" s="9"/>
     </row>
-    <row r="229" spans="8:27" s="1" customFormat="1">
+    <row r="229" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H229" s="5"/>
       <c r="I229" s="5"/>
       <c r="J229" s="5"/>
@@ -11061,7 +11071,7 @@
       <c r="Y229" s="9"/>
       <c r="AA229" s="9"/>
     </row>
-    <row r="230" spans="8:27" s="1" customFormat="1">
+    <row r="230" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H230" s="5"/>
       <c r="I230" s="5"/>
       <c r="J230" s="5"/>
@@ -11072,7 +11082,7 @@
       <c r="Y230" s="9"/>
       <c r="AA230" s="9"/>
     </row>
-    <row r="231" spans="8:27" s="1" customFormat="1">
+    <row r="231" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H231" s="5"/>
       <c r="I231" s="5"/>
       <c r="J231" s="5"/>
@@ -11083,7 +11093,7 @@
       <c r="Y231" s="9"/>
       <c r="AA231" s="9"/>
     </row>
-    <row r="232" spans="8:27" s="1" customFormat="1">
+    <row r="232" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H232" s="5"/>
       <c r="I232" s="5"/>
       <c r="J232" s="5"/>
@@ -11094,7 +11104,7 @@
       <c r="Y232" s="9"/>
       <c r="AA232" s="9"/>
     </row>
-    <row r="233" spans="8:27" s="1" customFormat="1">
+    <row r="233" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H233" s="5"/>
       <c r="I233" s="5"/>
       <c r="J233" s="5"/>
@@ -11105,7 +11115,7 @@
       <c r="Y233" s="9"/>
       <c r="AA233" s="9"/>
     </row>
-    <row r="234" spans="8:27" s="1" customFormat="1">
+    <row r="234" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H234" s="5"/>
       <c r="I234" s="5"/>
       <c r="J234" s="5"/>
@@ -11116,7 +11126,7 @@
       <c r="Y234" s="9"/>
       <c r="AA234" s="9"/>
     </row>
-    <row r="235" spans="8:27" s="1" customFormat="1">
+    <row r="235" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H235" s="5"/>
       <c r="I235" s="5"/>
       <c r="J235" s="5"/>
@@ -11127,7 +11137,7 @@
       <c r="Y235" s="9"/>
       <c r="AA235" s="9"/>
     </row>
-    <row r="236" spans="8:27" s="1" customFormat="1">
+    <row r="236" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H236" s="5"/>
       <c r="I236" s="5"/>
       <c r="J236" s="5"/>
@@ -11138,7 +11148,7 @@
       <c r="Y236" s="9"/>
       <c r="AA236" s="9"/>
     </row>
-    <row r="237" spans="8:27" s="1" customFormat="1">
+    <row r="237" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H237" s="5"/>
       <c r="I237" s="5"/>
       <c r="J237" s="5"/>
@@ -11149,7 +11159,7 @@
       <c r="Y237" s="9"/>
       <c r="AA237" s="9"/>
     </row>
-    <row r="238" spans="8:27" s="1" customFormat="1">
+    <row r="238" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H238" s="5"/>
       <c r="I238" s="5"/>
       <c r="J238" s="5"/>
@@ -11160,7 +11170,7 @@
       <c r="Y238" s="9"/>
       <c r="AA238" s="9"/>
     </row>
-    <row r="239" spans="8:27" s="1" customFormat="1">
+    <row r="239" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H239" s="5"/>
       <c r="I239" s="5"/>
       <c r="J239" s="5"/>
@@ -11171,7 +11181,7 @@
       <c r="Y239" s="9"/>
       <c r="AA239" s="9"/>
     </row>
-    <row r="240" spans="8:27" s="1" customFormat="1">
+    <row r="240" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H240" s="5"/>
       <c r="I240" s="5"/>
       <c r="J240" s="5"/>
@@ -11182,7 +11192,7 @@
       <c r="Y240" s="9"/>
       <c r="AA240" s="9"/>
     </row>
-    <row r="241" spans="8:27" s="1" customFormat="1">
+    <row r="241" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H241" s="5"/>
       <c r="I241" s="5"/>
       <c r="J241" s="5"/>
@@ -11193,7 +11203,7 @@
       <c r="Y241" s="9"/>
       <c r="AA241" s="9"/>
     </row>
-    <row r="242" spans="8:27" s="1" customFormat="1">
+    <row r="242" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H242" s="5"/>
       <c r="I242" s="5"/>
       <c r="J242" s="5"/>
@@ -11204,7 +11214,7 @@
       <c r="Y242" s="9"/>
       <c r="AA242" s="9"/>
     </row>
-    <row r="243" spans="8:27" s="1" customFormat="1">
+    <row r="243" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H243" s="5"/>
       <c r="I243" s="5"/>
       <c r="J243" s="5"/>
@@ -11215,7 +11225,7 @@
       <c r="Y243" s="9"/>
       <c r="AA243" s="9"/>
     </row>
-    <row r="244" spans="8:27" s="1" customFormat="1">
+    <row r="244" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H244" s="5"/>
       <c r="I244" s="5"/>
       <c r="J244" s="5"/>
@@ -11226,7 +11236,7 @@
       <c r="Y244" s="9"/>
       <c r="AA244" s="9"/>
     </row>
-    <row r="245" spans="8:27" s="1" customFormat="1">
+    <row r="245" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H245" s="5"/>
       <c r="I245" s="5"/>
       <c r="J245" s="5"/>
@@ -11237,7 +11247,7 @@
       <c r="Y245" s="9"/>
       <c r="AA245" s="9"/>
     </row>
-    <row r="246" spans="8:27" s="1" customFormat="1">
+    <row r="246" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H246" s="5"/>
       <c r="I246" s="5"/>
       <c r="J246" s="5"/>
@@ -11248,7 +11258,7 @@
       <c r="Y246" s="9"/>
       <c r="AA246" s="9"/>
     </row>
-    <row r="247" spans="8:27" s="1" customFormat="1">
+    <row r="247" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H247" s="5"/>
       <c r="I247" s="5"/>
       <c r="J247" s="5"/>
@@ -11259,7 +11269,7 @@
       <c r="Y247" s="9"/>
       <c r="AA247" s="9"/>
     </row>
-    <row r="248" spans="8:27" s="1" customFormat="1">
+    <row r="248" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H248" s="5"/>
       <c r="I248" s="5"/>
       <c r="J248" s="5"/>
@@ -11270,7 +11280,7 @@
       <c r="Y248" s="9"/>
       <c r="AA248" s="9"/>
     </row>
-    <row r="249" spans="8:27" s="1" customFormat="1">
+    <row r="249" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H249" s="5"/>
       <c r="I249" s="5"/>
       <c r="J249" s="5"/>
@@ -11281,7 +11291,7 @@
       <c r="Y249" s="9"/>
       <c r="AA249" s="9"/>
     </row>
-    <row r="250" spans="8:27" s="1" customFormat="1">
+    <row r="250" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H250" s="5"/>
       <c r="I250" s="5"/>
       <c r="J250" s="5"/>
@@ -11292,7 +11302,7 @@
       <c r="Y250" s="9"/>
       <c r="AA250" s="9"/>
     </row>
-    <row r="251" spans="8:27" s="1" customFormat="1">
+    <row r="251" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H251" s="5"/>
       <c r="I251" s="5"/>
       <c r="J251" s="5"/>
@@ -11303,7 +11313,7 @@
       <c r="Y251" s="9"/>
       <c r="AA251" s="9"/>
     </row>
-    <row r="252" spans="8:27" s="1" customFormat="1">
+    <row r="252" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H252" s="5"/>
       <c r="I252" s="5"/>
       <c r="J252" s="5"/>
@@ -11314,7 +11324,7 @@
       <c r="Y252" s="9"/>
       <c r="AA252" s="9"/>
     </row>
-    <row r="253" spans="8:27" s="1" customFormat="1">
+    <row r="253" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H253" s="5"/>
       <c r="I253" s="5"/>
       <c r="J253" s="5"/>
@@ -11325,7 +11335,7 @@
       <c r="Y253" s="9"/>
       <c r="AA253" s="9"/>
     </row>
-    <row r="254" spans="8:27" s="1" customFormat="1">
+    <row r="254" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H254" s="5"/>
       <c r="I254" s="5"/>
       <c r="J254" s="5"/>
@@ -11336,7 +11346,7 @@
       <c r="Y254" s="9"/>
       <c r="AA254" s="9"/>
     </row>
-    <row r="255" spans="8:27" s="1" customFormat="1">
+    <row r="255" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H255" s="5"/>
       <c r="I255" s="5"/>
       <c r="J255" s="5"/>
@@ -11347,7 +11357,7 @@
       <c r="Y255" s="9"/>
       <c r="AA255" s="9"/>
     </row>
-    <row r="256" spans="8:27" s="1" customFormat="1">
+    <row r="256" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H256" s="5"/>
       <c r="I256" s="5"/>
       <c r="J256" s="5"/>
@@ -11358,7 +11368,7 @@
       <c r="Y256" s="9"/>
       <c r="AA256" s="9"/>
     </row>
-    <row r="257" spans="8:27" s="1" customFormat="1">
+    <row r="257" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H257" s="5"/>
       <c r="I257" s="5"/>
       <c r="J257" s="5"/>
@@ -11369,7 +11379,7 @@
       <c r="Y257" s="9"/>
       <c r="AA257" s="9"/>
     </row>
-    <row r="258" spans="8:27" s="1" customFormat="1">
+    <row r="258" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H258" s="5"/>
       <c r="I258" s="5"/>
       <c r="J258" s="5"/>
@@ -11380,7 +11390,7 @@
       <c r="Y258" s="9"/>
       <c r="AA258" s="9"/>
     </row>
-    <row r="259" spans="8:27" s="1" customFormat="1">
+    <row r="259" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H259" s="5"/>
       <c r="I259" s="5"/>
       <c r="J259" s="5"/>
@@ -11391,7 +11401,7 @@
       <c r="Y259" s="9"/>
       <c r="AA259" s="9"/>
     </row>
-    <row r="260" spans="8:27" s="1" customFormat="1">
+    <row r="260" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H260" s="5"/>
       <c r="I260" s="5"/>
       <c r="J260" s="5"/>
@@ -11402,7 +11412,7 @@
       <c r="Y260" s="9"/>
       <c r="AA260" s="9"/>
     </row>
-    <row r="261" spans="8:27" s="1" customFormat="1">
+    <row r="261" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H261" s="5"/>
       <c r="I261" s="5"/>
       <c r="J261" s="5"/>
@@ -11413,7 +11423,7 @@
       <c r="Y261" s="9"/>
       <c r="AA261" s="9"/>
     </row>
-    <row r="262" spans="8:27" s="1" customFormat="1">
+    <row r="262" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H262" s="5"/>
       <c r="I262" s="5"/>
       <c r="J262" s="5"/>
@@ -11424,7 +11434,7 @@
       <c r="Y262" s="9"/>
       <c r="AA262" s="9"/>
     </row>
-    <row r="263" spans="8:27" s="1" customFormat="1">
+    <row r="263" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H263" s="5"/>
       <c r="I263" s="5"/>
       <c r="J263" s="5"/>
@@ -11435,7 +11445,7 @@
       <c r="Y263" s="9"/>
       <c r="AA263" s="9"/>
     </row>
-    <row r="264" spans="8:27" s="1" customFormat="1">
+    <row r="264" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H264" s="5"/>
       <c r="I264" s="5"/>
       <c r="J264" s="5"/>
@@ -11446,7 +11456,7 @@
       <c r="Y264" s="9"/>
       <c r="AA264" s="9"/>
     </row>
-    <row r="265" spans="8:27" s="1" customFormat="1">
+    <row r="265" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H265" s="5"/>
       <c r="I265" s="5"/>
       <c r="J265" s="5"/>
@@ -11457,7 +11467,7 @@
       <c r="Y265" s="9"/>
       <c r="AA265" s="9"/>
     </row>
-    <row r="266" spans="8:27" s="1" customFormat="1">
+    <row r="266" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H266" s="5"/>
       <c r="I266" s="5"/>
       <c r="J266" s="5"/>
@@ -11468,7 +11478,7 @@
       <c r="Y266" s="9"/>
       <c r="AA266" s="9"/>
     </row>
-    <row r="267" spans="8:27" s="1" customFormat="1">
+    <row r="267" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H267" s="5"/>
       <c r="I267" s="5"/>
       <c r="J267" s="5"/>
@@ -11479,7 +11489,7 @@
       <c r="Y267" s="9"/>
       <c r="AA267" s="9"/>
     </row>
-    <row r="268" spans="8:27" s="1" customFormat="1">
+    <row r="268" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H268" s="5"/>
       <c r="I268" s="5"/>
       <c r="J268" s="5"/>
@@ -11490,7 +11500,7 @@
       <c r="Y268" s="9"/>
       <c r="AA268" s="9"/>
     </row>
-    <row r="269" spans="8:27" s="1" customFormat="1">
+    <row r="269" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H269" s="5"/>
       <c r="I269" s="5"/>
       <c r="J269" s="5"/>
@@ -11501,7 +11511,7 @@
       <c r="Y269" s="9"/>
       <c r="AA269" s="9"/>
     </row>
-    <row r="270" spans="8:27" s="1" customFormat="1">
+    <row r="270" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H270" s="5"/>
       <c r="I270" s="5"/>
       <c r="J270" s="5"/>
@@ -11512,7 +11522,7 @@
       <c r="Y270" s="9"/>
       <c r="AA270" s="9"/>
     </row>
-    <row r="271" spans="8:27" s="1" customFormat="1">
+    <row r="271" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H271" s="5"/>
       <c r="I271" s="5"/>
       <c r="J271" s="5"/>
@@ -11523,7 +11533,7 @@
       <c r="Y271" s="9"/>
       <c r="AA271" s="9"/>
     </row>
-    <row r="272" spans="8:27" s="1" customFormat="1">
+    <row r="272" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H272" s="5"/>
       <c r="I272" s="5"/>
       <c r="J272" s="5"/>
@@ -11534,7 +11544,7 @@
       <c r="Y272" s="9"/>
       <c r="AA272" s="9"/>
     </row>
-    <row r="273" spans="8:27" s="1" customFormat="1">
+    <row r="273" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H273" s="5"/>
       <c r="I273" s="5"/>
       <c r="J273" s="5"/>
@@ -11545,7 +11555,7 @@
       <c r="Y273" s="9"/>
       <c r="AA273" s="9"/>
     </row>
-    <row r="274" spans="8:27" s="1" customFormat="1">
+    <row r="274" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H274" s="5"/>
       <c r="I274" s="5"/>
       <c r="J274" s="5"/>
@@ -11556,7 +11566,7 @@
       <c r="Y274" s="9"/>
       <c r="AA274" s="9"/>
     </row>
-    <row r="275" spans="8:27" s="1" customFormat="1">
+    <row r="275" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H275" s="5"/>
       <c r="I275" s="5"/>
       <c r="J275" s="5"/>
@@ -11567,7 +11577,7 @@
       <c r="Y275" s="9"/>
       <c r="AA275" s="9"/>
     </row>
-    <row r="276" spans="8:27" s="1" customFormat="1">
+    <row r="276" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H276" s="5"/>
       <c r="I276" s="5"/>
       <c r="J276" s="5"/>
@@ -11578,7 +11588,7 @@
       <c r="Y276" s="9"/>
       <c r="AA276" s="9"/>
     </row>
-    <row r="277" spans="8:27" s="1" customFormat="1">
+    <row r="277" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H277" s="5"/>
       <c r="I277" s="5"/>
       <c r="J277" s="5"/>
@@ -11589,7 +11599,7 @@
       <c r="Y277" s="9"/>
       <c r="AA277" s="9"/>
     </row>
-    <row r="278" spans="8:27" s="1" customFormat="1">
+    <row r="278" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H278" s="5"/>
       <c r="I278" s="5"/>
       <c r="J278" s="5"/>
@@ -11600,7 +11610,7 @@
       <c r="Y278" s="9"/>
       <c r="AA278" s="9"/>
     </row>
-    <row r="279" spans="8:27" s="1" customFormat="1">
+    <row r="279" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H279" s="5"/>
       <c r="I279" s="5"/>
       <c r="J279" s="5"/>
@@ -11611,7 +11621,7 @@
       <c r="Y279" s="9"/>
       <c r="AA279" s="9"/>
     </row>
-    <row r="280" spans="8:27" s="1" customFormat="1">
+    <row r="280" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H280" s="5"/>
       <c r="I280" s="5"/>
       <c r="J280" s="5"/>
@@ -11622,7 +11632,7 @@
       <c r="Y280" s="9"/>
       <c r="AA280" s="9"/>
     </row>
-    <row r="281" spans="8:27" s="1" customFormat="1">
+    <row r="281" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H281" s="5"/>
       <c r="I281" s="5"/>
       <c r="J281" s="5"/>
@@ -11633,7 +11643,7 @@
       <c r="Y281" s="9"/>
       <c r="AA281" s="9"/>
     </row>
-    <row r="282" spans="8:27" s="1" customFormat="1">
+    <row r="282" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H282" s="5"/>
       <c r="I282" s="5"/>
       <c r="J282" s="5"/>
@@ -11644,7 +11654,7 @@
       <c r="Y282" s="9"/>
       <c r="AA282" s="9"/>
     </row>
-    <row r="283" spans="8:27" s="1" customFormat="1">
+    <row r="283" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H283" s="5"/>
       <c r="I283" s="5"/>
       <c r="J283" s="5"/>
@@ -11655,7 +11665,7 @@
       <c r="Y283" s="9"/>
       <c r="AA283" s="9"/>
     </row>
-    <row r="284" spans="8:27" s="1" customFormat="1">
+    <row r="284" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H284" s="5"/>
       <c r="I284" s="5"/>
       <c r="J284" s="5"/>
@@ -11666,7 +11676,7 @@
       <c r="Y284" s="9"/>
       <c r="AA284" s="9"/>
     </row>
-    <row r="285" spans="8:27" s="1" customFormat="1">
+    <row r="285" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H285" s="5"/>
       <c r="I285" s="5"/>
       <c r="J285" s="5"/>
@@ -11677,7 +11687,7 @@
       <c r="Y285" s="9"/>
       <c r="AA285" s="9"/>
     </row>
-    <row r="286" spans="8:27" s="1" customFormat="1">
+    <row r="286" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H286" s="5"/>
       <c r="I286" s="5"/>
       <c r="J286" s="5"/>
@@ -11688,7 +11698,7 @@
       <c r="Y286" s="9"/>
       <c r="AA286" s="9"/>
     </row>
-    <row r="287" spans="8:27" s="1" customFormat="1">
+    <row r="287" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H287" s="5"/>
       <c r="I287" s="5"/>
       <c r="J287" s="5"/>
@@ -11699,7 +11709,7 @@
       <c r="Y287" s="9"/>
       <c r="AA287" s="9"/>
     </row>
-    <row r="288" spans="8:27" s="1" customFormat="1">
+    <row r="288" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H288" s="5"/>
       <c r="I288" s="5"/>
       <c r="J288" s="5"/>
@@ -11710,7 +11720,7 @@
       <c r="Y288" s="9"/>
       <c r="AA288" s="9"/>
     </row>
-    <row r="289" spans="8:27" s="1" customFormat="1">
+    <row r="289" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H289" s="5"/>
       <c r="I289" s="5"/>
       <c r="J289" s="5"/>
@@ -11721,7 +11731,7 @@
       <c r="Y289" s="9"/>
       <c r="AA289" s="9"/>
     </row>
-    <row r="290" spans="8:27" s="1" customFormat="1">
+    <row r="290" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H290" s="5"/>
       <c r="I290" s="5"/>
       <c r="J290" s="5"/>
@@ -11732,7 +11742,7 @@
       <c r="Y290" s="9"/>
       <c r="AA290" s="9"/>
     </row>
-    <row r="291" spans="8:27" s="1" customFormat="1">
+    <row r="291" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H291" s="5"/>
       <c r="I291" s="5"/>
       <c r="J291" s="5"/>
@@ -11743,7 +11753,7 @@
       <c r="Y291" s="9"/>
       <c r="AA291" s="9"/>
     </row>
-    <row r="292" spans="8:27" s="1" customFormat="1">
+    <row r="292" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H292" s="5"/>
       <c r="I292" s="5"/>
       <c r="J292" s="5"/>
@@ -11754,7 +11764,7 @@
       <c r="Y292" s="9"/>
       <c r="AA292" s="9"/>
     </row>
-    <row r="293" spans="8:27" s="1" customFormat="1">
+    <row r="293" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H293" s="5"/>
       <c r="I293" s="5"/>
       <c r="J293" s="5"/>
@@ -11765,7 +11775,7 @@
       <c r="Y293" s="9"/>
       <c r="AA293" s="9"/>
     </row>
-    <row r="294" spans="8:27" s="1" customFormat="1">
+    <row r="294" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H294" s="5"/>
       <c r="I294" s="5"/>
       <c r="J294" s="5"/>
@@ -11776,7 +11786,7 @@
       <c r="Y294" s="9"/>
       <c r="AA294" s="9"/>
     </row>
-    <row r="295" spans="8:27" s="1" customFormat="1">
+    <row r="295" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H295" s="5"/>
       <c r="I295" s="5"/>
       <c r="J295" s="5"/>
@@ -11787,7 +11797,7 @@
       <c r="Y295" s="9"/>
       <c r="AA295" s="9"/>
     </row>
-    <row r="296" spans="8:27" s="1" customFormat="1">
+    <row r="296" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H296" s="5"/>
       <c r="I296" s="5"/>
       <c r="J296" s="5"/>
@@ -11798,7 +11808,7 @@
       <c r="Y296" s="9"/>
       <c r="AA296" s="9"/>
     </row>
-    <row r="297" spans="8:27" s="1" customFormat="1">
+    <row r="297" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H297" s="5"/>
       <c r="I297" s="5"/>
       <c r="J297" s="5"/>
@@ -11809,7 +11819,7 @@
       <c r="Y297" s="9"/>
       <c r="AA297" s="9"/>
     </row>
-    <row r="298" spans="8:27" s="1" customFormat="1">
+    <row r="298" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H298" s="5"/>
       <c r="I298" s="5"/>
       <c r="J298" s="5"/>
@@ -11820,7 +11830,7 @@
       <c r="Y298" s="9"/>
       <c r="AA298" s="9"/>
     </row>
-    <row r="299" spans="8:27" s="1" customFormat="1">
+    <row r="299" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H299" s="5"/>
       <c r="I299" s="5"/>
       <c r="J299" s="5"/>
@@ -11831,7 +11841,7 @@
       <c r="Y299" s="9"/>
       <c r="AA299" s="9"/>
     </row>
-    <row r="300" spans="8:27" s="1" customFormat="1">
+    <row r="300" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H300" s="5"/>
       <c r="I300" s="5"/>
       <c r="J300" s="5"/>
@@ -11842,7 +11852,7 @@
       <c r="Y300" s="9"/>
       <c r="AA300" s="9"/>
     </row>
-    <row r="301" spans="8:27" s="1" customFormat="1">
+    <row r="301" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H301" s="5"/>
       <c r="I301" s="5"/>
       <c r="J301" s="5"/>
@@ -11853,7 +11863,7 @@
       <c r="Y301" s="9"/>
       <c r="AA301" s="9"/>
     </row>
-    <row r="302" spans="8:27" s="1" customFormat="1">
+    <row r="302" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H302" s="5"/>
       <c r="I302" s="5"/>
       <c r="J302" s="5"/>
@@ -11864,7 +11874,7 @@
       <c r="Y302" s="9"/>
       <c r="AA302" s="9"/>
     </row>
-    <row r="303" spans="8:27" s="1" customFormat="1">
+    <row r="303" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H303" s="5"/>
       <c r="I303" s="5"/>
       <c r="J303" s="5"/>
@@ -11875,7 +11885,7 @@
       <c r="Y303" s="9"/>
       <c r="AA303" s="9"/>
     </row>
-    <row r="304" spans="8:27" s="1" customFormat="1">
+    <row r="304" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H304" s="5"/>
       <c r="I304" s="5"/>
       <c r="J304" s="5"/>
@@ -11886,7 +11896,7 @@
       <c r="Y304" s="9"/>
       <c r="AA304" s="9"/>
     </row>
-    <row r="305" spans="8:27" s="1" customFormat="1">
+    <row r="305" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H305" s="5"/>
       <c r="I305" s="5"/>
       <c r="J305" s="5"/>
@@ -11897,7 +11907,7 @@
       <c r="Y305" s="9"/>
       <c r="AA305" s="9"/>
     </row>
-    <row r="306" spans="8:27" s="1" customFormat="1">
+    <row r="306" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H306" s="5"/>
       <c r="I306" s="5"/>
       <c r="J306" s="5"/>
@@ -11908,7 +11918,7 @@
       <c r="Y306" s="9"/>
       <c r="AA306" s="9"/>
     </row>
-    <row r="307" spans="8:27" s="1" customFormat="1">
+    <row r="307" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H307" s="5"/>
       <c r="I307" s="5"/>
       <c r="J307" s="5"/>
@@ -11919,7 +11929,7 @@
       <c r="Y307" s="9"/>
       <c r="AA307" s="9"/>
     </row>
-    <row r="308" spans="8:27" s="1" customFormat="1">
+    <row r="308" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H308" s="5"/>
       <c r="I308" s="5"/>
       <c r="J308" s="5"/>
@@ -11930,7 +11940,7 @@
       <c r="Y308" s="9"/>
       <c r="AA308" s="9"/>
     </row>
-    <row r="309" spans="8:27" s="1" customFormat="1">
+    <row r="309" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H309" s="5"/>
       <c r="I309" s="5"/>
       <c r="J309" s="5"/>
@@ -11941,7 +11951,7 @@
       <c r="Y309" s="9"/>
       <c r="AA309" s="9"/>
     </row>
-    <row r="310" spans="8:27" s="1" customFormat="1">
+    <row r="310" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H310" s="5"/>
       <c r="I310" s="5"/>
       <c r="J310" s="5"/>
@@ -11952,7 +11962,7 @@
       <c r="Y310" s="9"/>
       <c r="AA310" s="9"/>
     </row>
-    <row r="311" spans="8:27" s="1" customFormat="1">
+    <row r="311" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H311" s="5"/>
       <c r="I311" s="5"/>
       <c r="J311" s="5"/>
@@ -11963,7 +11973,7 @@
       <c r="Y311" s="9"/>
       <c r="AA311" s="9"/>
     </row>
-    <row r="312" spans="8:27" s="1" customFormat="1">
+    <row r="312" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H312" s="5"/>
       <c r="I312" s="5"/>
       <c r="J312" s="5"/>
@@ -11974,7 +11984,7 @@
       <c r="Y312" s="9"/>
       <c r="AA312" s="9"/>
     </row>
-    <row r="313" spans="8:27" s="1" customFormat="1">
+    <row r="313" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H313" s="5"/>
       <c r="I313" s="5"/>
       <c r="J313" s="5"/>
@@ -11985,7 +11995,7 @@
       <c r="Y313" s="9"/>
       <c r="AA313" s="9"/>
     </row>
-    <row r="314" spans="8:27" s="1" customFormat="1">
+    <row r="314" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H314" s="5"/>
       <c r="I314" s="5"/>
       <c r="J314" s="5"/>
@@ -11996,7 +12006,7 @@
       <c r="Y314" s="9"/>
       <c r="AA314" s="9"/>
     </row>
-    <row r="315" spans="8:27" s="1" customFormat="1">
+    <row r="315" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H315" s="5"/>
       <c r="I315" s="5"/>
       <c r="J315" s="5"/>
@@ -12007,7 +12017,7 @@
       <c r="Y315" s="9"/>
       <c r="AA315" s="9"/>
     </row>
-    <row r="316" spans="8:27" s="1" customFormat="1">
+    <row r="316" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H316" s="5"/>
       <c r="I316" s="5"/>
       <c r="J316" s="5"/>
@@ -12018,7 +12028,7 @@
       <c r="Y316" s="9"/>
       <c r="AA316" s="9"/>
     </row>
-    <row r="317" spans="8:27" s="1" customFormat="1">
+    <row r="317" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H317" s="5"/>
       <c r="I317" s="5"/>
       <c r="J317" s="5"/>
@@ -12029,7 +12039,7 @@
       <c r="Y317" s="9"/>
       <c r="AA317" s="9"/>
     </row>
-    <row r="318" spans="8:27" s="1" customFormat="1">
+    <row r="318" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H318" s="5"/>
       <c r="I318" s="5"/>
       <c r="J318" s="5"/>
@@ -12040,7 +12050,7 @@
       <c r="Y318" s="9"/>
       <c r="AA318" s="9"/>
     </row>
-    <row r="319" spans="8:27" s="1" customFormat="1">
+    <row r="319" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H319" s="5"/>
       <c r="I319" s="5"/>
       <c r="J319" s="5"/>
@@ -12051,7 +12061,7 @@
       <c r="Y319" s="9"/>
       <c r="AA319" s="9"/>
     </row>
-    <row r="320" spans="8:27" s="1" customFormat="1">
+    <row r="320" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H320" s="5"/>
       <c r="I320" s="5"/>
       <c r="J320" s="5"/>
@@ -12062,7 +12072,7 @@
       <c r="Y320" s="9"/>
       <c r="AA320" s="9"/>
     </row>
-    <row r="321" spans="8:27" s="1" customFormat="1">
+    <row r="321" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H321" s="5"/>
       <c r="I321" s="5"/>
       <c r="J321" s="5"/>
@@ -12073,7 +12083,7 @@
       <c r="Y321" s="9"/>
       <c r="AA321" s="9"/>
     </row>
-    <row r="322" spans="8:27" s="1" customFormat="1">
+    <row r="322" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H322" s="5"/>
       <c r="I322" s="5"/>
       <c r="J322" s="5"/>
@@ -12084,7 +12094,7 @@
       <c r="Y322" s="9"/>
       <c r="AA322" s="9"/>
     </row>
-    <row r="323" spans="8:27" s="1" customFormat="1">
+    <row r="323" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H323" s="5"/>
       <c r="I323" s="5"/>
       <c r="J323" s="5"/>
@@ -12095,7 +12105,7 @@
       <c r="Y323" s="9"/>
       <c r="AA323" s="9"/>
     </row>
-    <row r="324" spans="8:27" s="1" customFormat="1">
+    <row r="324" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H324" s="5"/>
       <c r="I324" s="5"/>
       <c r="J324" s="5"/>
@@ -12106,7 +12116,7 @@
       <c r="Y324" s="9"/>
       <c r="AA324" s="9"/>
     </row>
-    <row r="325" spans="8:27" s="1" customFormat="1">
+    <row r="325" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H325" s="5"/>
       <c r="I325" s="5"/>
       <c r="J325" s="5"/>
@@ -12117,7 +12127,7 @@
       <c r="Y325" s="9"/>
       <c r="AA325" s="9"/>
     </row>
-    <row r="326" spans="8:27" s="1" customFormat="1">
+    <row r="326" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H326" s="5"/>
       <c r="I326" s="5"/>
       <c r="J326" s="5"/>
@@ -12128,7 +12138,7 @@
       <c r="Y326" s="9"/>
       <c r="AA326" s="9"/>
     </row>
-    <row r="327" spans="8:27" s="1" customFormat="1">
+    <row r="327" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H327" s="5"/>
       <c r="I327" s="5"/>
       <c r="J327" s="5"/>
@@ -12139,7 +12149,7 @@
       <c r="Y327" s="9"/>
       <c r="AA327" s="9"/>
     </row>
-    <row r="328" spans="8:27" s="1" customFormat="1">
+    <row r="328" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H328" s="5"/>
       <c r="I328" s="5"/>
       <c r="J328" s="5"/>
@@ -12150,7 +12160,7 @@
       <c r="Y328" s="9"/>
       <c r="AA328" s="9"/>
     </row>
-    <row r="329" spans="8:27" s="1" customFormat="1">
+    <row r="329" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H329" s="5"/>
       <c r="I329" s="5"/>
       <c r="J329" s="5"/>
@@ -12161,7 +12171,7 @@
       <c r="Y329" s="9"/>
       <c r="AA329" s="9"/>
     </row>
-    <row r="330" spans="8:27" s="1" customFormat="1">
+    <row r="330" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H330" s="5"/>
       <c r="I330" s="5"/>
       <c r="J330" s="5"/>
@@ -12172,7 +12182,7 @@
       <c r="Y330" s="9"/>
       <c r="AA330" s="9"/>
     </row>
-    <row r="331" spans="8:27" s="1" customFormat="1">
+    <row r="331" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H331" s="5"/>
       <c r="I331" s="5"/>
       <c r="J331" s="5"/>
@@ -12183,7 +12193,7 @@
       <c r="Y331" s="9"/>
       <c r="AA331" s="9"/>
     </row>
-    <row r="332" spans="8:27" s="1" customFormat="1">
+    <row r="332" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H332" s="5"/>
       <c r="I332" s="5"/>
       <c r="J332" s="5"/>
@@ -12194,7 +12204,7 @@
       <c r="Y332" s="9"/>
       <c r="AA332" s="9"/>
     </row>
-    <row r="333" spans="8:27" s="1" customFormat="1">
+    <row r="333" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H333" s="5"/>
       <c r="I333" s="5"/>
       <c r="J333" s="5"/>
@@ -12205,7 +12215,7 @@
       <c r="Y333" s="9"/>
       <c r="AA333" s="9"/>
     </row>
-    <row r="334" spans="8:27" s="1" customFormat="1">
+    <row r="334" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H334" s="5"/>
       <c r="I334" s="5"/>
       <c r="J334" s="5"/>
@@ -12216,7 +12226,7 @@
       <c r="Y334" s="9"/>
       <c r="AA334" s="9"/>
     </row>
-    <row r="335" spans="8:27" s="1" customFormat="1">
+    <row r="335" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H335" s="5"/>
       <c r="I335" s="5"/>
       <c r="J335" s="5"/>
@@ -12227,7 +12237,7 @@
       <c r="Y335" s="9"/>
       <c r="AA335" s="9"/>
     </row>
-    <row r="336" spans="8:27" s="1" customFormat="1">
+    <row r="336" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H336" s="5"/>
       <c r="I336" s="5"/>
       <c r="J336" s="5"/>
@@ -12238,7 +12248,7 @@
       <c r="Y336" s="9"/>
       <c r="AA336" s="9"/>
     </row>
-    <row r="337" spans="8:27" s="1" customFormat="1">
+    <row r="337" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H337" s="5"/>
       <c r="I337" s="5"/>
       <c r="J337" s="5"/>
@@ -12249,7 +12259,7 @@
       <c r="Y337" s="9"/>
       <c r="AA337" s="9"/>
     </row>
-    <row r="338" spans="8:27" s="1" customFormat="1">
+    <row r="338" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H338" s="5"/>
       <c r="I338" s="5"/>
       <c r="J338" s="5"/>
@@ -12260,7 +12270,7 @@
       <c r="Y338" s="9"/>
       <c r="AA338" s="9"/>
     </row>
-    <row r="339" spans="8:27" s="1" customFormat="1">
+    <row r="339" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H339" s="5"/>
       <c r="I339" s="5"/>
       <c r="J339" s="5"/>
@@ -12271,7 +12281,7 @@
       <c r="Y339" s="9"/>
       <c r="AA339" s="9"/>
     </row>
-    <row r="340" spans="8:27" s="1" customFormat="1">
+    <row r="340" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H340" s="5"/>
       <c r="I340" s="5"/>
       <c r="J340" s="5"/>
@@ -12282,7 +12292,7 @@
       <c r="Y340" s="9"/>
       <c r="AA340" s="9"/>
     </row>
-    <row r="341" spans="8:27" s="1" customFormat="1">
+    <row r="341" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H341" s="5"/>
       <c r="I341" s="5"/>
       <c r="J341" s="5"/>
@@ -12293,7 +12303,7 @@
       <c r="Y341" s="9"/>
       <c r="AA341" s="9"/>
     </row>
-    <row r="342" spans="8:27" s="1" customFormat="1">
+    <row r="342" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H342" s="5"/>
       <c r="I342" s="5"/>
       <c r="J342" s="5"/>
@@ -12304,7 +12314,7 @@
       <c r="Y342" s="9"/>
       <c r="AA342" s="9"/>
     </row>
-    <row r="343" spans="8:27" s="1" customFormat="1">
+    <row r="343" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H343" s="5"/>
       <c r="I343" s="5"/>
       <c r="J343" s="5"/>
@@ -12315,7 +12325,7 @@
       <c r="Y343" s="9"/>
       <c r="AA343" s="9"/>
     </row>
-    <row r="344" spans="8:27" s="1" customFormat="1">
+    <row r="344" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H344" s="5"/>
       <c r="I344" s="5"/>
       <c r="J344" s="5"/>
@@ -12326,7 +12336,7 @@
       <c r="Y344" s="9"/>
       <c r="AA344" s="9"/>
     </row>
-    <row r="345" spans="8:27" s="1" customFormat="1">
+    <row r="345" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H345" s="5"/>
       <c r="I345" s="5"/>
       <c r="J345" s="5"/>
@@ -12337,7 +12347,7 @@
       <c r="Y345" s="9"/>
       <c r="AA345" s="9"/>
     </row>
-    <row r="346" spans="8:27" s="1" customFormat="1">
+    <row r="346" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H346" s="5"/>
       <c r="I346" s="5"/>
       <c r="J346" s="5"/>
@@ -12348,7 +12358,7 @@
       <c r="Y346" s="9"/>
       <c r="AA346" s="9"/>
     </row>
-    <row r="347" spans="8:27" s="1" customFormat="1">
+    <row r="347" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H347" s="5"/>
       <c r="I347" s="5"/>
       <c r="J347" s="5"/>
@@ -12359,7 +12369,7 @@
       <c r="Y347" s="9"/>
       <c r="AA347" s="9"/>
     </row>
-    <row r="348" spans="8:27" s="1" customFormat="1">
+    <row r="348" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H348" s="5"/>
       <c r="I348" s="5"/>
       <c r="J348" s="5"/>
@@ -12370,7 +12380,7 @@
       <c r="Y348" s="9"/>
       <c r="AA348" s="9"/>
     </row>
-    <row r="349" spans="8:27" s="1" customFormat="1">
+    <row r="349" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H349" s="5"/>
       <c r="I349" s="5"/>
       <c r="J349" s="5"/>
@@ -12381,7 +12391,7 @@
       <c r="Y349" s="9"/>
       <c r="AA349" s="9"/>
     </row>
-    <row r="350" spans="8:27" s="1" customFormat="1">
+    <row r="350" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H350" s="5"/>
       <c r="I350" s="5"/>
       <c r="J350" s="5"/>
@@ -12392,7 +12402,7 @@
       <c r="Y350" s="9"/>
       <c r="AA350" s="9"/>
     </row>
-    <row r="351" spans="8:27" s="1" customFormat="1">
+    <row r="351" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H351" s="5"/>
       <c r="I351" s="5"/>
       <c r="J351" s="5"/>
@@ -12403,7 +12413,7 @@
       <c r="Y351" s="9"/>
       <c r="AA351" s="9"/>
     </row>
-    <row r="352" spans="8:27" s="1" customFormat="1">
+    <row r="352" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H352" s="5"/>
       <c r="I352" s="5"/>
       <c r="J352" s="5"/>
@@ -12414,7 +12424,7 @@
       <c r="Y352" s="9"/>
       <c r="AA352" s="9"/>
     </row>
-    <row r="353" spans="8:27" s="1" customFormat="1">
+    <row r="353" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H353" s="5"/>
       <c r="I353" s="5"/>
       <c r="J353" s="5"/>
@@ -12425,7 +12435,7 @@
       <c r="Y353" s="9"/>
       <c r="AA353" s="9"/>
     </row>
-    <row r="354" spans="8:27" s="1" customFormat="1">
+    <row r="354" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H354" s="5"/>
       <c r="I354" s="5"/>
       <c r="J354" s="5"/>
@@ -12436,7 +12446,7 @@
       <c r="Y354" s="9"/>
       <c r="AA354" s="9"/>
     </row>
-    <row r="355" spans="8:27" s="1" customFormat="1">
+    <row r="355" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H355" s="5"/>
       <c r="I355" s="5"/>
       <c r="J355" s="5"/>
@@ -12447,7 +12457,7 @@
       <c r="Y355" s="9"/>
       <c r="AA355" s="9"/>
     </row>
-    <row r="356" spans="8:27" s="1" customFormat="1">
+    <row r="356" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H356" s="5"/>
       <c r="I356" s="5"/>
       <c r="J356" s="5"/>
@@ -12458,7 +12468,7 @@
       <c r="Y356" s="9"/>
       <c r="AA356" s="9"/>
     </row>
-    <row r="357" spans="8:27" s="1" customFormat="1">
+    <row r="357" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H357" s="5"/>
       <c r="I357" s="5"/>
       <c r="J357" s="5"/>
@@ -12469,7 +12479,7 @@
       <c r="Y357" s="9"/>
       <c r="AA357" s="9"/>
     </row>
-    <row r="358" spans="8:27" s="1" customFormat="1">
+    <row r="358" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H358" s="5"/>
       <c r="I358" s="5"/>
       <c r="J358" s="5"/>
@@ -12480,7 +12490,7 @@
       <c r="Y358" s="9"/>
       <c r="AA358" s="9"/>
     </row>
-    <row r="359" spans="8:27" s="1" customFormat="1">
+    <row r="359" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H359" s="5"/>
       <c r="I359" s="5"/>
       <c r="J359" s="5"/>
@@ -12491,7 +12501,7 @@
       <c r="Y359" s="9"/>
       <c r="AA359" s="9"/>
     </row>
-    <row r="360" spans="8:27" s="1" customFormat="1">
+    <row r="360" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H360" s="5"/>
       <c r="I360" s="5"/>
       <c r="J360" s="5"/>
@@ -12502,7 +12512,7 @@
       <c r="Y360" s="9"/>
       <c r="AA360" s="9"/>
     </row>
-    <row r="361" spans="8:27" s="1" customFormat="1">
+    <row r="361" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H361" s="5"/>
       <c r="I361" s="5"/>
       <c r="J361" s="5"/>
@@ -12513,7 +12523,7 @@
       <c r="Y361" s="9"/>
       <c r="AA361" s="9"/>
     </row>
-    <row r="362" spans="8:27" s="1" customFormat="1">
+    <row r="362" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H362" s="5"/>
       <c r="I362" s="5"/>
       <c r="J362" s="5"/>
@@ -12524,7 +12534,7 @@
       <c r="Y362" s="9"/>
       <c r="AA362" s="9"/>
     </row>
-    <row r="363" spans="8:27" s="1" customFormat="1">
+    <row r="363" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H363" s="5"/>
       <c r="I363" s="5"/>
       <c r="J363" s="5"/>
@@ -12535,7 +12545,7 @@
       <c r="Y363" s="9"/>
       <c r="AA363" s="9"/>
     </row>
-    <row r="364" spans="8:27" s="1" customFormat="1">
+    <row r="364" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H364" s="5"/>
       <c r="I364" s="5"/>
       <c r="J364" s="5"/>
@@ -12546,7 +12556,7 @@
       <c r="Y364" s="9"/>
       <c r="AA364" s="9"/>
     </row>
-    <row r="365" spans="8:27" s="1" customFormat="1">
+    <row r="365" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H365" s="5"/>
       <c r="I365" s="5"/>
       <c r="J365" s="5"/>
@@ -12557,7 +12567,7 @@
       <c r="Y365" s="9"/>
       <c r="AA365" s="9"/>
     </row>
-    <row r="366" spans="8:27" s="1" customFormat="1">
+    <row r="366" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H366" s="5"/>
       <c r="I366" s="5"/>
       <c r="J366" s="5"/>
@@ -12568,7 +12578,7 @@
       <c r="Y366" s="9"/>
       <c r="AA366" s="9"/>
     </row>
-    <row r="367" spans="8:27" s="1" customFormat="1">
+    <row r="367" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H367" s="5"/>
       <c r="I367" s="5"/>
       <c r="J367" s="5"/>
@@ -12579,7 +12589,7 @@
       <c r="Y367" s="9"/>
       <c r="AA367" s="9"/>
     </row>
-    <row r="368" spans="8:27" s="1" customFormat="1">
+    <row r="368" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H368" s="5"/>
       <c r="I368" s="5"/>
       <c r="J368" s="5"/>
@@ -12590,7 +12600,7 @@
       <c r="Y368" s="9"/>
       <c r="AA368" s="9"/>
     </row>
-    <row r="369" spans="8:27" s="1" customFormat="1">
+    <row r="369" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H369" s="5"/>
       <c r="I369" s="5"/>
       <c r="J369" s="5"/>
@@ -12601,7 +12611,7 @@
       <c r="Y369" s="9"/>
       <c r="AA369" s="9"/>
     </row>
-    <row r="370" spans="8:27" s="1" customFormat="1">
+    <row r="370" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H370" s="5"/>
       <c r="I370" s="5"/>
       <c r="J370" s="5"/>
@@ -12612,7 +12622,7 @@
       <c r="Y370" s="9"/>
       <c r="AA370" s="9"/>
     </row>
-    <row r="371" spans="8:27" s="1" customFormat="1">
+    <row r="371" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H371" s="5"/>
       <c r="I371" s="5"/>
       <c r="J371" s="5"/>
@@ -12623,7 +12633,7 @@
       <c r="Y371" s="9"/>
       <c r="AA371" s="9"/>
     </row>
-    <row r="372" spans="8:27" s="1" customFormat="1">
+    <row r="372" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H372" s="5"/>
       <c r="I372" s="5"/>
       <c r="J372" s="5"/>
@@ -12634,7 +12644,7 @@
       <c r="Y372" s="9"/>
       <c r="AA372" s="9"/>
     </row>
-    <row r="373" spans="8:27" s="1" customFormat="1">
+    <row r="373" spans="8:27" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H373" s="5"/>
       <c r="I373" s="5"/>
       <c r="J373" s="5"/>
@@ -12647,6 +12657,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AMJ373" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>